<commit_message>
update cell summary: sorting quality for bat 34
</commit_message>
<xml_diff>
--- a/inclusion_lists/cells_summary.xlsx
+++ b/inclusion_lists/cells_summary.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="522">
   <si>
     <t>bat</t>
   </si>
@@ -1559,6 +1559,42 @@
   </si>
   <si>
     <t>not sure+there is another cell on this tt!!</t>
+  </si>
+  <si>
+    <t>not stable; noise added due to instability;</t>
+  </si>
+  <si>
+    <t>taking some noise in the cluster</t>
+  </si>
+  <si>
+    <t>doesn’t look like spikes….</t>
+  </si>
+  <si>
+    <t>more than one cell (see the two clusters at Sleep1)</t>
+  </si>
+  <si>
+    <t>taking some noise in the cluster (can be seen in the beginning of recordings)</t>
+  </si>
+  <si>
+    <t>not sure</t>
+  </si>
+  <si>
+    <t>there are more clusters in this tt!</t>
+  </si>
+  <si>
+    <t>there is a clear abrupt instability!! Need to re-sort this TT!</t>
+  </si>
+  <si>
+    <t>not stable</t>
+  </si>
+  <si>
+    <t>not so isolated??</t>
+  </si>
+  <si>
+    <t>I don't think it's a single-unit+there is time instability</t>
+  </si>
+  <si>
+    <t>appears only in sleep2</t>
   </si>
 </sst>
 </file>
@@ -1886,8 +1922,8 @@
   <dimension ref="A1:T482"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J76" sqref="J76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1897,7 +1933,7 @@
     <col min="3" max="3" width="7.875" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.75" style="1" customWidth="1"/>
     <col min="5" max="7" width="7.875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="51.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="67.125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.875" style="1" customWidth="1"/>
     <col min="10" max="10" width="11.875" style="1" customWidth="1"/>
     <col min="11" max="11" width="30.5" style="1" customWidth="1"/>
@@ -2896,6 +2932,12 @@
       <c r="F35" s="1">
         <v>1</v>
       </c>
+      <c r="G35" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>510</v>
+      </c>
       <c r="J35" s="1" t="s">
         <v>489</v>
       </c>
@@ -2920,6 +2962,9 @@
       <c r="F36" s="1">
         <v>2</v>
       </c>
+      <c r="G36" s="1">
+        <v>1</v>
+      </c>
       <c r="J36" s="1" t="s">
         <v>489</v>
       </c>
@@ -2944,6 +2989,9 @@
       <c r="F37" s="1">
         <v>3</v>
       </c>
+      <c r="G37" s="1">
+        <v>1</v>
+      </c>
       <c r="J37" s="1" t="s">
         <v>489</v>
       </c>
@@ -2968,6 +3016,9 @@
       <c r="F38" s="1">
         <v>4</v>
       </c>
+      <c r="G38" s="1">
+        <v>1</v>
+      </c>
       <c r="J38" s="1" t="s">
         <v>489</v>
       </c>
@@ -2992,6 +3043,12 @@
       <c r="F39" s="1">
         <v>5</v>
       </c>
+      <c r="G39" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>511</v>
+      </c>
       <c r="J39" s="1" t="s">
         <v>489</v>
       </c>
@@ -3016,6 +3073,9 @@
       <c r="F40" s="1">
         <v>6</v>
       </c>
+      <c r="G40" s="1">
+        <v>1</v>
+      </c>
       <c r="J40" s="1" t="s">
         <v>489</v>
       </c>
@@ -3040,6 +3100,12 @@
       <c r="F41" s="1">
         <v>7</v>
       </c>
+      <c r="G41" s="1">
+        <v>0</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>512</v>
+      </c>
       <c r="J41" s="1" t="s">
         <v>489</v>
       </c>
@@ -3064,6 +3130,12 @@
       <c r="F42" s="1">
         <v>8</v>
       </c>
+      <c r="G42" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>513</v>
+      </c>
       <c r="J42" s="1" t="s">
         <v>489</v>
       </c>
@@ -3088,6 +3160,9 @@
       <c r="F43" s="1">
         <v>1</v>
       </c>
+      <c r="G43" s="1">
+        <v>1</v>
+      </c>
       <c r="J43" s="1" t="s">
         <v>489</v>
       </c>
@@ -3112,6 +3187,9 @@
       <c r="F44" s="1">
         <v>2</v>
       </c>
+      <c r="G44" s="1">
+        <v>1</v>
+      </c>
       <c r="J44" s="1" t="s">
         <v>489</v>
       </c>
@@ -3139,6 +3217,12 @@
       <c r="F45" s="1">
         <v>3</v>
       </c>
+      <c r="G45" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>514</v>
+      </c>
       <c r="J45" s="1" t="s">
         <v>489</v>
       </c>
@@ -3163,6 +3247,9 @@
       <c r="F46" s="1">
         <v>4</v>
       </c>
+      <c r="G46" s="1">
+        <v>1</v>
+      </c>
       <c r="J46" s="1" t="s">
         <v>489</v>
       </c>
@@ -3187,6 +3274,12 @@
       <c r="F47" s="1">
         <v>1</v>
       </c>
+      <c r="G47" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>515</v>
+      </c>
       <c r="J47" s="1" t="s">
         <v>489</v>
       </c>
@@ -3211,6 +3304,12 @@
       <c r="F48" s="1">
         <v>2</v>
       </c>
+      <c r="G48" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>515</v>
+      </c>
       <c r="J48" s="1" t="s">
         <v>489</v>
       </c>
@@ -3235,6 +3334,12 @@
       <c r="F49" s="1">
         <v>1</v>
       </c>
+      <c r="G49" s="1">
+        <v>1</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>516</v>
+      </c>
       <c r="J49" s="1" t="s">
         <v>489</v>
       </c>
@@ -3259,6 +3364,12 @@
       <c r="F50" s="1">
         <v>1</v>
       </c>
+      <c r="G50" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>517</v>
+      </c>
       <c r="J50" s="1" t="s">
         <v>489</v>
       </c>
@@ -3283,6 +3394,12 @@
       <c r="F51" s="1">
         <v>3</v>
       </c>
+      <c r="G51" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>517</v>
+      </c>
       <c r="J51" s="1" t="s">
         <v>489</v>
       </c>
@@ -3307,6 +3424,12 @@
       <c r="F52" s="1">
         <v>4</v>
       </c>
+      <c r="G52" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>517</v>
+      </c>
       <c r="J52" s="1" t="s">
         <v>489</v>
       </c>
@@ -3331,6 +3454,12 @@
       <c r="F53" s="1">
         <v>5</v>
       </c>
+      <c r="G53" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>517</v>
+      </c>
       <c r="J53" s="1" t="s">
         <v>489</v>
       </c>
@@ -3355,6 +3484,12 @@
       <c r="F54" s="1">
         <v>1</v>
       </c>
+      <c r="G54" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>518</v>
+      </c>
       <c r="J54" s="1" t="s">
         <v>489</v>
       </c>
@@ -3379,6 +3514,12 @@
       <c r="F55" s="1">
         <v>2</v>
       </c>
+      <c r="G55" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>519</v>
+      </c>
       <c r="J55" s="1" t="s">
         <v>489</v>
       </c>
@@ -3403,6 +3544,12 @@
       <c r="F56" s="1">
         <v>1</v>
       </c>
+      <c r="G56" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>520</v>
+      </c>
       <c r="J56" s="1" t="s">
         <v>489</v>
       </c>
@@ -3427,6 +3574,12 @@
       <c r="F57" s="1">
         <v>1</v>
       </c>
+      <c r="G57" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>515</v>
+      </c>
       <c r="J57" s="1" t="s">
         <v>489</v>
       </c>
@@ -3451,6 +3604,12 @@
       <c r="F58" s="1">
         <v>2</v>
       </c>
+      <c r="G58" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>521</v>
+      </c>
       <c r="J58" s="1" t="s">
         <v>489</v>
       </c>
@@ -3475,6 +3634,12 @@
       <c r="F59" s="1">
         <v>3</v>
       </c>
+      <c r="G59" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>515</v>
+      </c>
       <c r="J59" s="1" t="s">
         <v>489</v>
       </c>
@@ -13682,6 +13847,18 @@
     </row>
   </sheetData>
   <autoFilter ref="B1:J482"/>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="597" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update cell spike-sorting stability
</commit_message>
<xml_diff>
--- a/inclusion_lists/cells_summary.xlsx
+++ b/inclusion_lists/cells_summary.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="523">
   <si>
     <t>bat</t>
   </si>
@@ -1558,9 +1558,6 @@
     <t>not stable (abrupt disappear!!!)</t>
   </si>
   <si>
-    <t>not sure+there is another cell on this tt!!</t>
-  </si>
-  <si>
     <t>not stable; noise added due to instability;</t>
   </si>
   <si>
@@ -1588,13 +1585,19 @@
     <t>not stable</t>
   </si>
   <si>
-    <t>not so isolated??</t>
-  </si>
-  <si>
-    <t>I don't think it's a single-unit+there is time instability</t>
-  </si>
-  <si>
     <t>appears only in sleep2</t>
+  </si>
+  <si>
+    <t>maybe even take more towards the noise</t>
+  </si>
+  <si>
+    <t>try to resort in windows (density problem)</t>
+  </si>
+  <si>
+    <t>I don't think it's a single-unit+there is time instability - resort in windows</t>
+  </si>
+  <si>
+    <t>not sure; looks multi unit</t>
   </si>
 </sst>
 </file>
@@ -1921,9 +1924,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T482"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J76" sqref="J76"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2798,7 +2801,7 @@
         <v>0.5</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>509</v>
+        <v>520</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>489</v>
@@ -2936,7 +2939,7 @@
         <v>0.5</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>489</v>
@@ -3047,7 +3050,7 @@
         <v>0.5</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>489</v>
@@ -3104,7 +3107,7 @@
         <v>0</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>489</v>
@@ -3134,7 +3137,7 @@
         <v>0.5</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>489</v>
@@ -3221,7 +3224,7 @@
         <v>0.5</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>489</v>
@@ -3278,7 +3281,7 @@
         <v>0.5</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>515</v>
+        <v>519</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>489</v>
@@ -3308,7 +3311,7 @@
         <v>0.5</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>515</v>
+        <v>519</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>489</v>
@@ -3338,7 +3341,7 @@
         <v>1</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>489</v>
@@ -3368,7 +3371,7 @@
         <v>0.5</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>489</v>
@@ -3398,7 +3401,7 @@
         <v>0.5</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>489</v>
@@ -3428,7 +3431,7 @@
         <v>0.5</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>489</v>
@@ -3458,7 +3461,7 @@
         <v>0.5</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>489</v>
@@ -3488,7 +3491,7 @@
         <v>0.5</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>489</v>
@@ -3518,7 +3521,7 @@
         <v>0.5</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>489</v>
@@ -3548,7 +3551,7 @@
         <v>0.5</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>489</v>
@@ -3578,7 +3581,7 @@
         <v>0.5</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J57" s="1" t="s">
         <v>489</v>
@@ -3608,7 +3611,7 @@
         <v>0.5</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="J58" s="1" t="s">
         <v>489</v>
@@ -3638,7 +3641,7 @@
         <v>0.5</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>515</v>
+        <v>522</v>
       </c>
       <c r="J59" s="1" t="s">
         <v>489</v>

</xml_diff>

<commit_message>
update sorting quality summary
</commit_message>
<xml_diff>
--- a/inclusion_lists/cells_summary.xlsx
+++ b/inclusion_lists/cells_summary.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="571">
   <si>
     <t>bat</t>
   </si>
@@ -1739,6 +1739,9 @@
   </si>
   <si>
     <t>b0034_d180315_TT4_SS04</t>
+  </si>
+  <si>
+    <t>re-sorted by Tamir (further cleaning+new spikes); first half spikes from unit 2</t>
   </si>
 </sst>
 </file>
@@ -2078,8 +2081,8 @@
   <dimension ref="A1:T513"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4327,10 +4330,10 @@
         <v>3</v>
       </c>
       <c r="G76" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H76" s="4" t="s">
-        <v>558</v>
+        <v>570</v>
       </c>
       <c r="J76" s="1" t="s">
         <v>488</v>
@@ -5087,6 +5090,12 @@
       </c>
       <c r="F104" s="1">
         <v>3</v>
+      </c>
+      <c r="G104" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>549</v>
       </c>
       <c r="J104" s="1" t="s">
         <v>488</v>

</xml_diff>

<commit_message>
add new sorted cells to summary for bat 34
</commit_message>
<xml_diff>
--- a/inclusion_lists/cells_summary.xlsx
+++ b/inclusion_lists/cells_summary.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="67">
   <si>
     <t>bat</t>
   </si>
@@ -49,6 +49,33 @@
     <t>b0034_d180306_TT4_SS03</t>
   </si>
   <si>
+    <t>b0034_d180310_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b0034_d180310_TT3_SS01</t>
+  </si>
+  <si>
+    <t>b0034_d180310_TT3_SS02</t>
+  </si>
+  <si>
+    <t>b0034_d180310_TT4_SS01</t>
+  </si>
+  <si>
+    <t>b0034_d180310_TT4_SS02</t>
+  </si>
+  <si>
+    <t>b0034_d180310_TT4_SS03</t>
+  </si>
+  <si>
+    <t>b0034_d180310_TT4_SS04</t>
+  </si>
+  <si>
+    <t>b0034_d180310_TT4_SS05</t>
+  </si>
+  <si>
+    <t>b0034_d180311_TT1_SS01</t>
+  </si>
+  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -73,6 +100,12 @@
     <t>sorting_comment</t>
   </si>
   <si>
+    <t>b0034_d180311_TT1_SS02</t>
+  </si>
+  <si>
+    <t>b0034_d180308_TT4_SS01</t>
+  </si>
+  <si>
     <t>multi-unit</t>
   </si>
   <si>
@@ -167,6 +200,36 @@
   </si>
   <si>
     <t>part of unit 3?</t>
+  </si>
+  <si>
+    <t>b0034_d180308_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b0034_d180308_TT1_SS02</t>
+  </si>
+  <si>
+    <t>[57051958925 60107136206]</t>
+  </si>
+  <si>
+    <t>too close to the noise</t>
+  </si>
+  <si>
+    <t>probably multi-unit</t>
+  </si>
+  <si>
+    <t>b0034_d180310_TT3_SS03</t>
+  </si>
+  <si>
+    <t>inverted</t>
+  </si>
+  <si>
+    <t>low FR</t>
+  </si>
+  <si>
+    <t>part of unit 4 or 5?</t>
+  </si>
+  <si>
+    <t>b0034_d180310_TT4_SS06</t>
   </si>
 </sst>
 </file>
@@ -491,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S25"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -506,8 +569,9 @@
     <col min="4" max="4" width="4.75" style="1" customWidth="1"/>
     <col min="5" max="5" width="4" style="1" customWidth="1"/>
     <col min="6" max="6" width="7.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="67.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="7.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="46.25" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.875" style="1" customWidth="1"/>
     <col min="10" max="10" width="30.5" style="1" customWidth="1"/>
     <col min="11" max="11" width="40.375" style="1" customWidth="1"/>
     <col min="12" max="12" width="42.125" style="1" customWidth="1"/>
@@ -528,39 +592,39 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B2" s="1">
         <v>34</v>
@@ -578,15 +642,15 @@
         <v>2</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1">
         <v>34</v>
@@ -604,15 +668,15 @@
         <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1">
         <v>34</v>
@@ -630,15 +694,15 @@
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B5" s="1">
         <v>34</v>
@@ -656,15 +720,15 @@
         <v>2</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B6" s="1">
         <v>34</v>
@@ -682,12 +746,12 @@
         <v>2</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1">
         <v>34</v>
@@ -705,12 +769,12 @@
         <v>2</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B8" s="1">
         <v>34</v>
@@ -728,12 +792,12 @@
         <v>1</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1">
         <v>34</v>
@@ -751,12 +815,12 @@
         <v>1</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1">
         <v>34</v>
@@ -774,12 +838,12 @@
         <v>1</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B11" s="1">
         <v>34</v>
@@ -797,12 +861,12 @@
         <v>1</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="B12" s="1">
         <v>34</v>
@@ -820,12 +884,12 @@
         <v>1</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B13" s="1">
         <v>34</v>
@@ -843,12 +907,12 @@
         <v>2</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B14" s="1">
         <v>34</v>
@@ -866,12 +930,12 @@
         <v>1</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="B15" s="1">
         <v>34</v>
@@ -889,12 +953,12 @@
         <v>2</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B16" s="1">
         <v>34</v>
@@ -912,12 +976,12 @@
         <v>2</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B17" s="1">
         <v>34</v>
@@ -935,15 +999,15 @@
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B18" s="1">
         <v>34</v>
@@ -961,12 +1025,12 @@
         <v>2</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B19" s="1">
         <v>34</v>
@@ -984,15 +1048,15 @@
         <v>1</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B20" s="1">
         <v>34</v>
@@ -1010,12 +1074,12 @@
         <v>2</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="B21" s="1">
         <v>34</v>
@@ -1033,13 +1097,13 @@
         <v>1</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
@@ -1058,8 +1122,11 @@
       <c r="F22" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I22" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
@@ -1079,10 +1146,13 @@
         <v>1</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
@@ -1101,10 +1171,13 @@
       <c r="F24" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I24" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B25" s="1">
         <v>34</v>
@@ -1122,7 +1195,355 @@
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>45</v>
+        <v>56</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="1">
+        <v>34</v>
+      </c>
+      <c r="C26" s="2">
+        <v>43167</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="1">
+        <v>34</v>
+      </c>
+      <c r="C27" s="2">
+        <v>43167</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
+        <v>2</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="1">
+        <v>34</v>
+      </c>
+      <c r="C28" s="2">
+        <v>43167</v>
+      </c>
+      <c r="D28" s="1">
+        <v>4</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="1">
+        <v>34</v>
+      </c>
+      <c r="C29" s="2">
+        <v>43169</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="1">
+        <v>34</v>
+      </c>
+      <c r="C30" s="2">
+        <v>43169</v>
+      </c>
+      <c r="D30" s="1">
+        <v>3</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="1">
+        <v>34</v>
+      </c>
+      <c r="C31" s="2">
+        <v>43169</v>
+      </c>
+      <c r="D31" s="1">
+        <v>3</v>
+      </c>
+      <c r="E31" s="1">
+        <v>2</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="1">
+        <v>34</v>
+      </c>
+      <c r="C32" s="2">
+        <v>43169</v>
+      </c>
+      <c r="D32" s="1">
+        <v>3</v>
+      </c>
+      <c r="E32" s="1">
+        <v>3</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="1">
+        <v>34</v>
+      </c>
+      <c r="C33" s="2">
+        <v>43169</v>
+      </c>
+      <c r="D33" s="1">
+        <v>4</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="1">
+        <v>34</v>
+      </c>
+      <c r="C34" s="2">
+        <v>43169</v>
+      </c>
+      <c r="D34" s="1">
+        <v>4</v>
+      </c>
+      <c r="E34" s="1">
+        <v>2</v>
+      </c>
+      <c r="F34" s="1">
+        <v>2</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="1">
+        <v>34</v>
+      </c>
+      <c r="C35" s="2">
+        <v>43169</v>
+      </c>
+      <c r="D35" s="1">
+        <v>4</v>
+      </c>
+      <c r="E35" s="1">
+        <v>3</v>
+      </c>
+      <c r="F35" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="1">
+        <v>34</v>
+      </c>
+      <c r="C36" s="2">
+        <v>43169</v>
+      </c>
+      <c r="D36" s="1">
+        <v>4</v>
+      </c>
+      <c r="E36" s="1">
+        <v>4</v>
+      </c>
+      <c r="F36" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="1">
+        <v>34</v>
+      </c>
+      <c r="C37" s="2">
+        <v>43169</v>
+      </c>
+      <c r="D37" s="1">
+        <v>4</v>
+      </c>
+      <c r="E37" s="1">
+        <v>5</v>
+      </c>
+      <c r="F37" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" s="1">
+        <v>34</v>
+      </c>
+      <c r="C38" s="2">
+        <v>43169</v>
+      </c>
+      <c r="D38" s="1">
+        <v>4</v>
+      </c>
+      <c r="E38" s="1">
+        <v>6</v>
+      </c>
+      <c r="F38" s="1">
+        <v>1</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="1">
+        <v>34</v>
+      </c>
+      <c r="C39" s="2">
+        <v>43170</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1</v>
+      </c>
+      <c r="E39" s="1">
+        <v>1</v>
+      </c>
+      <c r="F39" s="1">
+        <v>2</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" s="1">
+        <v>34</v>
+      </c>
+      <c r="C40" s="2">
+        <v>43170</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1</v>
+      </c>
+      <c r="E40" s="1">
+        <v>2</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update sorting summary for bat 34
</commit_message>
<xml_diff>
--- a/inclusion_lists/cells_summary.xlsx
+++ b/inclusion_lists/cells_summary.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="94">
   <si>
     <t>bat</t>
   </si>
@@ -76,6 +76,54 @@
     <t>b0034_d180311_TT1_SS01</t>
   </si>
   <si>
+    <t>b0034_d180311_TT4_SS01</t>
+  </si>
+  <si>
+    <t>b0034_d180311_TT4_SS02</t>
+  </si>
+  <si>
+    <t>b0034_d180311_TT4_SS03</t>
+  </si>
+  <si>
+    <t>b0034_d180311_TT4_SS04</t>
+  </si>
+  <si>
+    <t>b0034_d180312_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b0034_d180312_TT1_SS02</t>
+  </si>
+  <si>
+    <t>b0034_d180312_TT1_SS03</t>
+  </si>
+  <si>
+    <t>b0034_d180312_TT3_SS01</t>
+  </si>
+  <si>
+    <t>b0034_d180312_TT3_SS02</t>
+  </si>
+  <si>
+    <t>b0034_d180312_TT3_SS03</t>
+  </si>
+  <si>
+    <t>b0034_d180312_TT3_SS04</t>
+  </si>
+  <si>
+    <t>b0034_d180312_TT3_SS05</t>
+  </si>
+  <si>
+    <t>b0034_d180312_TT3_SS06</t>
+  </si>
+  <si>
+    <t>b0034_d180312_TT4_SS01</t>
+  </si>
+  <si>
+    <t>b0034_d180312_TT4_SS02</t>
+  </si>
+  <si>
+    <t>b0034_d180312_TT4_SS03</t>
+  </si>
+  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -103,6 +151,15 @@
     <t>b0034_d180311_TT1_SS02</t>
   </si>
   <si>
+    <t>b0034_d180311_TT4_SS05</t>
+  </si>
+  <si>
+    <t>b0034_d180312_TT4_SS04</t>
+  </si>
+  <si>
+    <t>b0034_d180312_TT4_SS05</t>
+  </si>
+  <si>
     <t>b0034_d180308_TT4_SS01</t>
   </si>
   <si>
@@ -230,6 +287,30 @@
   </si>
   <si>
     <t>b0034_d180310_TT4_SS06</t>
+  </si>
+  <si>
+    <t>partially stable; units 3+4+5 are mixed</t>
+  </si>
+  <si>
+    <t>b0034_d180312_TT1_SS04</t>
+  </si>
+  <si>
+    <t>b0034_d180312_TT1_SS05</t>
+  </si>
+  <si>
+    <t>flight artifacts!</t>
+  </si>
+  <si>
+    <t>not well isolated</t>
+  </si>
+  <si>
+    <t>maybe multi-unit</t>
+  </si>
+  <si>
+    <t>a bit contaminated</t>
+  </si>
+  <si>
+    <t>AMAZING FIELDS! Very clean</t>
   </si>
 </sst>
 </file>
@@ -246,12 +327,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -266,13 +353,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -554,11 +647,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:S62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G40" sqref="G40"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -592,39 +685,39 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="B2" s="1">
         <v>34</v>
@@ -642,15 +735,15 @@
         <v>2</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="B3" s="1">
         <v>34</v>
@@ -668,15 +761,15 @@
         <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="B4" s="1">
         <v>34</v>
@@ -694,15 +787,15 @@
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="B5" s="1">
         <v>34</v>
@@ -720,15 +813,15 @@
         <v>2</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="B6" s="1">
         <v>34</v>
@@ -746,12 +839,12 @@
         <v>2</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="B7" s="1">
         <v>34</v>
@@ -769,12 +862,12 @@
         <v>2</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="B8" s="1">
         <v>34</v>
@@ -792,12 +885,12 @@
         <v>1</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="B9" s="1">
         <v>34</v>
@@ -815,12 +908,12 @@
         <v>1</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="B10" s="1">
         <v>34</v>
@@ -838,12 +931,12 @@
         <v>1</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="B11" s="1">
         <v>34</v>
@@ -861,12 +954,12 @@
         <v>1</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="B12" s="1">
         <v>34</v>
@@ -884,12 +977,12 @@
         <v>1</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="B13" s="1">
         <v>34</v>
@@ -907,12 +1000,12 @@
         <v>2</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B14" s="1">
         <v>34</v>
@@ -930,12 +1023,12 @@
         <v>1</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="B15" s="1">
         <v>34</v>
@@ -953,12 +1046,12 @@
         <v>2</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="B16" s="1">
         <v>34</v>
@@ -976,12 +1069,12 @@
         <v>2</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="B17" s="1">
         <v>34</v>
@@ -999,15 +1092,15 @@
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="B18" s="1">
         <v>34</v>
@@ -1025,12 +1118,12 @@
         <v>2</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="B19" s="1">
         <v>34</v>
@@ -1048,15 +1141,15 @@
         <v>1</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="B20" s="1">
         <v>34</v>
@@ -1074,12 +1167,12 @@
         <v>2</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="B21" s="1">
         <v>34</v>
@@ -1097,10 +1190,10 @@
         <v>1</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -1123,7 +1216,7 @@
         <v>2</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -1146,10 +1239,10 @@
         <v>1</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -1172,12 +1265,12 @@
         <v>2</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="B25" s="1">
         <v>34</v>
@@ -1195,15 +1288,15 @@
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="B26" s="1">
         <v>34</v>
@@ -1221,12 +1314,12 @@
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="B27" s="1">
         <v>34</v>
@@ -1244,12 +1337,12 @@
         <v>1</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B28" s="1">
         <v>34</v>
@@ -1267,13 +1360,13 @@
         <v>2</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -1296,7 +1389,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -1319,7 +1412,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -1342,12 +1435,12 @@
         <v>1</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="B32" s="1">
         <v>34</v>
@@ -1365,7 +1458,7 @@
         <v>1</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -1388,7 +1481,7 @@
         <v>1</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -1411,7 +1504,7 @@
         <v>2</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
@@ -1476,7 +1569,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="B38" s="1">
         <v>34</v>
@@ -1494,7 +1587,7 @@
         <v>1</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -1517,15 +1610,15 @@
         <v>2</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B40" s="1">
         <v>34</v>
@@ -1543,8 +1636,471 @@
         <v>1</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>60</v>
-      </c>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41" s="1">
+        <v>34</v>
+      </c>
+      <c r="C41" s="2">
+        <v>43170</v>
+      </c>
+      <c r="D41" s="1">
+        <v>4</v>
+      </c>
+      <c r="E41" s="1">
+        <v>1</v>
+      </c>
+      <c r="F41" s="1">
+        <v>2</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="1">
+        <v>34</v>
+      </c>
+      <c r="C42" s="2">
+        <v>43170</v>
+      </c>
+      <c r="D42" s="1">
+        <v>4</v>
+      </c>
+      <c r="E42" s="1">
+        <v>2</v>
+      </c>
+      <c r="F42" s="1">
+        <v>2</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B43" s="1">
+        <v>34</v>
+      </c>
+      <c r="C43" s="2">
+        <v>43170</v>
+      </c>
+      <c r="D43" s="1">
+        <v>4</v>
+      </c>
+      <c r="E43" s="1">
+        <v>3</v>
+      </c>
+      <c r="F43" s="1">
+        <v>1</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" s="1">
+        <v>34</v>
+      </c>
+      <c r="C44" s="2">
+        <v>43170</v>
+      </c>
+      <c r="D44" s="1">
+        <v>4</v>
+      </c>
+      <c r="E44" s="1">
+        <v>4</v>
+      </c>
+      <c r="F44" s="1">
+        <v>1</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45" s="1">
+        <v>34</v>
+      </c>
+      <c r="C45" s="2">
+        <v>43170</v>
+      </c>
+      <c r="D45" s="1">
+        <v>4</v>
+      </c>
+      <c r="E45" s="1">
+        <v>5</v>
+      </c>
+      <c r="F45" s="1">
+        <v>1</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="1">
+        <v>34</v>
+      </c>
+      <c r="C46" s="2">
+        <v>43171</v>
+      </c>
+      <c r="D46" s="1">
+        <v>1</v>
+      </c>
+      <c r="E46" s="1">
+        <v>1</v>
+      </c>
+      <c r="F46" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47" s="1">
+        <v>34</v>
+      </c>
+      <c r="C47" s="2">
+        <v>43171</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1">
+        <v>2</v>
+      </c>
+      <c r="F47" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" s="1">
+        <v>34</v>
+      </c>
+      <c r="C48" s="2">
+        <v>43171</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1</v>
+      </c>
+      <c r="E48" s="1">
+        <v>3</v>
+      </c>
+      <c r="F48" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B49" s="1">
+        <v>34</v>
+      </c>
+      <c r="C49" s="2">
+        <v>43171</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1</v>
+      </c>
+      <c r="E49" s="1">
+        <v>4</v>
+      </c>
+      <c r="F49" s="1">
+        <v>1</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" s="1">
+        <v>34</v>
+      </c>
+      <c r="C50" s="2">
+        <v>43171</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1</v>
+      </c>
+      <c r="E50" s="1">
+        <v>5</v>
+      </c>
+      <c r="F50" s="1">
+        <v>1</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" s="1">
+        <v>34</v>
+      </c>
+      <c r="C51" s="2">
+        <v>43171</v>
+      </c>
+      <c r="D51" s="1">
+        <v>3</v>
+      </c>
+      <c r="E51" s="1">
+        <v>1</v>
+      </c>
+      <c r="F51" s="1">
+        <v>2</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B52" s="1">
+        <v>34</v>
+      </c>
+      <c r="C52" s="2">
+        <v>43171</v>
+      </c>
+      <c r="D52" s="1">
+        <v>3</v>
+      </c>
+      <c r="E52" s="1">
+        <v>2</v>
+      </c>
+      <c r="F52" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B53" s="1">
+        <v>34</v>
+      </c>
+      <c r="C53" s="2">
+        <v>43171</v>
+      </c>
+      <c r="D53" s="1">
+        <v>3</v>
+      </c>
+      <c r="E53" s="1">
+        <v>3</v>
+      </c>
+      <c r="F53" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B54" s="1">
+        <v>34</v>
+      </c>
+      <c r="C54" s="2">
+        <v>43171</v>
+      </c>
+      <c r="D54" s="1">
+        <v>3</v>
+      </c>
+      <c r="E54" s="1">
+        <v>4</v>
+      </c>
+      <c r="F54" s="1">
+        <v>1</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="1">
+        <v>34</v>
+      </c>
+      <c r="C55" s="2">
+        <v>43171</v>
+      </c>
+      <c r="D55" s="1">
+        <v>3</v>
+      </c>
+      <c r="E55" s="1">
+        <v>5</v>
+      </c>
+      <c r="F55" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" s="1">
+        <v>34</v>
+      </c>
+      <c r="C56" s="2">
+        <v>43171</v>
+      </c>
+      <c r="D56" s="1">
+        <v>3</v>
+      </c>
+      <c r="E56" s="1">
+        <v>6</v>
+      </c>
+      <c r="F56" s="1">
+        <v>0</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B57" s="1">
+        <v>34</v>
+      </c>
+      <c r="C57" s="2">
+        <v>43171</v>
+      </c>
+      <c r="D57" s="1">
+        <v>4</v>
+      </c>
+      <c r="E57" s="1">
+        <v>1</v>
+      </c>
+      <c r="F57" s="1">
+        <v>2</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B58" s="1">
+        <v>34</v>
+      </c>
+      <c r="C58" s="2">
+        <v>43171</v>
+      </c>
+      <c r="D58" s="1">
+        <v>4</v>
+      </c>
+      <c r="E58" s="1">
+        <v>2</v>
+      </c>
+      <c r="F58" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="1">
+        <v>34</v>
+      </c>
+      <c r="C59" s="2">
+        <v>43171</v>
+      </c>
+      <c r="D59" s="1">
+        <v>4</v>
+      </c>
+      <c r="E59" s="1">
+        <v>3</v>
+      </c>
+      <c r="F59" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B60" s="1">
+        <v>34</v>
+      </c>
+      <c r="C60" s="2">
+        <v>43171</v>
+      </c>
+      <c r="D60" s="1">
+        <v>4</v>
+      </c>
+      <c r="E60" s="1">
+        <v>4</v>
+      </c>
+      <c r="F60" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B61" s="1">
+        <v>34</v>
+      </c>
+      <c r="C61" s="2">
+        <v>43171</v>
+      </c>
+      <c r="D61" s="1">
+        <v>4</v>
+      </c>
+      <c r="E61" s="1">
+        <v>5</v>
+      </c>
+      <c r="F61" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C62" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="B1:H1"/>

</xml_diff>

<commit_message>
update sorting bat 34
</commit_message>
<xml_diff>
--- a/inclusion_lists/cells_summary.xlsx
+++ b/inclusion_lists/cells_summary.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$H$95</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="142">
   <si>
     <t>bat</t>
   </si>
@@ -124,6 +124,81 @@
     <t>b0034_d180312_TT4_SS03</t>
   </si>
   <si>
+    <t>b0034_d180313_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b0034_d180313_TT1_SS02</t>
+  </si>
+  <si>
+    <t>b0034_d180313_TT1_SS03</t>
+  </si>
+  <si>
+    <t>b0034_d180313_TT1_SS04</t>
+  </si>
+  <si>
+    <t>b0034_d180313_TT3_SS01</t>
+  </si>
+  <si>
+    <t>b0034_d180313_TT3_SS02</t>
+  </si>
+  <si>
+    <t>b0034_d180313_TT3_SS03</t>
+  </si>
+  <si>
+    <t>b0034_d180313_TT3_SS04</t>
+  </si>
+  <si>
+    <t>b0034_d180313_TT3_SS05</t>
+  </si>
+  <si>
+    <t>b0034_d180313_TT3_SS06</t>
+  </si>
+  <si>
+    <t>b0034_d180313_TT4_SS01</t>
+  </si>
+  <si>
+    <t>b0034_d180313_TT4_SS02</t>
+  </si>
+  <si>
+    <t>b0034_d180313_TT4_SS03</t>
+  </si>
+  <si>
+    <t>b0034_d180313_TT4_SS04</t>
+  </si>
+  <si>
+    <t>b0034_d180314_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b0034_d180314_TT1_SS02</t>
+  </si>
+  <si>
+    <t>b0034_d180314_TT3_SS01</t>
+  </si>
+  <si>
+    <t>b0034_d180314_TT4_SS01</t>
+  </si>
+  <si>
+    <t>b0034_d180314_TT4_SS03</t>
+  </si>
+  <si>
+    <t>b0034_d180314_TT4_SS04</t>
+  </si>
+  <si>
+    <t>b0034_d180314_TT4_SS05</t>
+  </si>
+  <si>
+    <t>b0034_d180315_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b0034_d180315_TT3_SS01</t>
+  </si>
+  <si>
+    <t>b0034_d180315_TT4_SS01</t>
+  </si>
+  <si>
+    <t>b0034_d180315_TT4_SS02</t>
+  </si>
+  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -163,9 +238,39 @@
     <t>b0034_d180308_TT4_SS01</t>
   </si>
   <si>
+    <t>b0034_d180313_TT4_SS05</t>
+  </si>
+  <si>
+    <t>b0034_d180313_TT4_SS06</t>
+  </si>
+  <si>
+    <t>b0034_d180313_TT4_SS07</t>
+  </si>
+  <si>
+    <t>b0034_d180313_TT4_SS08</t>
+  </si>
+  <si>
+    <t>b0034_d180314_TT1_SS03</t>
+  </si>
+  <si>
+    <t>b0034_d180314_TT1_SS04</t>
+  </si>
+  <si>
     <t>multi-unit</t>
   </si>
   <si>
+    <t>b0034_d180314_TT3_SS02</t>
+  </si>
+  <si>
+    <t>b0034_d180314_TT4_SS02</t>
+  </si>
+  <si>
+    <t>b0034_d180315_TT3_SS02</t>
+  </si>
+  <si>
+    <t>b0034_d180315_TT3_SS03</t>
+  </si>
+  <si>
     <t>unit</t>
   </si>
   <si>
@@ -311,6 +416,45 @@
   </si>
   <si>
     <t>AMAZING FIELDS! Very clean</t>
+  </si>
+  <si>
+    <t>maybe multi-unit?</t>
+  </si>
+  <si>
+    <t>interneuron</t>
+  </si>
+  <si>
+    <t>end of burst looks like a different cluster (I checked the xcorr)</t>
+  </si>
+  <si>
+    <t>b0034_d180313_TT3_SS07</t>
+  </si>
+  <si>
+    <t>mixed of unit 6 and 7</t>
+  </si>
+  <si>
+    <t>maybe a bit contaminated with spikes from unit 4</t>
+  </si>
+  <si>
+    <t>contaminated a bit with unit 2</t>
+  </si>
+  <si>
+    <t>two interneurons - there are some time segments they can be seperated</t>
+  </si>
+  <si>
+    <t>multi-unit;partially stable</t>
+  </si>
+  <si>
+    <t>rapid large change in the middle, maybe use only one part?</t>
+  </si>
+  <si>
+    <t>b0034_d180314_TT4_SS06</t>
+  </si>
+  <si>
+    <t>a bit contaminated; interneuron/multi-unit?</t>
+  </si>
+  <si>
+    <t>cleaning of unit 1</t>
   </si>
 </sst>
 </file>
@@ -647,11 +791,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S62"/>
+  <dimension ref="A1:S100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A62" sqref="A62"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G98" sqref="G98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -662,7 +806,7 @@
     <col min="4" max="4" width="4.75" style="1" customWidth="1"/>
     <col min="5" max="5" width="4" style="1" customWidth="1"/>
     <col min="6" max="6" width="7.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="46.25" style="1" customWidth="1"/>
+    <col min="7" max="7" width="50.75" style="1" customWidth="1"/>
     <col min="8" max="8" width="25.625" style="1" customWidth="1"/>
     <col min="9" max="9" width="7.875" style="1" customWidth="1"/>
     <col min="10" max="10" width="30.5" style="1" customWidth="1"/>
@@ -685,39 +829,39 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="B2" s="1">
         <v>34</v>
@@ -735,15 +879,15 @@
         <v>2</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>46</v>
+        <v>81</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
       <c r="B3" s="1">
         <v>34</v>
@@ -761,15 +905,15 @@
         <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="B4" s="1">
         <v>34</v>
@@ -787,15 +931,15 @@
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>48</v>
+        <v>83</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="B5" s="1">
         <v>34</v>
@@ -812,16 +956,16 @@
       <c r="F5" s="1">
         <v>2</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>49</v>
+      <c r="G5" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
       <c r="B6" s="1">
         <v>34</v>
@@ -839,12 +983,12 @@
         <v>2</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1">
         <v>34</v>
@@ -862,12 +1006,12 @@
         <v>2</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="B8" s="1">
         <v>34</v>
@@ -885,12 +1029,12 @@
         <v>1</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="B9" s="1">
         <v>34</v>
@@ -908,12 +1052,12 @@
         <v>1</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="B10" s="1">
         <v>34</v>
@@ -931,12 +1075,12 @@
         <v>1</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="B11" s="1">
         <v>34</v>
@@ -954,12 +1098,12 @@
         <v>1</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="B12" s="1">
         <v>34</v>
@@ -977,12 +1121,12 @@
         <v>1</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="B13" s="1">
         <v>34</v>
@@ -1000,12 +1144,12 @@
         <v>2</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="B14" s="1">
         <v>34</v>
@@ -1023,12 +1167,12 @@
         <v>1</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>68</v>
+        <v>103</v>
       </c>
       <c r="B15" s="1">
         <v>34</v>
@@ -1046,12 +1190,12 @@
         <v>2</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>69</v>
+        <v>104</v>
       </c>
       <c r="B16" s="1">
         <v>34</v>
@@ -1069,12 +1213,12 @@
         <v>2</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="B17" s="1">
         <v>34</v>
@@ -1092,15 +1236,15 @@
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>66</v>
+        <v>101</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>71</v>
+        <v>106</v>
       </c>
       <c r="B18" s="1">
         <v>34</v>
@@ -1118,12 +1262,12 @@
         <v>2</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="B19" s="1">
         <v>34</v>
@@ -1141,15 +1285,15 @@
         <v>1</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>67</v>
+        <v>102</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="B20" s="1">
         <v>34</v>
@@ -1167,12 +1311,12 @@
         <v>2</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="B21" s="1">
         <v>34</v>
@@ -1190,10 +1334,10 @@
         <v>1</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -1216,7 +1360,7 @@
         <v>2</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -1239,10 +1383,10 @@
         <v>1</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>66</v>
+        <v>101</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -1265,12 +1409,12 @@
         <v>2</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>74</v>
+        <v>109</v>
       </c>
       <c r="B25" s="1">
         <v>34</v>
@@ -1288,15 +1432,15 @@
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>76</v>
+        <v>111</v>
       </c>
       <c r="B26" s="1">
         <v>34</v>
@@ -1314,12 +1458,12 @@
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="B27" s="1">
         <v>34</v>
@@ -1337,12 +1481,12 @@
         <v>1</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="B28" s="1">
         <v>34</v>
@@ -1359,14 +1503,14 @@
       <c r="F28" s="1">
         <v>2</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>49</v>
+      <c r="G28" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>82</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -1389,7 +1533,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -1412,7 +1556,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>80</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -1434,13 +1578,13 @@
       <c r="F31" s="1">
         <v>1</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>49</v>
+      <c r="G31" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>81</v>
+        <v>116</v>
       </c>
       <c r="B32" s="1">
         <v>34</v>
@@ -1457,8 +1601,8 @@
       <c r="F32" s="1">
         <v>1</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>49</v>
+      <c r="G32" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -1481,7 +1625,7 @@
         <v>1</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>82</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -1504,7 +1648,7 @@
         <v>2</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
@@ -1569,7 +1713,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>85</v>
+        <v>120</v>
       </c>
       <c r="B38" s="1">
         <v>34</v>
@@ -1587,7 +1731,7 @@
         <v>1</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>84</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -1610,15 +1754,15 @@
         <v>2</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>49</v>
+        <v>84</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="B40" s="1">
         <v>34</v>
@@ -1636,7 +1780,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -1659,7 +1803,7 @@
         <v>2</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>49</v>
+        <v>84</v>
       </c>
       <c r="H41" s="4"/>
     </row>
@@ -1683,7 +1827,7 @@
         <v>2</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>49</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
@@ -1706,7 +1850,7 @@
         <v>1</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>86</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -1729,12 +1873,12 @@
         <v>1</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>86</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="B45" s="1">
         <v>34</v>
@@ -1752,7 +1896,7 @@
         <v>1</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>86</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
@@ -1817,7 +1961,7 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>87</v>
+        <v>122</v>
       </c>
       <c r="B49" s="1">
         <v>34</v>
@@ -1835,12 +1979,12 @@
         <v>1</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>88</v>
+        <v>123</v>
       </c>
       <c r="B50" s="1">
         <v>34</v>
@@ -1858,7 +2002,7 @@
         <v>1</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
@@ -1881,7 +2025,7 @@
         <v>2</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>49</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
@@ -1944,7 +2088,7 @@
         <v>1</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>90</v>
+        <v>125</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
@@ -1987,7 +2131,7 @@
         <v>0</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>89</v>
+        <v>124</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
@@ -2010,7 +2154,7 @@
         <v>2</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>93</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
@@ -2055,7 +2199,7 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="B60" s="1">
         <v>34</v>
@@ -2073,12 +2217,12 @@
         <v>1.5</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>92</v>
+        <v>127</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="B61" s="1">
         <v>34</v>
@@ -2096,170 +2240,841 @@
         <v>1.5</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>91</v>
+        <v>126</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C62" s="2"/>
+      <c r="A62" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B62" s="1">
+        <v>34</v>
+      </c>
+      <c r="C62" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D62" s="1">
+        <v>1</v>
+      </c>
+      <c r="E62" s="1">
+        <v>1</v>
+      </c>
+      <c r="F62" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B63" s="1">
+        <v>34</v>
+      </c>
+      <c r="C63" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D63" s="1">
+        <v>1</v>
+      </c>
+      <c r="E63" s="1">
+        <v>2</v>
+      </c>
+      <c r="F63" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B64" s="1">
+        <v>34</v>
+      </c>
+      <c r="C64" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D64" s="1">
+        <v>1</v>
+      </c>
+      <c r="E64" s="1">
+        <v>3</v>
+      </c>
+      <c r="F64" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B65" s="1">
+        <v>34</v>
+      </c>
+      <c r="C65" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D65" s="1">
+        <v>1</v>
+      </c>
+      <c r="E65" s="1">
+        <v>4</v>
+      </c>
+      <c r="F65" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B66" s="1">
+        <v>34</v>
+      </c>
+      <c r="C66" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D66" s="1">
+        <v>3</v>
+      </c>
+      <c r="E66" s="1">
+        <v>1</v>
+      </c>
+      <c r="F66" s="1">
+        <v>2</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B67" s="1">
+        <v>34</v>
+      </c>
+      <c r="C67" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D67" s="1">
+        <v>3</v>
+      </c>
+      <c r="E67" s="1">
+        <v>2</v>
+      </c>
+      <c r="F67" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B68" s="1">
+        <v>34</v>
+      </c>
+      <c r="C68" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D68" s="1">
+        <v>3</v>
+      </c>
+      <c r="E68" s="1">
+        <v>3</v>
+      </c>
+      <c r="F68" s="1">
+        <v>2</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B69" s="1">
+        <v>34</v>
+      </c>
+      <c r="C69" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D69" s="1">
+        <v>3</v>
+      </c>
+      <c r="E69" s="1">
+        <v>4</v>
+      </c>
+      <c r="F69" s="1">
+        <v>2</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B70" s="1">
+        <v>34</v>
+      </c>
+      <c r="C70" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D70" s="1">
+        <v>3</v>
+      </c>
+      <c r="E70" s="1">
+        <v>5</v>
+      </c>
+      <c r="F70" s="1">
+        <v>1</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B71" s="1">
+        <v>34</v>
+      </c>
+      <c r="C71" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D71" s="1">
+        <v>3</v>
+      </c>
+      <c r="E71" s="1">
+        <v>6</v>
+      </c>
+      <c r="F71" s="1">
+        <v>2</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B72" s="1">
+        <v>34</v>
+      </c>
+      <c r="C72" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D72" s="1">
+        <v>3</v>
+      </c>
+      <c r="E72" s="1">
+        <v>7</v>
+      </c>
+      <c r="F72" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B73" s="1">
+        <v>34</v>
+      </c>
+      <c r="C73" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D73" s="1">
+        <v>4</v>
+      </c>
+      <c r="E73" s="1">
+        <v>1</v>
+      </c>
+      <c r="F73" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B74" s="1">
+        <v>34</v>
+      </c>
+      <c r="C74" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D74" s="1">
+        <v>4</v>
+      </c>
+      <c r="E74" s="1">
+        <v>2</v>
+      </c>
+      <c r="F74" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B75" s="1">
+        <v>34</v>
+      </c>
+      <c r="C75" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D75" s="1">
+        <v>4</v>
+      </c>
+      <c r="E75" s="1">
+        <v>3</v>
+      </c>
+      <c r="F75" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B76" s="1">
+        <v>34</v>
+      </c>
+      <c r="C76" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D76" s="1">
+        <v>4</v>
+      </c>
+      <c r="E76" s="1">
+        <v>4</v>
+      </c>
+      <c r="F76" s="1">
+        <v>1</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B77" s="1">
+        <v>34</v>
+      </c>
+      <c r="C77" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D77" s="1">
+        <v>4</v>
+      </c>
+      <c r="E77" s="1">
+        <v>5</v>
+      </c>
+      <c r="F77" s="1">
+        <v>1</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B78" s="1">
+        <v>34</v>
+      </c>
+      <c r="C78" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D78" s="1">
+        <v>4</v>
+      </c>
+      <c r="E78" s="1">
+        <v>6</v>
+      </c>
+      <c r="F78" s="1">
+        <v>1</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B79" s="1">
+        <v>34</v>
+      </c>
+      <c r="C79" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D79" s="1">
+        <v>4</v>
+      </c>
+      <c r="E79" s="1">
+        <v>7</v>
+      </c>
+      <c r="F79" s="1">
+        <v>1</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B80" s="1">
+        <v>34</v>
+      </c>
+      <c r="C80" s="2">
+        <v>43172</v>
+      </c>
+      <c r="D80" s="1">
+        <v>4</v>
+      </c>
+      <c r="E80" s="1">
+        <v>8</v>
+      </c>
+      <c r="F80" s="1">
+        <v>1</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B81" s="1">
+        <v>34</v>
+      </c>
+      <c r="C81" s="2">
+        <v>43173</v>
+      </c>
+      <c r="D81" s="1">
+        <v>1</v>
+      </c>
+      <c r="E81" s="1">
+        <v>1</v>
+      </c>
+      <c r="F81" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B82" s="1">
+        <v>34</v>
+      </c>
+      <c r="C82" s="2">
+        <v>43173</v>
+      </c>
+      <c r="D82" s="1">
+        <v>1</v>
+      </c>
+      <c r="E82" s="1">
+        <v>2</v>
+      </c>
+      <c r="F82" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B83" s="1">
+        <v>34</v>
+      </c>
+      <c r="C83" s="2">
+        <v>43173</v>
+      </c>
+      <c r="D83" s="1">
+        <v>1</v>
+      </c>
+      <c r="E83" s="1">
+        <v>3</v>
+      </c>
+      <c r="F83" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B84" s="1">
+        <v>34</v>
+      </c>
+      <c r="C84" s="2">
+        <v>43173</v>
+      </c>
+      <c r="D84" s="1">
+        <v>1</v>
+      </c>
+      <c r="E84" s="1">
+        <v>4</v>
+      </c>
+      <c r="F84" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B85" s="1">
+        <v>34</v>
+      </c>
+      <c r="C85" s="2">
+        <v>43173</v>
+      </c>
+      <c r="D85" s="1">
+        <v>3</v>
+      </c>
+      <c r="E85" s="1">
+        <v>1</v>
+      </c>
+      <c r="F85" s="1">
+        <v>1</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B86" s="1">
+        <v>34</v>
+      </c>
+      <c r="C86" s="2">
+        <v>43173</v>
+      </c>
+      <c r="D86" s="1">
+        <v>3</v>
+      </c>
+      <c r="E86" s="1">
+        <v>2</v>
+      </c>
+      <c r="F86" s="1">
+        <v>2</v>
+      </c>
+      <c r="K86" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B87" s="1">
+        <v>34</v>
+      </c>
+      <c r="C87" s="2">
+        <v>43173</v>
+      </c>
+      <c r="D87" s="1">
+        <v>4</v>
+      </c>
+      <c r="E87" s="1">
+        <v>1</v>
+      </c>
+      <c r="F87" s="1">
+        <v>2</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B88" s="1">
+        <v>34</v>
+      </c>
+      <c r="C88" s="2">
+        <v>43173</v>
+      </c>
+      <c r="D88" s="1">
+        <v>4</v>
+      </c>
+      <c r="E88" s="1">
+        <v>2</v>
+      </c>
+      <c r="F88" s="1">
+        <v>2</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B89" s="1">
+        <v>34</v>
+      </c>
+      <c r="C89" s="2">
+        <v>43173</v>
+      </c>
+      <c r="D89" s="1">
+        <v>4</v>
+      </c>
+      <c r="E89" s="1">
+        <v>3</v>
+      </c>
+      <c r="F89" s="1">
+        <v>2</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B90" s="1">
+        <v>34</v>
+      </c>
+      <c r="C90" s="2">
+        <v>43173</v>
+      </c>
+      <c r="D90" s="1">
+        <v>4</v>
+      </c>
+      <c r="E90" s="1">
+        <v>4</v>
+      </c>
+      <c r="F90" s="1">
+        <v>1</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B91" s="1">
+        <v>34</v>
+      </c>
+      <c r="C91" s="2">
+        <v>43173</v>
+      </c>
+      <c r="D91" s="1">
+        <v>4</v>
+      </c>
+      <c r="E91" s="1">
+        <v>5</v>
+      </c>
+      <c r="F91" s="1">
+        <v>2</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B92" s="1">
+        <v>34</v>
+      </c>
+      <c r="C92" s="2">
+        <v>43173</v>
+      </c>
+      <c r="D92" s="1">
+        <v>4</v>
+      </c>
+      <c r="E92" s="1">
+        <v>6</v>
+      </c>
+      <c r="F92" s="1">
+        <v>1</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B93" s="1">
+        <v>34</v>
+      </c>
+      <c r="C93" s="2">
+        <v>43174</v>
+      </c>
+      <c r="D93" s="1">
+        <v>1</v>
+      </c>
+      <c r="E93" s="1">
+        <v>1</v>
+      </c>
+      <c r="F93" s="1">
+        <v>1</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B94" s="1">
+        <v>34</v>
+      </c>
+      <c r="C94" s="2">
+        <v>43174</v>
+      </c>
+      <c r="D94" s="1">
+        <v>3</v>
+      </c>
+      <c r="E94" s="1">
+        <v>1</v>
+      </c>
+      <c r="F94" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B95" s="1">
+        <v>34</v>
+      </c>
+      <c r="C95" s="2">
+        <v>43174</v>
+      </c>
+      <c r="D95" s="1">
+        <v>3</v>
+      </c>
+      <c r="E95" s="1">
+        <v>2</v>
+      </c>
+      <c r="F95" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B96" s="1">
+        <v>34</v>
+      </c>
+      <c r="C96" s="2">
+        <v>43174</v>
+      </c>
+      <c r="D96" s="1">
+        <v>3</v>
+      </c>
+      <c r="E96" s="1">
+        <v>3</v>
+      </c>
+      <c r="F96" s="1">
+        <v>0</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B97" s="1">
+        <v>34</v>
+      </c>
+      <c r="C97" s="2">
+        <v>43174</v>
+      </c>
+      <c r="D97" s="1">
+        <v>4</v>
+      </c>
+      <c r="E97" s="1">
+        <v>1</v>
+      </c>
+      <c r="F97" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B98" s="1">
+        <v>34</v>
+      </c>
+      <c r="C98" s="2">
+        <v>43174</v>
+      </c>
+      <c r="D98" s="1">
+        <v>4</v>
+      </c>
+      <c r="E98" s="1">
+        <v>2</v>
+      </c>
+      <c r="F98" s="1">
+        <v>1</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C99" s="2"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C100" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:H1"/>
-  <conditionalFormatting sqref="F1:F2 F6:F1048576">
-    <cfRule type="colorScale" priority="39">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F2 F6:F1048576">
-    <cfRule type="colorScale" priority="351">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F2 F6:F1048576">
-    <cfRule type="colorScale" priority="354">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F2 F6:F1048576">
-    <cfRule type="colorScale" priority="357">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F2 F6:F1048576">
-    <cfRule type="colorScale" priority="360">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F2 F6:F1048576">
-    <cfRule type="colorScale" priority="363">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F2 F6:F1048576">
-    <cfRule type="colorScale" priority="366">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F2 F6:F1048576">
-    <cfRule type="colorScale" priority="369">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F2 F6:F1048576">
-    <cfRule type="colorScale" priority="375">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F2 F6:F1048576">
-    <cfRule type="colorScale" priority="378">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F2 F6:F1048576">
-    <cfRule type="colorScale" priority="381">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F2 F6:F1048576">
-    <cfRule type="colorScale" priority="384">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3">
-    <cfRule type="colorScale" priority="27">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
+  <autoFilter ref="B1:H95"/>
   <conditionalFormatting sqref="F3">
     <cfRule type="colorScale" priority="28">
       <colorScale>
@@ -2392,8 +3207,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4">
-    <cfRule type="colorScale" priority="15">
+  <conditionalFormatting sqref="F3">
+    <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2536,7 +3351,151 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F4 F6:F1048576">
+  <conditionalFormatting sqref="F4">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -2560,139 +3519,31 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
+  <conditionalFormatting sqref="F1:F2 F73:F1048576 F6:F71">
+    <cfRule type="colorScale" priority="386">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F4 F73:F1048576 F6:F71">
+    <cfRule type="colorScale" priority="434">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
update spike sorting summary bat 9861
</commit_message>
<xml_diff>
--- a/inclusion_lists/cells_summary.xlsx
+++ b/inclusion_lists/cells_summary.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="195">
   <si>
     <t>bat</t>
   </si>
@@ -506,6 +506,114 @@
   </si>
   <si>
     <t>b9861_d180519_TT3_SS01</t>
+  </si>
+  <si>
+    <t>b9861_d180521_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b9861_d180521_TT1_SS02</t>
+  </si>
+  <si>
+    <t>b9861_d180521_TT1_SS03</t>
+  </si>
+  <si>
+    <t>b9861_d180521_TT1_SS04</t>
+  </si>
+  <si>
+    <t>b9861_d180521_TT2_SS01</t>
+  </si>
+  <si>
+    <t>weird spikes partially stable</t>
+  </si>
+  <si>
+    <t>b9861_d180521_TT2_SS02</t>
+  </si>
+  <si>
+    <t>b9861_d180521_TT2_SS03</t>
+  </si>
+  <si>
+    <t>b9861_d180521_TT2_SS04</t>
+  </si>
+  <si>
+    <t>too close to the noise; partially stable</t>
+  </si>
+  <si>
+    <t>b9861_d180521_TT2_SS05</t>
+  </si>
+  <si>
+    <t>b9861_d180521_TT2_SS06</t>
+  </si>
+  <si>
+    <t>b9861_d180521_TT2_SS07</t>
+  </si>
+  <si>
+    <t>b9861_d180521_TT2_SS08</t>
+  </si>
+  <si>
+    <t>b9861_d180521_TT2_SS09</t>
+  </si>
+  <si>
+    <t>b9861_d180521_TT3_SS01</t>
+  </si>
+  <si>
+    <t>inverted spikes</t>
+  </si>
+  <si>
+    <t>b9861_d180521_TT4_SS01</t>
+  </si>
+  <si>
+    <t>b9861_d180521_TT4_SS02</t>
+  </si>
+  <si>
+    <t>very low spikes count</t>
+  </si>
+  <si>
+    <t>b9861_d180521_TT4_SS03</t>
+  </si>
+  <si>
+    <t>b9861_d180521_TT4_SS04</t>
+  </si>
+  <si>
+    <t>b9861_d180521_TT4_SS05</t>
+  </si>
+  <si>
+    <t>b9861_d180522_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b9861_d180522_TT1_SS02</t>
+  </si>
+  <si>
+    <t>b9861_d180522_TT1_SS03</t>
+  </si>
+  <si>
+    <t>b9861_d180522_TT1_SS04</t>
+  </si>
+  <si>
+    <t>b9861_d180522_TT1_SS05</t>
+  </si>
+  <si>
+    <t>b9861_d180522_TT1_SS06</t>
+  </si>
+  <si>
+    <t>b9861_d180522_TT1_SS07</t>
+  </si>
+  <si>
+    <t>b9861_d180522_TT4_SS01</t>
+  </si>
+  <si>
+    <t>b9861_d180522_TT4_SS02</t>
+  </si>
+  <si>
+    <t>merging with unit 3</t>
+  </si>
+  <si>
+    <t>b9861_d180522_TT4_SS03</t>
+  </si>
+  <si>
+    <t>merging with unit 2 + close to noise</t>
+  </si>
+  <si>
+    <t>b9861_d180522_TT4_SS04</t>
   </si>
 </sst>
 </file>
@@ -842,11 +950,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S111"/>
+  <dimension ref="A1:S141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I112" sqref="I112"/>
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G138" sqref="G138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3442,6 +3550,717 @@
       </c>
       <c r="K111" s="1" t="s">
         <v>134</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A112" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B112" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C112" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D112" s="1">
+        <v>1</v>
+      </c>
+      <c r="E112" s="1">
+        <v>1</v>
+      </c>
+      <c r="F112" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B113" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C113" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D113" s="1">
+        <v>1</v>
+      </c>
+      <c r="E113" s="1">
+        <v>2</v>
+      </c>
+      <c r="F113" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A114" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B114" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C114" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D114" s="1">
+        <v>1</v>
+      </c>
+      <c r="E114" s="1">
+        <v>3</v>
+      </c>
+      <c r="F114" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A115" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B115" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C115" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D115" s="1">
+        <v>1</v>
+      </c>
+      <c r="E115" s="1">
+        <v>4</v>
+      </c>
+      <c r="F115" s="1">
+        <v>1</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B116" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C116" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D116" s="1">
+        <v>2</v>
+      </c>
+      <c r="E116" s="1">
+        <v>1</v>
+      </c>
+      <c r="F116" s="1">
+        <v>2</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="I116" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B117" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C117" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D117" s="1">
+        <v>2</v>
+      </c>
+      <c r="E117" s="1">
+        <v>2</v>
+      </c>
+      <c r="F117" s="1">
+        <v>2</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I117" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K117" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B118" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C118" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D118" s="1">
+        <v>2</v>
+      </c>
+      <c r="E118" s="1">
+        <v>3</v>
+      </c>
+      <c r="F118" s="1">
+        <v>2</v>
+      </c>
+      <c r="I118" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K118" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A119" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B119" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C119" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D119" s="1">
+        <v>2</v>
+      </c>
+      <c r="E119" s="1">
+        <v>4</v>
+      </c>
+      <c r="F119" s="1">
+        <v>2</v>
+      </c>
+      <c r="I119" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K119" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B120" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C120" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D120" s="1">
+        <v>2</v>
+      </c>
+      <c r="E120" s="1">
+        <v>5</v>
+      </c>
+      <c r="F120" s="1">
+        <v>1</v>
+      </c>
+      <c r="G120" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="I120" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B121" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C121" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D121" s="1">
+        <v>2</v>
+      </c>
+      <c r="E121" s="1">
+        <v>6</v>
+      </c>
+      <c r="F121" s="1">
+        <v>1</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I121" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A122" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B122" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C122" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D122" s="1">
+        <v>2</v>
+      </c>
+      <c r="E122" s="1">
+        <v>7</v>
+      </c>
+      <c r="F122" s="1">
+        <v>1</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I122" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A123" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B123" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C123" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D123" s="1">
+        <v>2</v>
+      </c>
+      <c r="E123" s="1">
+        <v>8</v>
+      </c>
+      <c r="F123" s="1">
+        <v>1</v>
+      </c>
+      <c r="G123" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I123" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B124" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C124" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D124" s="1">
+        <v>2</v>
+      </c>
+      <c r="E124" s="1">
+        <v>9</v>
+      </c>
+      <c r="F124" s="1">
+        <v>1</v>
+      </c>
+      <c r="G124" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I124" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A125" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B125" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C125" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D125" s="1">
+        <v>3</v>
+      </c>
+      <c r="E125" s="1">
+        <v>1</v>
+      </c>
+      <c r="F125" s="1">
+        <v>2</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="I125" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K125" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B126" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C126" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D126" s="1">
+        <v>4</v>
+      </c>
+      <c r="E126" s="1">
+        <v>1</v>
+      </c>
+      <c r="F126" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B127" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C127" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D127" s="1">
+        <v>4</v>
+      </c>
+      <c r="E127" s="1">
+        <v>2</v>
+      </c>
+      <c r="F127" s="1">
+        <v>1</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A128" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B128" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C128" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D128" s="1">
+        <v>4</v>
+      </c>
+      <c r="E128" s="1">
+        <v>3</v>
+      </c>
+      <c r="F128" s="1">
+        <v>2</v>
+      </c>
+      <c r="G128" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A129" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B129" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C129" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D129" s="1">
+        <v>4</v>
+      </c>
+      <c r="E129" s="1">
+        <v>4</v>
+      </c>
+      <c r="F129" s="1">
+        <v>2</v>
+      </c>
+      <c r="G129" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B130" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C130" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D130" s="1">
+        <v>4</v>
+      </c>
+      <c r="E130" s="1">
+        <v>5</v>
+      </c>
+      <c r="F130" s="1">
+        <v>1</v>
+      </c>
+      <c r="G130" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A131" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B131" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C131" s="2">
+        <v>43242</v>
+      </c>
+      <c r="D131" s="1">
+        <v>1</v>
+      </c>
+      <c r="E131" s="1">
+        <v>1</v>
+      </c>
+      <c r="F131" s="1">
+        <v>2</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="K131" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A132" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B132" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C132" s="2">
+        <v>43242</v>
+      </c>
+      <c r="D132" s="1">
+        <v>1</v>
+      </c>
+      <c r="E132" s="1">
+        <v>2</v>
+      </c>
+      <c r="F132" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A133" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B133" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C133" s="2">
+        <v>43242</v>
+      </c>
+      <c r="D133" s="1">
+        <v>1</v>
+      </c>
+      <c r="E133" s="1">
+        <v>3</v>
+      </c>
+      <c r="F133" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A134" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B134" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C134" s="2">
+        <v>43242</v>
+      </c>
+      <c r="D134" s="1">
+        <v>1</v>
+      </c>
+      <c r="E134" s="1">
+        <v>4</v>
+      </c>
+      <c r="F134" s="1">
+        <v>1</v>
+      </c>
+      <c r="G134" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A135" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B135" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C135" s="2">
+        <v>43242</v>
+      </c>
+      <c r="D135" s="1">
+        <v>1</v>
+      </c>
+      <c r="E135" s="1">
+        <v>5</v>
+      </c>
+      <c r="F135" s="1">
+        <v>1</v>
+      </c>
+      <c r="G135" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A136" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B136" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C136" s="2">
+        <v>43242</v>
+      </c>
+      <c r="D136" s="1">
+        <v>1</v>
+      </c>
+      <c r="E136" s="1">
+        <v>6</v>
+      </c>
+      <c r="F136" s="1">
+        <v>1</v>
+      </c>
+      <c r="G136" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A137" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B137" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C137" s="2">
+        <v>43242</v>
+      </c>
+      <c r="D137" s="1">
+        <v>1</v>
+      </c>
+      <c r="E137" s="1">
+        <v>7</v>
+      </c>
+      <c r="F137" s="1">
+        <v>1</v>
+      </c>
+      <c r="G137" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A138" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B138" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C138" s="2">
+        <v>43242</v>
+      </c>
+      <c r="D138" s="1">
+        <v>4</v>
+      </c>
+      <c r="E138" s="1">
+        <v>1</v>
+      </c>
+      <c r="F138" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A139" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B139" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C139" s="2">
+        <v>43242</v>
+      </c>
+      <c r="D139" s="1">
+        <v>4</v>
+      </c>
+      <c r="E139" s="1">
+        <v>2</v>
+      </c>
+      <c r="F139" s="1">
+        <v>1</v>
+      </c>
+      <c r="G139" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A140" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B140" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C140" s="2">
+        <v>43242</v>
+      </c>
+      <c r="D140" s="1">
+        <v>4</v>
+      </c>
+      <c r="E140" s="1">
+        <v>3</v>
+      </c>
+      <c r="F140" s="1">
+        <v>1</v>
+      </c>
+      <c r="G140" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A141" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B141" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C141" s="2">
+        <v>43242</v>
+      </c>
+      <c r="D141" s="1">
+        <v>4</v>
+      </c>
+      <c r="E141" s="1">
+        <v>4</v>
+      </c>
+      <c r="F141" s="1">
+        <v>1</v>
+      </c>
+      <c r="G141" s="1" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update spikes sorting summaries + small fixes
</commit_message>
<xml_diff>
--- a/inclusion_lists/cells_summary.xlsx
+++ b/inclusion_lists/cells_summary.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="367">
   <si>
     <t>bat</t>
   </si>
@@ -1022,6 +1022,114 @@
   </si>
   <si>
     <t>leftovers, ignore this unit</t>
+  </si>
+  <si>
+    <t>b9861_d180530_TT2_SS01</t>
+  </si>
+  <si>
+    <t>b9861_d180530_TT2_SS02</t>
+  </si>
+  <si>
+    <t>b9861_d180530_TT2_SS03</t>
+  </si>
+  <si>
+    <t>b9861_d180531_TT3_SS01</t>
+  </si>
+  <si>
+    <t>b9861_d180531_TT4_SS01</t>
+  </si>
+  <si>
+    <t>b9861_d180531_TT4_SS02</t>
+  </si>
+  <si>
+    <t>b9861_d180601_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b9861_d180601_TT1_SS02</t>
+  </si>
+  <si>
+    <t>b9861_d180601_TT1_SS03</t>
+  </si>
+  <si>
+    <t>b9861_d180601_TT3_SS02</t>
+  </si>
+  <si>
+    <t>b9861_d180601_TT3_SS01</t>
+  </si>
+  <si>
+    <t>b9861_d180601_TT3_SS03</t>
+  </si>
+  <si>
+    <t>b9861_d180601_TT3_SS04</t>
+  </si>
+  <si>
+    <t>b9861_d180601_TT3_SS05</t>
+  </si>
+  <si>
+    <t>b9861_d180603_TT1_SS01</t>
+  </si>
+  <si>
+    <t>lots of flight artifacts in that TT</t>
+  </si>
+  <si>
+    <t>b9861_d180603_TT2_SS01</t>
+  </si>
+  <si>
+    <t>b9861_d180603_TT3_SS01</t>
+  </si>
+  <si>
+    <t>b9861_d180603_TT3_SS02</t>
+  </si>
+  <si>
+    <t>b9861_d180604_TT3_SS01</t>
+  </si>
+  <si>
+    <t>b9861_d180604_TT3_SS02</t>
+  </si>
+  <si>
+    <t>b9861_d180604_TT3_SS03</t>
+  </si>
+  <si>
+    <t>b9861_d180604_TT3_SS04</t>
+  </si>
+  <si>
+    <t>b9861_d180604_TT3_SS05</t>
+  </si>
+  <si>
+    <t>b9861_d180605_TT3_SS01</t>
+  </si>
+  <si>
+    <t>b9861_d180605_TT3_SS02</t>
+  </si>
+  <si>
+    <t>b9861_d180606_TT3_SS02</t>
+  </si>
+  <si>
+    <t>b9861_d180606_TT3_SS01</t>
+  </si>
+  <si>
+    <t>b9861_d180606_TT3_SS03</t>
+  </si>
+  <si>
+    <t>b9861_d180606_TT3_SS04</t>
+  </si>
+  <si>
+    <t>b9861_d180606_TT3_SS05</t>
+  </si>
+  <si>
+    <t>b9861_d180606_TT3_SS06</t>
+  </si>
+  <si>
+    <t>b9861_d180607_TT3_SS01</t>
+  </si>
+  <si>
+    <t>b9861_d180609_TT3_SS01</t>
+  </si>
+  <si>
+    <t>b9861_d180609_TT3_SS02</t>
+  </si>
+  <si>
+    <t>b9861_d180610_TT3_SS01</t>
   </si>
 </sst>
 </file>
@@ -1359,11 +1467,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:S260"/>
+  <dimension ref="A1:S295"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A219" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G263" sqref="G263"/>
+      <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G295" sqref="G295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7280,6 +7388,784 @@
         <v>1</v>
       </c>
       <c r="G260" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A261" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B261" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C261" s="2">
+        <v>43250</v>
+      </c>
+      <c r="D261" s="1">
+        <v>2</v>
+      </c>
+      <c r="E261" s="1">
+        <v>1</v>
+      </c>
+      <c r="F261" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A262" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B262" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C262" s="2">
+        <v>43250</v>
+      </c>
+      <c r="D262" s="1">
+        <v>2</v>
+      </c>
+      <c r="E262" s="1">
+        <v>2</v>
+      </c>
+      <c r="F262" s="1">
+        <v>1</v>
+      </c>
+      <c r="G262" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A263" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B263" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C263" s="2">
+        <v>43250</v>
+      </c>
+      <c r="D263" s="1">
+        <v>2</v>
+      </c>
+      <c r="E263" s="1">
+        <v>3</v>
+      </c>
+      <c r="F263" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A264" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B264" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C264" s="2">
+        <v>43251</v>
+      </c>
+      <c r="D264" s="1">
+        <v>3</v>
+      </c>
+      <c r="E264" s="1">
+        <v>1</v>
+      </c>
+      <c r="F264" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A265" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B265" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C265" s="2">
+        <v>43251</v>
+      </c>
+      <c r="D265" s="1">
+        <v>4</v>
+      </c>
+      <c r="E265" s="1">
+        <v>1</v>
+      </c>
+      <c r="F265" s="1">
+        <v>2</v>
+      </c>
+      <c r="G265" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A266" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B266" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C266" s="2">
+        <v>43251</v>
+      </c>
+      <c r="D266" s="1">
+        <v>4</v>
+      </c>
+      <c r="E266" s="1">
+        <v>2</v>
+      </c>
+      <c r="F266" s="1">
+        <v>1</v>
+      </c>
+      <c r="G266" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A267" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B267" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C267" s="2">
+        <v>43252</v>
+      </c>
+      <c r="D267" s="1">
+        <v>1</v>
+      </c>
+      <c r="E267" s="1">
+        <v>1</v>
+      </c>
+      <c r="F267" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A268" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B268" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C268" s="2">
+        <v>43252</v>
+      </c>
+      <c r="D268" s="1">
+        <v>1</v>
+      </c>
+      <c r="E268" s="1">
+        <v>2</v>
+      </c>
+      <c r="F268" s="1">
+        <v>1</v>
+      </c>
+      <c r="G268" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="269" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A269" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B269" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C269" s="2">
+        <v>43252</v>
+      </c>
+      <c r="D269" s="1">
+        <v>1</v>
+      </c>
+      <c r="E269" s="1">
+        <v>3</v>
+      </c>
+      <c r="F269" s="1">
+        <v>1</v>
+      </c>
+      <c r="G269" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="270" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A270" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B270" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C270" s="2">
+        <v>43252</v>
+      </c>
+      <c r="D270" s="1">
+        <v>3</v>
+      </c>
+      <c r="E270" s="1">
+        <v>1</v>
+      </c>
+      <c r="F270" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A271" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B271" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C271" s="2">
+        <v>43252</v>
+      </c>
+      <c r="D271" s="1">
+        <v>3</v>
+      </c>
+      <c r="E271" s="1">
+        <v>2</v>
+      </c>
+      <c r="F271" s="1">
+        <v>1</v>
+      </c>
+      <c r="G271" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A272" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B272" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C272" s="2">
+        <v>43252</v>
+      </c>
+      <c r="D272" s="1">
+        <v>3</v>
+      </c>
+      <c r="E272" s="1">
+        <v>3</v>
+      </c>
+      <c r="F272" s="1">
+        <v>1</v>
+      </c>
+      <c r="G272" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A273" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B273" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C273" s="2">
+        <v>43252</v>
+      </c>
+      <c r="D273" s="1">
+        <v>3</v>
+      </c>
+      <c r="E273" s="1">
+        <v>4</v>
+      </c>
+      <c r="F273" s="1">
+        <v>1</v>
+      </c>
+      <c r="G273" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A274" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B274" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C274" s="2">
+        <v>43252</v>
+      </c>
+      <c r="D274" s="1">
+        <v>3</v>
+      </c>
+      <c r="E274" s="1">
+        <v>5</v>
+      </c>
+      <c r="F274" s="1">
+        <v>1</v>
+      </c>
+      <c r="G274" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="275" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A275" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B275" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C275" s="2">
+        <v>43254</v>
+      </c>
+      <c r="D275" s="1">
+        <v>1</v>
+      </c>
+      <c r="E275" s="1">
+        <v>1</v>
+      </c>
+      <c r="F275" s="1">
+        <v>2</v>
+      </c>
+      <c r="G275" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="276" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A276" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B276" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C276" s="2">
+        <v>43254</v>
+      </c>
+      <c r="D276" s="1">
+        <v>2</v>
+      </c>
+      <c r="E276" s="1">
+        <v>1</v>
+      </c>
+      <c r="F276" s="1">
+        <v>1</v>
+      </c>
+      <c r="G276" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="277" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A277" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B277" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C277" s="2">
+        <v>43254</v>
+      </c>
+      <c r="D277" s="1">
+        <v>3</v>
+      </c>
+      <c r="E277" s="1">
+        <v>1</v>
+      </c>
+      <c r="F277" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="278" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A278" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B278" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C278" s="2">
+        <v>43254</v>
+      </c>
+      <c r="D278" s="1">
+        <v>3</v>
+      </c>
+      <c r="E278" s="1">
+        <v>2</v>
+      </c>
+      <c r="F278" s="1">
+        <v>1</v>
+      </c>
+      <c r="G278" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="279" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A279" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B279" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C279" s="2">
+        <v>43255</v>
+      </c>
+      <c r="D279" s="1">
+        <v>3</v>
+      </c>
+      <c r="E279" s="1">
+        <v>1</v>
+      </c>
+      <c r="F279" s="1">
+        <v>1</v>
+      </c>
+      <c r="G279" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="280" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A280" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B280" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C280" s="2">
+        <v>43255</v>
+      </c>
+      <c r="D280" s="1">
+        <v>3</v>
+      </c>
+      <c r="E280" s="1">
+        <v>2</v>
+      </c>
+      <c r="F280" s="1">
+        <v>1</v>
+      </c>
+      <c r="G280" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="281" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A281" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B281" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C281" s="2">
+        <v>43255</v>
+      </c>
+      <c r="D281" s="1">
+        <v>3</v>
+      </c>
+      <c r="E281" s="1">
+        <v>3</v>
+      </c>
+      <c r="F281" s="1">
+        <v>1</v>
+      </c>
+      <c r="G281" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A282" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B282" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C282" s="2">
+        <v>43255</v>
+      </c>
+      <c r="D282" s="1">
+        <v>3</v>
+      </c>
+      <c r="E282" s="1">
+        <v>4</v>
+      </c>
+      <c r="F282" s="1">
+        <v>1</v>
+      </c>
+      <c r="G282" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A283" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B283" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C283" s="2">
+        <v>43255</v>
+      </c>
+      <c r="D283" s="1">
+        <v>3</v>
+      </c>
+      <c r="E283" s="1">
+        <v>5</v>
+      </c>
+      <c r="F283" s="1">
+        <v>1</v>
+      </c>
+      <c r="G283" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="284" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A284" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B284" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C284" s="2">
+        <v>43256</v>
+      </c>
+      <c r="D284" s="1">
+        <v>3</v>
+      </c>
+      <c r="E284" s="1">
+        <v>1</v>
+      </c>
+      <c r="F284" s="1">
+        <v>1</v>
+      </c>
+      <c r="G284" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A285" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B285" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C285" s="2">
+        <v>43256</v>
+      </c>
+      <c r="D285" s="1">
+        <v>3</v>
+      </c>
+      <c r="E285" s="1">
+        <v>2</v>
+      </c>
+      <c r="F285" s="1">
+        <v>1</v>
+      </c>
+      <c r="G285" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A286" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B286" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C286" s="2">
+        <v>43257</v>
+      </c>
+      <c r="D286" s="1">
+        <v>3</v>
+      </c>
+      <c r="E286" s="1">
+        <v>1</v>
+      </c>
+      <c r="F286" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A287" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B287" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C287" s="2">
+        <v>43257</v>
+      </c>
+      <c r="D287" s="1">
+        <v>3</v>
+      </c>
+      <c r="E287" s="1">
+        <v>2</v>
+      </c>
+      <c r="F287" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A288" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B288" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C288" s="2">
+        <v>43257</v>
+      </c>
+      <c r="D288" s="1">
+        <v>3</v>
+      </c>
+      <c r="E288" s="1">
+        <v>3</v>
+      </c>
+      <c r="F288" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="289" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A289" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="B289" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C289" s="2">
+        <v>43257</v>
+      </c>
+      <c r="D289" s="1">
+        <v>3</v>
+      </c>
+      <c r="E289" s="1">
+        <v>4</v>
+      </c>
+      <c r="F289" s="1">
+        <v>1</v>
+      </c>
+      <c r="G289" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A290" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B290" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C290" s="2">
+        <v>43257</v>
+      </c>
+      <c r="D290" s="1">
+        <v>3</v>
+      </c>
+      <c r="E290" s="1">
+        <v>5</v>
+      </c>
+      <c r="F290" s="1">
+        <v>1</v>
+      </c>
+      <c r="G290" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A291" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B291" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C291" s="2">
+        <v>43257</v>
+      </c>
+      <c r="D291" s="1">
+        <v>3</v>
+      </c>
+      <c r="E291" s="1">
+        <v>6</v>
+      </c>
+      <c r="F291" s="1">
+        <v>1</v>
+      </c>
+      <c r="G291" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A292" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B292" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C292" s="2">
+        <v>43258</v>
+      </c>
+      <c r="D292" s="1">
+        <v>3</v>
+      </c>
+      <c r="E292" s="1">
+        <v>1</v>
+      </c>
+      <c r="F292" s="1">
+        <v>1</v>
+      </c>
+      <c r="G292" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="293" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A293" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B293" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C293" s="2">
+        <v>43260</v>
+      </c>
+      <c r="D293" s="1">
+        <v>3</v>
+      </c>
+      <c r="E293" s="1">
+        <v>1</v>
+      </c>
+      <c r="F293" s="1">
+        <v>1</v>
+      </c>
+      <c r="G293" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="294" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A294" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B294" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C294" s="2">
+        <v>43260</v>
+      </c>
+      <c r="D294" s="1">
+        <v>3</v>
+      </c>
+      <c r="E294" s="1">
+        <v>2</v>
+      </c>
+      <c r="F294" s="1">
+        <v>1</v>
+      </c>
+      <c r="G294" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="295" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A295" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B295" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C295" s="2">
+        <v>43261</v>
+      </c>
+      <c r="D295" s="1">
+        <v>3</v>
+      </c>
+      <c r="E295" s="1">
+        <v>1</v>
+      </c>
+      <c r="F295" s="1">
+        <v>1</v>
+      </c>
+      <c r="G295" s="1" t="s">
         <v>154</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update sorting for bat 9861
</commit_message>
<xml_diff>
--- a/inclusion_lists/cells_summary.xlsx
+++ b/inclusion_lists/cells_summary.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="381">
   <si>
     <t>bat</t>
   </si>
@@ -1130,6 +1130,48 @@
   </si>
   <si>
     <t>b9861_d180610_TT3_SS01</t>
+  </si>
+  <si>
+    <t>b9861_d180611_TT3_SS01</t>
+  </si>
+  <si>
+    <t>b9861_d180612_TT3_SS01</t>
+  </si>
+  <si>
+    <t>b9861_d180615_TT3_SS01</t>
+  </si>
+  <si>
+    <t>b9861_d180615_TT3_SS02</t>
+  </si>
+  <si>
+    <t>b9861_d180615_TT3_SS03</t>
+  </si>
+  <si>
+    <t>b9861_d180615_TT3_SS04</t>
+  </si>
+  <si>
+    <t>b9861_d180616_TT3_SS01</t>
+  </si>
+  <si>
+    <t>low spikes counts</t>
+  </si>
+  <si>
+    <t>b9861_d180616_TT3_SS02</t>
+  </si>
+  <si>
+    <t>b9861_d180616_TT3_SS03</t>
+  </si>
+  <si>
+    <t>b9861_d180617_TT3_SS01</t>
+  </si>
+  <si>
+    <t>b9861_d180617_TT3_SS02</t>
+  </si>
+  <si>
+    <t>b9861_d180617_TT3_SS03</t>
+  </si>
+  <si>
+    <t>b9861_d180617_TT3_SS04</t>
   </si>
 </sst>
 </file>
@@ -1467,11 +1509,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:S295"/>
+  <dimension ref="A1:S308"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G295" sqref="G295"/>
+      <pane ySplit="1" topLeftCell="A269" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E310" sqref="E310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -8166,6 +8208,296 @@
         <v>1</v>
       </c>
       <c r="G295" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A296" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B296" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C296" s="2">
+        <v>43262</v>
+      </c>
+      <c r="D296" s="1">
+        <v>3</v>
+      </c>
+      <c r="E296" s="1">
+        <v>1</v>
+      </c>
+      <c r="F296" s="1">
+        <v>1</v>
+      </c>
+      <c r="G296" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="297" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A297" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B297" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C297" s="2">
+        <v>43263</v>
+      </c>
+      <c r="D297" s="1">
+        <v>3</v>
+      </c>
+      <c r="E297" s="1">
+        <v>1</v>
+      </c>
+      <c r="F297" s="1">
+        <v>1</v>
+      </c>
+      <c r="G297" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="298" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A298" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="B298" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C298" s="2">
+        <v>43266</v>
+      </c>
+      <c r="D298" s="1">
+        <v>3</v>
+      </c>
+      <c r="E298" s="1">
+        <v>1</v>
+      </c>
+      <c r="F298" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="299" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A299" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B299" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C299" s="2">
+        <v>43266</v>
+      </c>
+      <c r="D299" s="1">
+        <v>3</v>
+      </c>
+      <c r="E299" s="1">
+        <v>2</v>
+      </c>
+      <c r="F299" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="300" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A300" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B300" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C300" s="2">
+        <v>43266</v>
+      </c>
+      <c r="D300" s="1">
+        <v>3</v>
+      </c>
+      <c r="E300" s="1">
+        <v>3</v>
+      </c>
+      <c r="F300" s="1">
+        <v>1</v>
+      </c>
+      <c r="G300" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="301" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A301" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B301" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C301" s="2">
+        <v>43266</v>
+      </c>
+      <c r="D301" s="1">
+        <v>3</v>
+      </c>
+      <c r="E301" s="1">
+        <v>4</v>
+      </c>
+      <c r="F301" s="1">
+        <v>1</v>
+      </c>
+      <c r="G301" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="302" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A302" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B302" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C302" s="2">
+        <v>43267</v>
+      </c>
+      <c r="D302" s="1">
+        <v>3</v>
+      </c>
+      <c r="E302" s="1">
+        <v>1</v>
+      </c>
+      <c r="F302" s="1">
+        <v>2</v>
+      </c>
+      <c r="G302" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="303" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A303" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B303" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C303" s="2">
+        <v>43267</v>
+      </c>
+      <c r="D303" s="1">
+        <v>3</v>
+      </c>
+      <c r="E303" s="1">
+        <v>2</v>
+      </c>
+      <c r="F303" s="1">
+        <v>1</v>
+      </c>
+      <c r="G303" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="304" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A304" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B304" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C304" s="2">
+        <v>43267</v>
+      </c>
+      <c r="D304" s="1">
+        <v>3</v>
+      </c>
+      <c r="E304" s="1">
+        <v>3</v>
+      </c>
+      <c r="F304" s="1">
+        <v>1</v>
+      </c>
+      <c r="G304" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="305" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A305" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B305" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C305" s="2">
+        <v>43268</v>
+      </c>
+      <c r="D305" s="1">
+        <v>3</v>
+      </c>
+      <c r="E305" s="1">
+        <v>1</v>
+      </c>
+      <c r="F305" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="306" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A306" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B306" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C306" s="2">
+        <v>43268</v>
+      </c>
+      <c r="D306" s="1">
+        <v>3</v>
+      </c>
+      <c r="E306" s="1">
+        <v>2</v>
+      </c>
+      <c r="F306" s="1">
+        <v>1</v>
+      </c>
+      <c r="G306" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="307" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A307" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B307" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C307" s="2">
+        <v>43268</v>
+      </c>
+      <c r="D307" s="1">
+        <v>3</v>
+      </c>
+      <c r="E307" s="1">
+        <v>3</v>
+      </c>
+      <c r="F307" s="1">
+        <v>1</v>
+      </c>
+      <c r="G307" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="308" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A308" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B308" s="1">
+        <v>9861</v>
+      </c>
+      <c r="C308" s="2">
+        <v>43268</v>
+      </c>
+      <c r="D308" s="1">
+        <v>3</v>
+      </c>
+      <c r="E308" s="1">
+        <v>4</v>
+      </c>
+      <c r="F308" s="1">
+        <v>1</v>
+      </c>
+      <c r="G308" s="1" t="s">
         <v>154</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update sorting for bat 2289
</commit_message>
<xml_diff>
--- a/inclusion_lists/cells_summary.xlsx
+++ b/inclusion_lists/cells_summary.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$H$260</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$H$308</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="443">
   <si>
     <t>bat</t>
   </si>
@@ -1172,6 +1172,192 @@
   </si>
   <si>
     <t>b9861_d180617_TT3_SS04</t>
+  </si>
+  <si>
+    <t>b2289_d180514_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b2289_d180514_TT1_SS02</t>
+  </si>
+  <si>
+    <t>b2289_d180514_TT1_SS03</t>
+  </si>
+  <si>
+    <t>b2289_d180514_TT1_SS04</t>
+  </si>
+  <si>
+    <t>too much into the noise</t>
+  </si>
+  <si>
+    <t>b2289_d180515_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b2289_d180514_TT1_SS01???</t>
+  </si>
+  <si>
+    <t>b2289_d180515_TT1_SS02</t>
+  </si>
+  <si>
+    <t>b2289_d180515_TT1_SS03</t>
+  </si>
+  <si>
+    <t>b2289_d180515_TT1_SS04</t>
+  </si>
+  <si>
+    <t>b2289_d180518_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b2289_d180518_TT1_SS02</t>
+  </si>
+  <si>
+    <t>b2289_d180518_TT1_SS03</t>
+  </si>
+  <si>
+    <t>b2289_d180518_TT1_SS04</t>
+  </si>
+  <si>
+    <t>b2289_d180518_TT1_SS05</t>
+  </si>
+  <si>
+    <t>b2289_d180518_TT1_SS06</t>
+  </si>
+  <si>
+    <t>b2289_d180518_TT1_SS07</t>
+  </si>
+  <si>
+    <t>b2289_d180518_TT2_SS01</t>
+  </si>
+  <si>
+    <t>b2289_d180518_TT2_SS02</t>
+  </si>
+  <si>
+    <t>b2289_d180518_TT2_SS03</t>
+  </si>
+  <si>
+    <t>b2289_d180518_TT2_SS04</t>
+  </si>
+  <si>
+    <t>b2289_d180518_TT2_SS05</t>
+  </si>
+  <si>
+    <t>b2289_d180518_TT2_SS06</t>
+  </si>
+  <si>
+    <t>b2289_d180518_TT2_SS07</t>
+  </si>
+  <si>
+    <t>b2289_d180518_TT2_SS08</t>
+  </si>
+  <si>
+    <t>merge with unit 7 and call it MU?</t>
+  </si>
+  <si>
+    <t>merge with unit 5 and call it MU?</t>
+  </si>
+  <si>
+    <t>b2289_d180518_TT2_SS09</t>
+  </si>
+  <si>
+    <t>b2289_d180520_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b2289_d180520_TT1_SS02</t>
+  </si>
+  <si>
+    <t>b2289_d180520_TT1_SS03</t>
+  </si>
+  <si>
+    <t>b2289_d180520_TT3_SS01</t>
+  </si>
+  <si>
+    <t>b2289_d180520_TT3_SS02</t>
+  </si>
+  <si>
+    <t>b2289_d180520_TT3_SS03</t>
+  </si>
+  <si>
+    <t>b2289_d180520_TT3_SS04</t>
+  </si>
+  <si>
+    <t>seperating units 3/4 using slices 3488,3200,3296</t>
+  </si>
+  <si>
+    <t>mono-synaptic to unit 2?</t>
+  </si>
+  <si>
+    <t>big cluster so I'm not sure if it is isolated (I used slices 3296,3136,3456) )</t>
+  </si>
+  <si>
+    <t>b2289_d180520_TT3_SS05</t>
+  </si>
+  <si>
+    <t>b2289_d180520_TT3_SS06</t>
+  </si>
+  <si>
+    <t>too close to unit 5</t>
+  </si>
+  <si>
+    <t>b2289_d180520_TT3_SS07</t>
+  </si>
+  <si>
+    <t>b2289_d180520_TT3_SS08</t>
+  </si>
+  <si>
+    <t>b2289_d180520_TT3_SS09</t>
+  </si>
+  <si>
+    <t>I merged here two clusters that merge in time</t>
+  </si>
+  <si>
+    <t>b2289_d180523_TT3_SS01</t>
+  </si>
+  <si>
+    <t>b2289_d180524_TT3_SS01</t>
+  </si>
+  <si>
+    <t>b2289_d180525_TT3_SS01</t>
+  </si>
+  <si>
+    <t>b2289_d180525_TT3_SS02</t>
+  </si>
+  <si>
+    <t>b2289_d180525_TT2_SS01</t>
+  </si>
+  <si>
+    <t>b2289_d180525_TT2_SS02</t>
+  </si>
+  <si>
+    <t>b2289_d180528_TT2_SS01</t>
+  </si>
+  <si>
+    <t>b2289_d180528_TT2_SS02</t>
+  </si>
+  <si>
+    <t>not sure if isolated enough+partially stable</t>
+  </si>
+  <si>
+    <t>b2289_d180528_TT3_SS01</t>
+  </si>
+  <si>
+    <t>b2289_d180528_TT3_SS02</t>
+  </si>
+  <si>
+    <t>multi-unit close to the noise+partially stable</t>
+  </si>
+  <si>
+    <t>b2289_d180529_TT2_SS01</t>
+  </si>
+  <si>
+    <t>b2289_d180531_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b2289_d180531_TT1_SS02</t>
+  </si>
+  <si>
+    <t>b2289_d180531_TT2_SS01</t>
+  </si>
+  <si>
+    <t>b2289_d180615_TT4_SS01</t>
   </si>
 </sst>
 </file>
@@ -1508,12 +1694,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:S308"/>
+  <dimension ref="A1:S359"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A269" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E310" sqref="E310"/>
+      <pane ySplit="1" topLeftCell="A333" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A360" sqref="A360"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1524,7 +1709,7 @@
     <col min="4" max="4" width="4.75" style="1" customWidth="1"/>
     <col min="5" max="5" width="4" style="1" customWidth="1"/>
     <col min="6" max="6" width="7.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="50.75" style="1" customWidth="1"/>
+    <col min="7" max="7" width="62.875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.625" style="1" customWidth="1"/>
     <col min="9" max="9" width="7.875" style="1" customWidth="1"/>
     <col min="10" max="10" width="30.5" style="1" customWidth="1"/>
@@ -1577,7 +1762,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>91</v>
       </c>
@@ -1603,7 +1788,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>93</v>
       </c>
@@ -1629,7 +1814,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>92</v>
       </c>
@@ -1655,7 +1840,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>94</v>
       </c>
@@ -1681,7 +1866,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>95</v>
       </c>
@@ -1704,7 +1889,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>90</v>
       </c>
@@ -1727,7 +1912,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>96</v>
       </c>
@@ -1750,7 +1935,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>97</v>
       </c>
@@ -1773,7 +1958,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>98</v>
       </c>
@@ -1796,7 +1981,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>99</v>
       </c>
@@ -1819,7 +2004,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>100</v>
       </c>
@@ -1842,7 +2027,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>102</v>
       </c>
@@ -1865,7 +2050,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>103</v>
       </c>
@@ -1888,7 +2073,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>107</v>
       </c>
@@ -1911,7 +2096,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>108</v>
       </c>
@@ -1934,7 +2119,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>109</v>
       </c>
@@ -1960,7 +2145,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>110</v>
       </c>
@@ -1983,7 +2168,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>111</v>
       </c>
@@ -2009,7 +2194,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>101</v>
       </c>
@@ -2032,7 +2217,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>112</v>
       </c>
@@ -2058,7 +2243,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
@@ -2081,7 +2266,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
@@ -2107,7 +2292,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
@@ -2130,7 +2315,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>113</v>
       </c>
@@ -2156,7 +2341,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>115</v>
       </c>
@@ -2179,7 +2364,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>116</v>
       </c>
@@ -2202,7 +2387,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>72</v>
       </c>
@@ -2231,7 +2416,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>6</v>
       </c>
@@ -2254,7 +2439,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
@@ -2277,7 +2462,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
@@ -2300,7 +2485,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>120</v>
       </c>
@@ -2323,7 +2508,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>9</v>
       </c>
@@ -2346,7 +2531,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>10</v>
       </c>
@@ -2369,7 +2554,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>11</v>
       </c>
@@ -2389,7 +2574,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>12</v>
       </c>
@@ -2409,7 +2594,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>13</v>
       </c>
@@ -2429,7 +2614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>124</v>
       </c>
@@ -2452,7 +2637,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>14</v>
       </c>
@@ -2478,7 +2663,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>68</v>
       </c>
@@ -2501,7 +2686,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>15</v>
       </c>
@@ -2525,7 +2710,7 @@
       </c>
       <c r="H41" s="4"/>
     </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>16</v>
       </c>
@@ -2548,7 +2733,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>17</v>
       </c>
@@ -2571,7 +2756,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>18</v>
       </c>
@@ -2594,7 +2779,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>69</v>
       </c>
@@ -2617,7 +2802,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>19</v>
       </c>
@@ -2637,7 +2822,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>20</v>
       </c>
@@ -2657,7 +2842,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>21</v>
       </c>
@@ -2677,7 +2862,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>126</v>
       </c>
@@ -2700,7 +2885,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>127</v>
       </c>
@@ -2723,7 +2908,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>22</v>
       </c>
@@ -2746,7 +2931,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>23</v>
       </c>
@@ -2766,7 +2951,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>24</v>
       </c>
@@ -2786,7 +2971,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>25</v>
       </c>
@@ -2809,7 +2994,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>26</v>
       </c>
@@ -2829,7 +3014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>27</v>
       </c>
@@ -2852,7 +3037,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>28</v>
       </c>
@@ -2875,7 +3060,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>29</v>
       </c>
@@ -2895,7 +3080,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>30</v>
       </c>
@@ -2915,7 +3100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>70</v>
       </c>
@@ -2938,7 +3123,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>71</v>
       </c>
@@ -2961,7 +3146,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>31</v>
       </c>
@@ -2981,7 +3166,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>32</v>
       </c>
@@ -3001,7 +3186,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>33</v>
       </c>
@@ -3024,7 +3209,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>34</v>
       </c>
@@ -3047,7 +3232,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>35</v>
       </c>
@@ -3073,7 +3258,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>36</v>
       </c>
@@ -3093,7 +3278,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>37</v>
       </c>
@@ -3116,7 +3301,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>38</v>
       </c>
@@ -3139,7 +3324,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>39</v>
       </c>
@@ -3162,7 +3347,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>40</v>
       </c>
@@ -3188,7 +3373,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>136</v>
       </c>
@@ -3208,7 +3393,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>41</v>
       </c>
@@ -3228,7 +3413,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>42</v>
       </c>
@@ -3248,7 +3433,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>43</v>
       </c>
@@ -3268,7 +3453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>44</v>
       </c>
@@ -3291,7 +3476,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>73</v>
       </c>
@@ -3314,7 +3499,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>74</v>
       </c>
@@ -3337,7 +3522,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>75</v>
       </c>
@@ -3360,7 +3545,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>76</v>
       </c>
@@ -3383,7 +3568,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>45</v>
       </c>
@@ -3406,7 +3591,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>46</v>
       </c>
@@ -3426,7 +3611,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>77</v>
       </c>
@@ -3449,7 +3634,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>78</v>
       </c>
@@ -3469,7 +3654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>47</v>
       </c>
@@ -3492,7 +3677,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>80</v>
       </c>
@@ -3515,7 +3700,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>48</v>
       </c>
@@ -3538,7 +3723,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>81</v>
       </c>
@@ -3561,7 +3746,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>49</v>
       </c>
@@ -3584,7 +3769,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>50</v>
       </c>
@@ -3607,7 +3792,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>51</v>
       </c>
@@ -3630,7 +3815,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>143</v>
       </c>
@@ -3653,7 +3838,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>52</v>
       </c>
@@ -3676,7 +3861,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>53</v>
       </c>
@@ -3696,7 +3881,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>82</v>
       </c>
@@ -3719,7 +3904,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>83</v>
       </c>
@@ -3742,7 +3927,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>54</v>
       </c>
@@ -3762,7 +3947,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>55</v>
       </c>
@@ -8412,7 +8597,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="305" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A305" s="1" t="s">
         <v>377</v>
       </c>
@@ -8432,7 +8617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="306" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A306" s="1" t="s">
         <v>378</v>
       </c>
@@ -8455,7 +8640,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="307" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A307" s="1" t="s">
         <v>379</v>
       </c>
@@ -8478,7 +8663,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="308" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A308" s="1" t="s">
         <v>380</v>
       </c>
@@ -8501,14 +8686,1181 @@
         <v>154</v>
       </c>
     </row>
+    <row r="309" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A309" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B309" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C309" s="2">
+        <v>43234</v>
+      </c>
+      <c r="D309" s="1">
+        <v>1</v>
+      </c>
+      <c r="E309" s="1">
+        <v>1</v>
+      </c>
+      <c r="F309" s="1">
+        <v>2</v>
+      </c>
+      <c r="K309" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="310" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A310" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B310" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C310" s="2">
+        <v>43234</v>
+      </c>
+      <c r="D310" s="1">
+        <v>1</v>
+      </c>
+      <c r="E310" s="1">
+        <v>2</v>
+      </c>
+      <c r="F310" s="1">
+        <v>0</v>
+      </c>
+      <c r="G310" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="311" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A311" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B311" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C311" s="2">
+        <v>43234</v>
+      </c>
+      <c r="D311" s="1">
+        <v>1</v>
+      </c>
+      <c r="E311" s="1">
+        <v>3</v>
+      </c>
+      <c r="F311" s="1">
+        <v>0</v>
+      </c>
+      <c r="G311" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="312" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A312" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="B312" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C312" s="2">
+        <v>43234</v>
+      </c>
+      <c r="D312" s="1">
+        <v>1</v>
+      </c>
+      <c r="E312" s="1">
+        <v>4</v>
+      </c>
+      <c r="F312" s="1">
+        <v>0</v>
+      </c>
+      <c r="G312" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="313" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A313" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B313" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C313" s="2">
+        <v>43235</v>
+      </c>
+      <c r="D313" s="1">
+        <v>1</v>
+      </c>
+      <c r="E313" s="1">
+        <v>1</v>
+      </c>
+      <c r="F313" s="1">
+        <v>2</v>
+      </c>
+      <c r="J313" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="K313" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="314" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A314" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="B314" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C314" s="2">
+        <v>43235</v>
+      </c>
+      <c r="D314" s="1">
+        <v>1</v>
+      </c>
+      <c r="E314" s="1">
+        <v>2</v>
+      </c>
+      <c r="F314" s="1">
+        <v>2</v>
+      </c>
+      <c r="K314" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="315" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A315" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B315" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C315" s="2">
+        <v>43235</v>
+      </c>
+      <c r="D315" s="1">
+        <v>1</v>
+      </c>
+      <c r="E315" s="1">
+        <v>3</v>
+      </c>
+      <c r="F315" s="1">
+        <v>2</v>
+      </c>
+      <c r="K315" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="316" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A316" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="B316" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C316" s="2">
+        <v>43235</v>
+      </c>
+      <c r="D316" s="1">
+        <v>1</v>
+      </c>
+      <c r="E316" s="1">
+        <v>4</v>
+      </c>
+      <c r="F316" s="1">
+        <v>0</v>
+      </c>
+      <c r="G316" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="K316" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="317" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A317" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B317" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C317" s="2">
+        <v>43238</v>
+      </c>
+      <c r="D317" s="1">
+        <v>1</v>
+      </c>
+      <c r="E317" s="1">
+        <v>1</v>
+      </c>
+      <c r="F317" s="1">
+        <v>2</v>
+      </c>
+      <c r="K317" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="318" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A318" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B318" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C318" s="2">
+        <v>43238</v>
+      </c>
+      <c r="D318" s="1">
+        <v>1</v>
+      </c>
+      <c r="E318" s="1">
+        <v>2</v>
+      </c>
+      <c r="F318" s="1">
+        <v>0</v>
+      </c>
+      <c r="G318" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="K318" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="319" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A319" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="B319" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C319" s="2">
+        <v>43238</v>
+      </c>
+      <c r="D319" s="1">
+        <v>1</v>
+      </c>
+      <c r="E319" s="1">
+        <v>3</v>
+      </c>
+      <c r="F319" s="1">
+        <v>2</v>
+      </c>
+      <c r="G319" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="K319" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="320" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A320" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B320" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C320" s="2">
+        <v>43238</v>
+      </c>
+      <c r="D320" s="1">
+        <v>1</v>
+      </c>
+      <c r="E320" s="1">
+        <v>4</v>
+      </c>
+      <c r="F320" s="1">
+        <v>2</v>
+      </c>
+      <c r="K320" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="321" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A321" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B321" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C321" s="2">
+        <v>43238</v>
+      </c>
+      <c r="D321" s="1">
+        <v>1</v>
+      </c>
+      <c r="E321" s="1">
+        <v>5</v>
+      </c>
+      <c r="F321" s="1">
+        <v>2</v>
+      </c>
+      <c r="K321" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="322" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A322" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B322" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C322" s="2">
+        <v>43238</v>
+      </c>
+      <c r="D322" s="1">
+        <v>1</v>
+      </c>
+      <c r="E322" s="1">
+        <v>6</v>
+      </c>
+      <c r="F322" s="1">
+        <v>2</v>
+      </c>
+      <c r="K322" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="323" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A323" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B323" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C323" s="2">
+        <v>43238</v>
+      </c>
+      <c r="D323" s="1">
+        <v>1</v>
+      </c>
+      <c r="E323" s="1">
+        <v>7</v>
+      </c>
+      <c r="F323" s="1">
+        <v>2</v>
+      </c>
+      <c r="K323" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="324" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A324" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B324" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C324" s="2">
+        <v>43238</v>
+      </c>
+      <c r="D324" s="1">
+        <v>2</v>
+      </c>
+      <c r="E324" s="1">
+        <v>1</v>
+      </c>
+      <c r="F324" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="325" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A325" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B325" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C325" s="2">
+        <v>43238</v>
+      </c>
+      <c r="D325" s="1">
+        <v>2</v>
+      </c>
+      <c r="E325" s="1">
+        <v>2</v>
+      </c>
+      <c r="F325" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="326" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A326" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B326" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C326" s="2">
+        <v>43238</v>
+      </c>
+      <c r="D326" s="1">
+        <v>2</v>
+      </c>
+      <c r="E326" s="1">
+        <v>3</v>
+      </c>
+      <c r="F326" s="1">
+        <v>2</v>
+      </c>
+      <c r="G326" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="327" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A327" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B327" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C327" s="2">
+        <v>43238</v>
+      </c>
+      <c r="D327" s="1">
+        <v>2</v>
+      </c>
+      <c r="E327" s="1">
+        <v>4</v>
+      </c>
+      <c r="F327" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="328" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A328" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B328" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C328" s="2">
+        <v>43238</v>
+      </c>
+      <c r="D328" s="1">
+        <v>2</v>
+      </c>
+      <c r="E328" s="1">
+        <v>5</v>
+      </c>
+      <c r="F328" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G328" s="1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="329" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A329" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B329" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C329" s="2">
+        <v>43238</v>
+      </c>
+      <c r="D329" s="1">
+        <v>2</v>
+      </c>
+      <c r="E329" s="1">
+        <v>6</v>
+      </c>
+      <c r="F329" s="1">
+        <v>2</v>
+      </c>
+      <c r="G329" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="330" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A330" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="B330" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C330" s="2">
+        <v>43238</v>
+      </c>
+      <c r="D330" s="1">
+        <v>2</v>
+      </c>
+      <c r="E330" s="1">
+        <v>7</v>
+      </c>
+      <c r="F330" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G330" s="1" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="331" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A331" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B331" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C331" s="2">
+        <v>43238</v>
+      </c>
+      <c r="D331" s="1">
+        <v>2</v>
+      </c>
+      <c r="E331" s="1">
+        <v>8</v>
+      </c>
+      <c r="F331" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="332" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A332" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B332" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C332" s="2">
+        <v>43238</v>
+      </c>
+      <c r="D332" s="1">
+        <v>2</v>
+      </c>
+      <c r="E332" s="1">
+        <v>9</v>
+      </c>
+      <c r="F332" s="1">
+        <v>1</v>
+      </c>
+      <c r="G332" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="333" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A333" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B333" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C333" s="2">
+        <v>43240</v>
+      </c>
+      <c r="D333" s="1">
+        <v>1</v>
+      </c>
+      <c r="E333" s="1">
+        <v>1</v>
+      </c>
+      <c r="F333" s="1">
+        <v>1</v>
+      </c>
+      <c r="G333" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="334" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A334" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B334" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C334" s="2">
+        <v>43240</v>
+      </c>
+      <c r="D334" s="1">
+        <v>1</v>
+      </c>
+      <c r="E334" s="1">
+        <v>2</v>
+      </c>
+      <c r="F334" s="1">
+        <v>1</v>
+      </c>
+      <c r="G334" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="335" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A335" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B335" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C335" s="2">
+        <v>43240</v>
+      </c>
+      <c r="D335" s="1">
+        <v>1</v>
+      </c>
+      <c r="E335" s="1">
+        <v>3</v>
+      </c>
+      <c r="F335" s="1">
+        <v>1</v>
+      </c>
+      <c r="G335" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="336" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A336" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B336" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C336" s="2">
+        <v>43240</v>
+      </c>
+      <c r="D336" s="1">
+        <v>3</v>
+      </c>
+      <c r="E336" s="1">
+        <v>1</v>
+      </c>
+      <c r="F336" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="337" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A337" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B337" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C337" s="2">
+        <v>43240</v>
+      </c>
+      <c r="D337" s="1">
+        <v>3</v>
+      </c>
+      <c r="E337" s="1">
+        <v>2</v>
+      </c>
+      <c r="F337" s="1">
+        <v>2</v>
+      </c>
+      <c r="G337" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="K337" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="338" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A338" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B338" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C338" s="2">
+        <v>43240</v>
+      </c>
+      <c r="D338" s="1">
+        <v>3</v>
+      </c>
+      <c r="E338" s="1">
+        <v>3</v>
+      </c>
+      <c r="F338" s="1">
+        <v>2</v>
+      </c>
+      <c r="G338" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="K338" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="339" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A339" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B339" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C339" s="2">
+        <v>43240</v>
+      </c>
+      <c r="D339" s="1">
+        <v>3</v>
+      </c>
+      <c r="E339" s="1">
+        <v>4</v>
+      </c>
+      <c r="F339" s="1">
+        <v>2</v>
+      </c>
+      <c r="G339" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="340" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A340" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B340" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C340" s="2">
+        <v>43240</v>
+      </c>
+      <c r="D340" s="1">
+        <v>3</v>
+      </c>
+      <c r="E340" s="1">
+        <v>5</v>
+      </c>
+      <c r="F340" s="1">
+        <v>1</v>
+      </c>
+      <c r="G340" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="341" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A341" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B341" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C341" s="2">
+        <v>43240</v>
+      </c>
+      <c r="D341" s="1">
+        <v>3</v>
+      </c>
+      <c r="E341" s="1">
+        <v>6</v>
+      </c>
+      <c r="F341" s="1">
+        <v>1</v>
+      </c>
+      <c r="G341" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="342" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A342" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B342" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C342" s="2">
+        <v>43240</v>
+      </c>
+      <c r="D342" s="1">
+        <v>3</v>
+      </c>
+      <c r="E342" s="1">
+        <v>7</v>
+      </c>
+      <c r="F342" s="1">
+        <v>1</v>
+      </c>
+      <c r="G342" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="343" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A343" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="B343" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C343" s="2">
+        <v>43240</v>
+      </c>
+      <c r="D343" s="1">
+        <v>3</v>
+      </c>
+      <c r="E343" s="1">
+        <v>8</v>
+      </c>
+      <c r="F343" s="1">
+        <v>1</v>
+      </c>
+      <c r="G343" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="344" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A344" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B344" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C344" s="2">
+        <v>43240</v>
+      </c>
+      <c r="D344" s="1">
+        <v>3</v>
+      </c>
+      <c r="E344" s="1">
+        <v>9</v>
+      </c>
+      <c r="F344" s="1">
+        <v>1</v>
+      </c>
+      <c r="G344" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="345" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A345" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B345" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C345" s="2">
+        <v>43243</v>
+      </c>
+      <c r="D345" s="1">
+        <v>3</v>
+      </c>
+      <c r="E345" s="1">
+        <v>1</v>
+      </c>
+      <c r="F345" s="1">
+        <v>1</v>
+      </c>
+      <c r="G345" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="346" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A346" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B346" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C346" s="2">
+        <v>43244</v>
+      </c>
+      <c r="D346" s="1">
+        <v>3</v>
+      </c>
+      <c r="E346" s="1">
+        <v>1</v>
+      </c>
+      <c r="F346" s="1">
+        <v>1</v>
+      </c>
+      <c r="G346" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="347" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A347" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="B347" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C347" s="2">
+        <v>43245</v>
+      </c>
+      <c r="D347" s="1">
+        <v>2</v>
+      </c>
+      <c r="E347" s="1">
+        <v>1</v>
+      </c>
+      <c r="F347" s="1">
+        <v>1</v>
+      </c>
+      <c r="G347" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="348" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A348" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B348" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C348" s="2">
+        <v>43245</v>
+      </c>
+      <c r="D348" s="1">
+        <v>2</v>
+      </c>
+      <c r="E348" s="1">
+        <v>2</v>
+      </c>
+      <c r="F348" s="1">
+        <v>1</v>
+      </c>
+      <c r="G348" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="349" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A349" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="B349" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C349" s="2">
+        <v>43245</v>
+      </c>
+      <c r="D349" s="1">
+        <v>3</v>
+      </c>
+      <c r="E349" s="1">
+        <v>1</v>
+      </c>
+      <c r="F349" s="1">
+        <v>1</v>
+      </c>
+      <c r="G349" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="350" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A350" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="B350" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C350" s="2">
+        <v>43245</v>
+      </c>
+      <c r="D350" s="1">
+        <v>3</v>
+      </c>
+      <c r="E350" s="1">
+        <v>2</v>
+      </c>
+      <c r="F350" s="1">
+        <v>1</v>
+      </c>
+      <c r="G350" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="351" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A351" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B351" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C351" s="2">
+        <v>43248</v>
+      </c>
+      <c r="D351" s="1">
+        <v>2</v>
+      </c>
+      <c r="E351" s="1">
+        <v>1</v>
+      </c>
+      <c r="F351" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G351" s="3" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="352" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A352" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B352" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C352" s="2">
+        <v>43248</v>
+      </c>
+      <c r="D352" s="1">
+        <v>2</v>
+      </c>
+      <c r="E352" s="1">
+        <v>2</v>
+      </c>
+      <c r="F352" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G352" s="3" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="353" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A353" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B353" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C353" s="2">
+        <v>43248</v>
+      </c>
+      <c r="D353" s="1">
+        <v>3</v>
+      </c>
+      <c r="E353" s="1">
+        <v>1</v>
+      </c>
+      <c r="F353" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G353" s="3" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="354" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A354" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B354" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C354" s="2">
+        <v>43248</v>
+      </c>
+      <c r="D354" s="1">
+        <v>3</v>
+      </c>
+      <c r="E354" s="1">
+        <v>2</v>
+      </c>
+      <c r="F354" s="1">
+        <v>1</v>
+      </c>
+      <c r="G354" s="3" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="355" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A355" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="B355" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C355" s="2">
+        <v>43249</v>
+      </c>
+      <c r="D355" s="1">
+        <v>2</v>
+      </c>
+      <c r="E355" s="1">
+        <v>1</v>
+      </c>
+      <c r="F355" s="1">
+        <v>1</v>
+      </c>
+      <c r="G355" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="356" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A356" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="B356" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C356" s="2">
+        <v>43251</v>
+      </c>
+      <c r="D356" s="1">
+        <v>1</v>
+      </c>
+      <c r="E356" s="1">
+        <v>1</v>
+      </c>
+      <c r="F356" s="1">
+        <v>1</v>
+      </c>
+      <c r="G356" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="357" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A357" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="B357" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C357" s="2">
+        <v>43251</v>
+      </c>
+      <c r="D357" s="1">
+        <v>1</v>
+      </c>
+      <c r="E357" s="1">
+        <v>2</v>
+      </c>
+      <c r="F357" s="1">
+        <v>1</v>
+      </c>
+      <c r="G357" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="358" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A358" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="B358" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C358" s="2">
+        <v>43251</v>
+      </c>
+      <c r="D358" s="1">
+        <v>2</v>
+      </c>
+      <c r="E358" s="1">
+        <v>1</v>
+      </c>
+      <c r="F358" s="1">
+        <v>1</v>
+      </c>
+      <c r="G358" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="359" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A359" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B359" s="1">
+        <v>2289</v>
+      </c>
+      <c r="C359" s="2">
+        <v>43266</v>
+      </c>
+      <c r="D359" s="1">
+        <v>4</v>
+      </c>
+      <c r="E359" s="1">
+        <v>1</v>
+      </c>
+      <c r="F359" s="1">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:H260">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="9861"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B1:H308"/>
   <conditionalFormatting sqref="F3">
     <cfRule type="colorScale" priority="28">
       <colorScale>

</xml_diff>

<commit_message>
join sorting summaries from shir
</commit_message>
<xml_diff>
--- a/inclusion_lists/cells_summary.xlsx
+++ b/inclusion_lists/cells_summary.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="895">
   <si>
     <t>bat</t>
   </si>
@@ -2147,6 +2147,573 @@
   </si>
   <si>
     <t>[75791192381 81075256803]</t>
+  </si>
+  <si>
+    <t>b0148_d170606_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170606_TT1_SS02</t>
+  </si>
+  <si>
+    <t>[66263161024 67223496690]</t>
+  </si>
+  <si>
+    <t>b0148_d170606_TT1_SS03</t>
+  </si>
+  <si>
+    <t>b0148_d170606_TT4_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170606_TT4_SS02</t>
+  </si>
+  <si>
+    <t>b0148_d170606_TT4_SS03</t>
+  </si>
+  <si>
+    <t>b0148_d170606_TT4_SS04</t>
+  </si>
+  <si>
+    <t>b0148_d170606_TT4_SS05</t>
+  </si>
+  <si>
+    <t>b0148_d170606_TT4_SS06</t>
+  </si>
+  <si>
+    <t>b0148_d170606_TT4_SS07</t>
+  </si>
+  <si>
+    <t>b0148_d170606_TT4_SS08</t>
+  </si>
+  <si>
+    <t>b0148_d170606_TT4_SS09</t>
+  </si>
+  <si>
+    <t>b0148_d170606_TT4_SS10</t>
+  </si>
+  <si>
+    <t>b0148_d170606_TT4_SS11</t>
+  </si>
+  <si>
+    <t>b0148_d170606_TT4_SS12</t>
+  </si>
+  <si>
+    <t>b0148_d170606_TT4_SS13</t>
+  </si>
+  <si>
+    <t>b0148_d170606_TT4_SS14</t>
+  </si>
+  <si>
+    <t>b0148_d170607_TT4_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170607_TT4_SS02</t>
+  </si>
+  <si>
+    <t>b0148_d170607_TT4_SS03</t>
+  </si>
+  <si>
+    <t>b0148_d170607_TT4_SS04</t>
+  </si>
+  <si>
+    <t>b0148_d170607_TT4_SS05</t>
+  </si>
+  <si>
+    <t>united based on functionality</t>
+  </si>
+  <si>
+    <t>b0148_d170607_TT4_SS06</t>
+  </si>
+  <si>
+    <t>maybe too close to the noise towards the end of the session</t>
+  </si>
+  <si>
+    <t>b0148_d170607_TT4_SS07</t>
+  </si>
+  <si>
+    <t>b0148_d170607_TT4_SS08</t>
+  </si>
+  <si>
+    <t>[65196544964 66958613745]</t>
+  </si>
+  <si>
+    <t>b0148_d170607_TT4_SS09</t>
+  </si>
+  <si>
+    <t>b0148_d170607_TT4_SS10</t>
+  </si>
+  <si>
+    <t>[66253786233 70482751312]</t>
+  </si>
+  <si>
+    <t>b0148_d170607_TT4_SS11</t>
+  </si>
+  <si>
+    <t>[68015855016 69777923798]</t>
+  </si>
+  <si>
+    <t>b0148_d170607_TT4_SS12</t>
+  </si>
+  <si>
+    <t>b0148_d170607_TT4_SS13</t>
+  </si>
+  <si>
+    <t>maybe mixed with other unitswards the end</t>
+  </si>
+  <si>
+    <t>[65548958720 70482751312]</t>
+  </si>
+  <si>
+    <t>b0148_d170607_TT4_SS14</t>
+  </si>
+  <si>
+    <t>close to noise</t>
+  </si>
+  <si>
+    <t>[67663441260 69777923798]</t>
+  </si>
+  <si>
+    <t>b0148_d170607_TT4_SS15</t>
+  </si>
+  <si>
+    <t>b0148_d170607_TT4_SS16</t>
+  </si>
+  <si>
+    <t>b0148_d170607_TT4_SS17</t>
+  </si>
+  <si>
+    <t>b0148_d170607_TT4_SS18</t>
+  </si>
+  <si>
+    <t>b0148_d170607_TT4_SS19</t>
+  </si>
+  <si>
+    <t>b0148_d170607_TT4_SS20</t>
+  </si>
+  <si>
+    <t>b0148_d170608_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170608_TT4_SS01</t>
+  </si>
+  <si>
+    <t>mixed with SS02 and SS07?</t>
+  </si>
+  <si>
+    <t>b0148_d170608_TT4_SS02</t>
+  </si>
+  <si>
+    <t>mixed with noise</t>
+  </si>
+  <si>
+    <t>b0148_d170608_TT4_SS03</t>
+  </si>
+  <si>
+    <t>b0148_d170608_TT4_SS04</t>
+  </si>
+  <si>
+    <t>[67291740683 68770680038]</t>
+  </si>
+  <si>
+    <t>b0148_d170608_TT4_SS05</t>
+  </si>
+  <si>
+    <t>[68031210361 73946967784]</t>
+  </si>
+  <si>
+    <t>b0148_d170608_TT4_SS06</t>
+  </si>
+  <si>
+    <t>b0148_d170608_TT4_SS07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">close to noise </t>
+  </si>
+  <si>
+    <t>b0148_d170608_TT4_SS08</t>
+  </si>
+  <si>
+    <t>not stable and close to noise</t>
+  </si>
+  <si>
+    <t>b0148_d170611_TT4_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170612_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170612_TT1_SS02</t>
+  </si>
+  <si>
+    <t>b0148_d170612_TT1_SS03</t>
+  </si>
+  <si>
+    <t>b0148_d170612_TT1_SS04</t>
+  </si>
+  <si>
+    <t>b0148_d170612_TT1_SS05</t>
+  </si>
+  <si>
+    <t>b0148_d170613_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170613_TT1_SS02</t>
+  </si>
+  <si>
+    <t>b0148_d170613_TT1_SS03</t>
+  </si>
+  <si>
+    <t>b0148_d170613_TT1_SS04</t>
+  </si>
+  <si>
+    <t>b0148_d170613_TT1_SS05</t>
+  </si>
+  <si>
+    <t>b0148_d170614_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170614_TT1_SS02</t>
+  </si>
+  <si>
+    <t>b0148_d170614_TT1_SS03</t>
+  </si>
+  <si>
+    <t>b0148_d170614_TT4_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170614_TT4_SS02</t>
+  </si>
+  <si>
+    <t>b0148_d170614_TT4_SS03</t>
+  </si>
+  <si>
+    <t>b0148_d170614_TT4_SS04</t>
+  </si>
+  <si>
+    <t>b0148_d170615_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170615_TT1_SS02</t>
+  </si>
+  <si>
+    <t>too close to noise</t>
+  </si>
+  <si>
+    <t>b0148_d170615_TT1_SS03</t>
+  </si>
+  <si>
+    <t>mixed with ss04</t>
+  </si>
+  <si>
+    <t>b0148_d170615_TT1_SS04</t>
+  </si>
+  <si>
+    <t>mixed with ss03</t>
+  </si>
+  <si>
+    <t>b0148_d170615_TT1_SS05</t>
+  </si>
+  <si>
+    <t>b0148_d170615_TT4_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170618_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170618_TT1_SS02</t>
+  </si>
+  <si>
+    <t>b0148_d170618_TT1_SS03</t>
+  </si>
+  <si>
+    <t>b0148_d170618_TT1_SS04</t>
+  </si>
+  <si>
+    <t>b0148_d170618_TT4_SS01</t>
+  </si>
+  <si>
+    <t>[67371241582 70702786495]</t>
+  </si>
+  <si>
+    <t>b0148_d170618_TT4_SS02</t>
+  </si>
+  <si>
+    <t>b0148_d170619_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170619_TT1_SS02</t>
+  </si>
+  <si>
+    <t>b0148_d170619_TT1_SS03</t>
+  </si>
+  <si>
+    <t>b0148_d170619_TT1_SS04</t>
+  </si>
+  <si>
+    <t>b0148_d170619_TT4_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170619_TT4_SS02</t>
+  </si>
+  <si>
+    <t>b0148_d170619_TT4_SS03</t>
+  </si>
+  <si>
+    <t>b0148_d170619_TT4_SS04</t>
+  </si>
+  <si>
+    <t>b0148_d170620_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170620_TT1_SS02</t>
+  </si>
+  <si>
+    <t>b0148_d170620_TT4_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170620_TT4_SS02</t>
+  </si>
+  <si>
+    <t>b0148_d170620_TT4_SS03</t>
+  </si>
+  <si>
+    <t>b0148_d170620_TT4_SS04</t>
+  </si>
+  <si>
+    <t>b0148_d170620_TT4_SS05</t>
+  </si>
+  <si>
+    <t>b0148_d170621_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170621_TT1_SS02</t>
+  </si>
+  <si>
+    <t>b0148_d170621_TT1_SS03</t>
+  </si>
+  <si>
+    <t>mixed with ss02</t>
+  </si>
+  <si>
+    <t>b0148_d170621_TT1_SS04</t>
+  </si>
+  <si>
+    <t>b0148_d170621_TT4_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170621_TT4_SS02</t>
+  </si>
+  <si>
+    <t>b0148_d170621_TT4_SS03</t>
+  </si>
+  <si>
+    <t>b0148_d170622_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170622_TT1_SS02</t>
+  </si>
+  <si>
+    <t>b0148_d170622_TT4_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170622_TT4_SS02</t>
+  </si>
+  <si>
+    <t>b0148_d170622_TT4_SS03</t>
+  </si>
+  <si>
+    <t>b0148_d170622_TT4_SS04</t>
+  </si>
+  <si>
+    <t>[70431810007 72679633729]</t>
+  </si>
+  <si>
+    <t>b0148_d170622_TT4_SS05</t>
+  </si>
+  <si>
+    <t>b0148_d170625_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170625_TT1_SS02</t>
+  </si>
+  <si>
+    <t>b0148_d170625_TT4_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170625_TT4_SS02</t>
+  </si>
+  <si>
+    <t>b0148_d170625_TT4_SS03</t>
+  </si>
+  <si>
+    <t>b0148_d170625_TT4_SS04</t>
+  </si>
+  <si>
+    <t>mixed with ss05 - check functionality</t>
+  </si>
+  <si>
+    <t>b0148_d170625_TT4_SS05</t>
+  </si>
+  <si>
+    <t>mixed with ss04 - check functionality</t>
+  </si>
+  <si>
+    <t>b0148_d170625_TT4_SS06</t>
+  </si>
+  <si>
+    <t>b0148_d170625_TT4_SS07</t>
+  </si>
+  <si>
+    <t>b0148_d170625_TT4_SS08</t>
+  </si>
+  <si>
+    <t>b0148_d170625_TT4_SS09</t>
+  </si>
+  <si>
+    <t>b0148_d170625_TT4_SS10</t>
+  </si>
+  <si>
+    <t>b0148_d170625_TT4_SS11</t>
+  </si>
+  <si>
+    <t>b0148_d170625_TT4_SS12</t>
+  </si>
+  <si>
+    <t>b0148_d170626_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170626_TT1_SS02</t>
+  </si>
+  <si>
+    <t>b0148_d170626_TT1_SS03</t>
+  </si>
+  <si>
+    <t>b0148_d170626_TT1_SS04</t>
+  </si>
+  <si>
+    <t>b0148_d170626_TT4_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170626_TT4_SS02</t>
+  </si>
+  <si>
+    <t>b0148_d170627_TT1_SS01</t>
+  </si>
+  <si>
+    <t>could be two cells</t>
+  </si>
+  <si>
+    <t>b0148_d170627_TT1_SS02</t>
+  </si>
+  <si>
+    <t>b0148_d170627_TT1_SS03</t>
+  </si>
+  <si>
+    <t>b0148_d170627_TT1_SS04</t>
+  </si>
+  <si>
+    <t>multi-unit - interesting functional with ss05</t>
+  </si>
+  <si>
+    <t>b0148_d170627_TT1_SS05</t>
+  </si>
+  <si>
+    <t>b0148_d170627_TT1_SS06</t>
+  </si>
+  <si>
+    <t>b0148_d170627_TT4_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170627_TT4_SS02</t>
+  </si>
+  <si>
+    <t>b0148_d170627_TT4_SS03</t>
+  </si>
+  <si>
+    <t>b0148_d170627_TT4_SS04</t>
+  </si>
+  <si>
+    <t>b0148_d170627_TT4_SS05</t>
+  </si>
+  <si>
+    <t>b0148_d170627_TT4_SS06</t>
+  </si>
+  <si>
+    <t>b0148_d170627_TT4_SS07</t>
+  </si>
+  <si>
+    <t>b0148_d170628_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170628_TT1_SS02</t>
+  </si>
+  <si>
+    <t>b0148_d170628_TT1_SS03</t>
+  </si>
+  <si>
+    <t>b0148_d170628_TT1_SS04</t>
+  </si>
+  <si>
+    <t>b0148_d170628_TT1_SS05</t>
+  </si>
+  <si>
+    <t>b0148_d170628_TT1_SS06</t>
+  </si>
+  <si>
+    <t>b0148_d170628_TT1_SS07</t>
+  </si>
+  <si>
+    <t>b0148_d170628_TT1_SS08</t>
+  </si>
+  <si>
+    <t>b0148_d170628_TT1_SS09</t>
+  </si>
+  <si>
+    <t>b0148_d170628_TT1_SS10</t>
+  </si>
+  <si>
+    <t>b0148_d170628_TT1_SS11</t>
+  </si>
+  <si>
+    <t>b0148_d170628_TT4_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170628_TT4_SS02</t>
+  </si>
+  <si>
+    <t>b0148_d170628_TT4_SS03</t>
+  </si>
+  <si>
+    <t>[72083014179 73197699965]</t>
+  </si>
+  <si>
+    <t>b0148_d170628_TT4_SS04</t>
+  </si>
+  <si>
+    <t>b0148_d170628_TT4_SS05</t>
+  </si>
+  <si>
+    <t>b0148_d170703_TT1_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170703_TT1_SS02</t>
+  </si>
+  <si>
+    <t>b0148_d170703_TT1_SS03</t>
+  </si>
+  <si>
+    <t>b0148_d170703_TT1_SS04</t>
+  </si>
+  <si>
+    <t>b0148_d170703_TT4_SS01</t>
+  </si>
+  <si>
+    <t>b0148_d170703_TT4_SS02</t>
+  </si>
+  <si>
+    <t>b0148_d170703_TT4_SS03</t>
+  </si>
+  <si>
+    <t>b0148_d170703_TT4_SS04</t>
   </si>
 </sst>
 </file>
@@ -2189,7 +2756,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2204,6 +2771,13 @@
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2486,11 +3060,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S562"/>
+  <dimension ref="A1:S724"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A390" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <pane ySplit="1" topLeftCell="A684" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G691" sqref="G691"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -15126,7 +15700,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="561" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="561" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A561" s="1" t="s">
         <v>655</v>
       </c>
@@ -15149,7 +15723,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="562" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="562" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A562" s="1" t="s">
         <v>656</v>
       </c>
@@ -15170,6 +15744,3734 @@
       </c>
       <c r="G562" s="1" t="s">
         <v>127</v>
+      </c>
+    </row>
+    <row r="563" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A563" s="7" t="s">
+        <v>706</v>
+      </c>
+      <c r="B563" s="7">
+        <v>148</v>
+      </c>
+      <c r="C563" s="8">
+        <v>42892</v>
+      </c>
+      <c r="D563" s="7">
+        <v>1</v>
+      </c>
+      <c r="E563" s="7">
+        <v>1</v>
+      </c>
+      <c r="F563" s="7">
+        <v>2</v>
+      </c>
+      <c r="G563" s="6"/>
+      <c r="H563" s="6"/>
+    </row>
+    <row r="564" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A564" s="7" t="s">
+        <v>707</v>
+      </c>
+      <c r="B564" s="7">
+        <v>148</v>
+      </c>
+      <c r="C564" s="8">
+        <v>42892</v>
+      </c>
+      <c r="D564" s="7">
+        <v>1</v>
+      </c>
+      <c r="E564" s="7">
+        <v>2</v>
+      </c>
+      <c r="F564" s="7">
+        <v>2</v>
+      </c>
+      <c r="G564" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="H564" s="7" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="565" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A565" s="7" t="s">
+        <v>709</v>
+      </c>
+      <c r="B565" s="7">
+        <v>148</v>
+      </c>
+      <c r="C565" s="8">
+        <v>42892</v>
+      </c>
+      <c r="D565" s="7">
+        <v>1</v>
+      </c>
+      <c r="E565" s="7">
+        <v>3</v>
+      </c>
+      <c r="F565" s="7">
+        <v>1</v>
+      </c>
+      <c r="G565" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H565" s="6"/>
+    </row>
+    <row r="566" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A566" s="7" t="s">
+        <v>710</v>
+      </c>
+      <c r="B566" s="7">
+        <v>148</v>
+      </c>
+      <c r="C566" s="8">
+        <v>42892</v>
+      </c>
+      <c r="D566" s="7">
+        <v>4</v>
+      </c>
+      <c r="E566" s="7">
+        <v>1</v>
+      </c>
+      <c r="F566" s="7">
+        <v>2</v>
+      </c>
+      <c r="G566" s="6"/>
+      <c r="H566" s="6"/>
+    </row>
+    <row r="567" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A567" s="7" t="s">
+        <v>711</v>
+      </c>
+      <c r="B567" s="7">
+        <v>148</v>
+      </c>
+      <c r="C567" s="8">
+        <v>42892</v>
+      </c>
+      <c r="D567" s="7">
+        <v>4</v>
+      </c>
+      <c r="E567" s="7">
+        <v>2</v>
+      </c>
+      <c r="F567" s="7">
+        <v>2</v>
+      </c>
+      <c r="G567" s="6"/>
+      <c r="H567" s="6"/>
+    </row>
+    <row r="568" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A568" s="7" t="s">
+        <v>712</v>
+      </c>
+      <c r="B568" s="7">
+        <v>148</v>
+      </c>
+      <c r="C568" s="8">
+        <v>42892</v>
+      </c>
+      <c r="D568" s="7">
+        <v>4</v>
+      </c>
+      <c r="E568" s="7">
+        <v>3</v>
+      </c>
+      <c r="F568" s="7">
+        <v>2</v>
+      </c>
+      <c r="G568" s="6"/>
+      <c r="H568" s="6"/>
+    </row>
+    <row r="569" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A569" s="7" t="s">
+        <v>713</v>
+      </c>
+      <c r="B569" s="7">
+        <v>148</v>
+      </c>
+      <c r="C569" s="8">
+        <v>42892</v>
+      </c>
+      <c r="D569" s="7">
+        <v>4</v>
+      </c>
+      <c r="E569" s="7">
+        <v>4</v>
+      </c>
+      <c r="F569" s="7">
+        <v>2</v>
+      </c>
+      <c r="G569" s="6"/>
+      <c r="H569" s="6"/>
+    </row>
+    <row r="570" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A570" s="7" t="s">
+        <v>714</v>
+      </c>
+      <c r="B570" s="7">
+        <v>148</v>
+      </c>
+      <c r="C570" s="8">
+        <v>42892</v>
+      </c>
+      <c r="D570" s="7">
+        <v>4</v>
+      </c>
+      <c r="E570" s="7">
+        <v>5</v>
+      </c>
+      <c r="F570" s="7">
+        <v>2</v>
+      </c>
+      <c r="G570" s="6"/>
+      <c r="H570" s="6"/>
+    </row>
+    <row r="571" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A571" s="7" t="s">
+        <v>715</v>
+      </c>
+      <c r="B571" s="7">
+        <v>148</v>
+      </c>
+      <c r="C571" s="8">
+        <v>42892</v>
+      </c>
+      <c r="D571" s="7">
+        <v>4</v>
+      </c>
+      <c r="E571" s="7">
+        <v>6</v>
+      </c>
+      <c r="F571" s="7">
+        <v>2</v>
+      </c>
+      <c r="G571" s="6"/>
+      <c r="H571" s="6"/>
+    </row>
+    <row r="572" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A572" s="7" t="s">
+        <v>716</v>
+      </c>
+      <c r="B572" s="7">
+        <v>148</v>
+      </c>
+      <c r="C572" s="8">
+        <v>42892</v>
+      </c>
+      <c r="D572" s="7">
+        <v>4</v>
+      </c>
+      <c r="E572" s="7">
+        <v>7</v>
+      </c>
+      <c r="F572" s="7">
+        <v>2</v>
+      </c>
+      <c r="G572" s="6"/>
+      <c r="H572" s="6"/>
+    </row>
+    <row r="573" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A573" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="B573" s="7">
+        <v>148</v>
+      </c>
+      <c r="C573" s="8">
+        <v>42892</v>
+      </c>
+      <c r="D573" s="7">
+        <v>4</v>
+      </c>
+      <c r="E573" s="7">
+        <v>8</v>
+      </c>
+      <c r="F573" s="7">
+        <v>2</v>
+      </c>
+      <c r="G573" s="6"/>
+      <c r="H573" s="6"/>
+    </row>
+    <row r="574" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A574" s="7" t="s">
+        <v>718</v>
+      </c>
+      <c r="B574" s="7">
+        <v>148</v>
+      </c>
+      <c r="C574" s="8">
+        <v>42892</v>
+      </c>
+      <c r="D574" s="7">
+        <v>4</v>
+      </c>
+      <c r="E574" s="7">
+        <v>9</v>
+      </c>
+      <c r="F574" s="7">
+        <v>2</v>
+      </c>
+      <c r="G574" s="6"/>
+      <c r="H574" s="6"/>
+    </row>
+    <row r="575" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A575" s="7" t="s">
+        <v>719</v>
+      </c>
+      <c r="B575" s="7">
+        <v>148</v>
+      </c>
+      <c r="C575" s="8">
+        <v>42892</v>
+      </c>
+      <c r="D575" s="7">
+        <v>4</v>
+      </c>
+      <c r="E575" s="7">
+        <v>10</v>
+      </c>
+      <c r="F575" s="7">
+        <v>2</v>
+      </c>
+      <c r="G575" s="6"/>
+      <c r="H575" s="6"/>
+    </row>
+    <row r="576" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A576" s="7" t="s">
+        <v>720</v>
+      </c>
+      <c r="B576" s="7">
+        <v>149</v>
+      </c>
+      <c r="C576" s="8">
+        <v>42892</v>
+      </c>
+      <c r="D576" s="7">
+        <v>4</v>
+      </c>
+      <c r="E576" s="7">
+        <v>11</v>
+      </c>
+      <c r="F576" s="7">
+        <v>1</v>
+      </c>
+      <c r="G576" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="H576" s="6"/>
+    </row>
+    <row r="577" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A577" s="7" t="s">
+        <v>721</v>
+      </c>
+      <c r="B577" s="7">
+        <v>149</v>
+      </c>
+      <c r="C577" s="8">
+        <v>42892</v>
+      </c>
+      <c r="D577" s="7">
+        <v>4</v>
+      </c>
+      <c r="E577" s="7">
+        <v>12</v>
+      </c>
+      <c r="F577" s="7">
+        <v>1</v>
+      </c>
+      <c r="G577" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="H577" s="6"/>
+    </row>
+    <row r="578" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A578" s="7" t="s">
+        <v>722</v>
+      </c>
+      <c r="B578" s="7">
+        <v>149</v>
+      </c>
+      <c r="C578" s="8">
+        <v>42892</v>
+      </c>
+      <c r="D578" s="7">
+        <v>4</v>
+      </c>
+      <c r="E578" s="7">
+        <v>13</v>
+      </c>
+      <c r="F578" s="7">
+        <v>1</v>
+      </c>
+      <c r="G578" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H578" s="6"/>
+    </row>
+    <row r="579" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A579" s="7" t="s">
+        <v>723</v>
+      </c>
+      <c r="B579" s="7">
+        <v>149</v>
+      </c>
+      <c r="C579" s="8">
+        <v>42892</v>
+      </c>
+      <c r="D579" s="7">
+        <v>4</v>
+      </c>
+      <c r="E579" s="7">
+        <v>14</v>
+      </c>
+      <c r="F579" s="7">
+        <v>1</v>
+      </c>
+      <c r="G579" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H579" s="6"/>
+    </row>
+    <row r="580" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A580" s="7" t="s">
+        <v>724</v>
+      </c>
+      <c r="B580" s="7">
+        <v>148</v>
+      </c>
+      <c r="C580" s="8">
+        <v>42893</v>
+      </c>
+      <c r="D580" s="7">
+        <v>4</v>
+      </c>
+      <c r="E580" s="7">
+        <v>1</v>
+      </c>
+      <c r="F580" s="7">
+        <v>2</v>
+      </c>
+      <c r="G580" s="6"/>
+      <c r="H580" s="6"/>
+    </row>
+    <row r="581" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A581" s="7" t="s">
+        <v>725</v>
+      </c>
+      <c r="B581" s="7">
+        <v>148</v>
+      </c>
+      <c r="C581" s="8">
+        <v>42893</v>
+      </c>
+      <c r="D581" s="7">
+        <v>4</v>
+      </c>
+      <c r="E581" s="7">
+        <v>2</v>
+      </c>
+      <c r="F581" s="7">
+        <v>2</v>
+      </c>
+      <c r="G581" s="6"/>
+      <c r="H581" s="6"/>
+    </row>
+    <row r="582" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A582" s="7" t="s">
+        <v>726</v>
+      </c>
+      <c r="B582" s="7">
+        <v>148</v>
+      </c>
+      <c r="C582" s="8">
+        <v>42893</v>
+      </c>
+      <c r="D582" s="7">
+        <v>4</v>
+      </c>
+      <c r="E582" s="7">
+        <v>3</v>
+      </c>
+      <c r="F582" s="7">
+        <v>2</v>
+      </c>
+      <c r="G582" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="H582" s="6"/>
+    </row>
+    <row r="583" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A583" s="7" t="s">
+        <v>727</v>
+      </c>
+      <c r="B583" s="7">
+        <v>148</v>
+      </c>
+      <c r="C583" s="8">
+        <v>42893</v>
+      </c>
+      <c r="D583" s="7">
+        <v>4</v>
+      </c>
+      <c r="E583" s="7">
+        <v>4</v>
+      </c>
+      <c r="F583" s="7">
+        <v>2</v>
+      </c>
+      <c r="G583" s="6"/>
+      <c r="H583" s="6"/>
+    </row>
+    <row r="584" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A584" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="B584" s="7">
+        <v>148</v>
+      </c>
+      <c r="C584" s="8">
+        <v>42893</v>
+      </c>
+      <c r="D584" s="7">
+        <v>4</v>
+      </c>
+      <c r="E584" s="7">
+        <v>5</v>
+      </c>
+      <c r="F584" s="7">
+        <v>2</v>
+      </c>
+      <c r="G584" s="7" t="s">
+        <v>729</v>
+      </c>
+      <c r="H584" s="6"/>
+    </row>
+    <row r="585" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A585" s="7" t="s">
+        <v>730</v>
+      </c>
+      <c r="B585" s="7">
+        <v>148</v>
+      </c>
+      <c r="C585" s="8">
+        <v>42893</v>
+      </c>
+      <c r="D585" s="7">
+        <v>4</v>
+      </c>
+      <c r="E585" s="7">
+        <v>6</v>
+      </c>
+      <c r="F585" s="7">
+        <v>2</v>
+      </c>
+      <c r="G585" s="7" t="s">
+        <v>731</v>
+      </c>
+      <c r="H585" s="6"/>
+    </row>
+    <row r="586" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A586" s="7" t="s">
+        <v>732</v>
+      </c>
+      <c r="B586" s="7">
+        <v>148</v>
+      </c>
+      <c r="C586" s="8">
+        <v>42893</v>
+      </c>
+      <c r="D586" s="7">
+        <v>4</v>
+      </c>
+      <c r="E586" s="7">
+        <v>7</v>
+      </c>
+      <c r="F586" s="7">
+        <v>2</v>
+      </c>
+      <c r="G586" s="7" t="s">
+        <v>729</v>
+      </c>
+      <c r="H586" s="6"/>
+    </row>
+    <row r="587" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A587" s="7" t="s">
+        <v>733</v>
+      </c>
+      <c r="B587" s="7">
+        <v>148</v>
+      </c>
+      <c r="C587" s="8">
+        <v>42893</v>
+      </c>
+      <c r="D587" s="7">
+        <v>4</v>
+      </c>
+      <c r="E587" s="7">
+        <v>8</v>
+      </c>
+      <c r="F587" s="7">
+        <v>2</v>
+      </c>
+      <c r="G587" s="6"/>
+      <c r="H587" s="7" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="588" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A588" s="7" t="s">
+        <v>735</v>
+      </c>
+      <c r="B588" s="7">
+        <v>148</v>
+      </c>
+      <c r="C588" s="8">
+        <v>42893</v>
+      </c>
+      <c r="D588" s="7">
+        <v>4</v>
+      </c>
+      <c r="E588" s="7">
+        <v>9</v>
+      </c>
+      <c r="F588" s="7">
+        <v>2</v>
+      </c>
+      <c r="G588" s="6"/>
+      <c r="H588" s="6"/>
+    </row>
+    <row r="589" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A589" s="7" t="s">
+        <v>736</v>
+      </c>
+      <c r="B589" s="7">
+        <v>148</v>
+      </c>
+      <c r="C589" s="8">
+        <v>42893</v>
+      </c>
+      <c r="D589" s="7">
+        <v>4</v>
+      </c>
+      <c r="E589" s="7">
+        <v>10</v>
+      </c>
+      <c r="F589" s="7">
+        <v>2</v>
+      </c>
+      <c r="G589" s="6"/>
+      <c r="H589" s="7" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="590" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A590" s="7" t="s">
+        <v>738</v>
+      </c>
+      <c r="B590" s="7">
+        <v>148</v>
+      </c>
+      <c r="C590" s="8">
+        <v>42893</v>
+      </c>
+      <c r="D590" s="7">
+        <v>4</v>
+      </c>
+      <c r="E590" s="7">
+        <v>11</v>
+      </c>
+      <c r="F590" s="7">
+        <v>2</v>
+      </c>
+      <c r="G590" s="6"/>
+      <c r="H590" s="7" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="591" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A591" s="7" t="s">
+        <v>740</v>
+      </c>
+      <c r="B591" s="7">
+        <v>148</v>
+      </c>
+      <c r="C591" s="8">
+        <v>42893</v>
+      </c>
+      <c r="D591" s="7">
+        <v>4</v>
+      </c>
+      <c r="E591" s="7">
+        <v>12</v>
+      </c>
+      <c r="F591" s="7">
+        <v>2</v>
+      </c>
+      <c r="G591" s="6"/>
+      <c r="H591" s="7" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="592" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A592" s="7" t="s">
+        <v>741</v>
+      </c>
+      <c r="B592" s="7">
+        <v>148</v>
+      </c>
+      <c r="C592" s="8">
+        <v>42893</v>
+      </c>
+      <c r="D592" s="7">
+        <v>4</v>
+      </c>
+      <c r="E592" s="7">
+        <v>13</v>
+      </c>
+      <c r="F592" s="7">
+        <v>2</v>
+      </c>
+      <c r="G592" s="7" t="s">
+        <v>742</v>
+      </c>
+      <c r="H592" s="7" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="593" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A593" s="7" t="s">
+        <v>744</v>
+      </c>
+      <c r="B593" s="7">
+        <v>148</v>
+      </c>
+      <c r="C593" s="8">
+        <v>42893</v>
+      </c>
+      <c r="D593" s="7">
+        <v>4</v>
+      </c>
+      <c r="E593" s="7">
+        <v>14</v>
+      </c>
+      <c r="F593" s="7">
+        <v>1</v>
+      </c>
+      <c r="G593" s="7" t="s">
+        <v>745</v>
+      </c>
+      <c r="H593" s="7" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="594" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A594" s="7" t="s">
+        <v>747</v>
+      </c>
+      <c r="B594" s="7">
+        <v>148</v>
+      </c>
+      <c r="C594" s="8">
+        <v>42893</v>
+      </c>
+      <c r="D594" s="7">
+        <v>4</v>
+      </c>
+      <c r="E594" s="7">
+        <v>15</v>
+      </c>
+      <c r="F594" s="7">
+        <v>1</v>
+      </c>
+      <c r="G594" s="7" t="s">
+        <v>745</v>
+      </c>
+      <c r="H594" s="6"/>
+    </row>
+    <row r="595" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A595" s="7" t="s">
+        <v>748</v>
+      </c>
+      <c r="B595" s="7">
+        <v>148</v>
+      </c>
+      <c r="C595" s="8">
+        <v>42893</v>
+      </c>
+      <c r="D595" s="7">
+        <v>4</v>
+      </c>
+      <c r="E595" s="7">
+        <v>16</v>
+      </c>
+      <c r="F595" s="7">
+        <v>1</v>
+      </c>
+      <c r="G595" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H595" s="6"/>
+    </row>
+    <row r="596" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A596" s="7" t="s">
+        <v>749</v>
+      </c>
+      <c r="B596" s="7">
+        <v>148</v>
+      </c>
+      <c r="C596" s="8">
+        <v>42893</v>
+      </c>
+      <c r="D596" s="7">
+        <v>4</v>
+      </c>
+      <c r="E596" s="7">
+        <v>17</v>
+      </c>
+      <c r="F596" s="7">
+        <v>1</v>
+      </c>
+      <c r="G596" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H596" s="6"/>
+    </row>
+    <row r="597" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A597" s="7" t="s">
+        <v>750</v>
+      </c>
+      <c r="B597" s="7">
+        <v>148</v>
+      </c>
+      <c r="C597" s="8">
+        <v>42893</v>
+      </c>
+      <c r="D597" s="7">
+        <v>4</v>
+      </c>
+      <c r="E597" s="7">
+        <v>18</v>
+      </c>
+      <c r="F597" s="7">
+        <v>1</v>
+      </c>
+      <c r="G597" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H597" s="6"/>
+    </row>
+    <row r="598" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A598" s="7" t="s">
+        <v>751</v>
+      </c>
+      <c r="B598" s="7">
+        <v>148</v>
+      </c>
+      <c r="C598" s="8">
+        <v>42893</v>
+      </c>
+      <c r="D598" s="7">
+        <v>4</v>
+      </c>
+      <c r="E598" s="7">
+        <v>19</v>
+      </c>
+      <c r="F598" s="7">
+        <v>1</v>
+      </c>
+      <c r="G598" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H598" s="6"/>
+    </row>
+    <row r="599" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A599" s="7" t="s">
+        <v>752</v>
+      </c>
+      <c r="B599" s="7">
+        <v>148</v>
+      </c>
+      <c r="C599" s="8">
+        <v>42893</v>
+      </c>
+      <c r="D599" s="7">
+        <v>4</v>
+      </c>
+      <c r="E599" s="7">
+        <v>20</v>
+      </c>
+      <c r="F599" s="7">
+        <v>1</v>
+      </c>
+      <c r="G599" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H599" s="6"/>
+    </row>
+    <row r="600" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A600" s="7" t="s">
+        <v>753</v>
+      </c>
+      <c r="B600" s="7">
+        <v>148</v>
+      </c>
+      <c r="C600" s="8">
+        <v>42894</v>
+      </c>
+      <c r="D600" s="7">
+        <v>1</v>
+      </c>
+      <c r="E600" s="7">
+        <v>1</v>
+      </c>
+      <c r="F600" s="7">
+        <v>1</v>
+      </c>
+      <c r="G600" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H600" s="6"/>
+    </row>
+    <row r="601" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A601" s="7" t="s">
+        <v>754</v>
+      </c>
+      <c r="B601" s="7">
+        <v>148</v>
+      </c>
+      <c r="C601" s="8">
+        <v>42894</v>
+      </c>
+      <c r="D601" s="7">
+        <v>4</v>
+      </c>
+      <c r="E601" s="7">
+        <v>1</v>
+      </c>
+      <c r="F601" s="7">
+        <v>2</v>
+      </c>
+      <c r="G601" s="7" t="s">
+        <v>755</v>
+      </c>
+      <c r="H601" s="6"/>
+    </row>
+    <row r="602" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A602" s="7" t="s">
+        <v>756</v>
+      </c>
+      <c r="B602" s="7">
+        <v>148</v>
+      </c>
+      <c r="C602" s="8">
+        <v>42894</v>
+      </c>
+      <c r="D602" s="7">
+        <v>4</v>
+      </c>
+      <c r="E602" s="7">
+        <v>2</v>
+      </c>
+      <c r="F602" s="7">
+        <v>1</v>
+      </c>
+      <c r="G602" s="7" t="s">
+        <v>757</v>
+      </c>
+      <c r="H602" s="6"/>
+    </row>
+    <row r="603" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A603" s="7" t="s">
+        <v>758</v>
+      </c>
+      <c r="B603" s="7">
+        <v>148</v>
+      </c>
+      <c r="C603" s="8">
+        <v>42894</v>
+      </c>
+      <c r="D603" s="7">
+        <v>4</v>
+      </c>
+      <c r="E603" s="7">
+        <v>3</v>
+      </c>
+      <c r="F603" s="7">
+        <v>2</v>
+      </c>
+      <c r="G603" s="6"/>
+      <c r="H603" s="6"/>
+    </row>
+    <row r="604" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A604" s="7" t="s">
+        <v>759</v>
+      </c>
+      <c r="B604" s="7">
+        <v>148</v>
+      </c>
+      <c r="C604" s="8">
+        <v>42894</v>
+      </c>
+      <c r="D604" s="7">
+        <v>4</v>
+      </c>
+      <c r="E604" s="7">
+        <v>4</v>
+      </c>
+      <c r="F604" s="7">
+        <v>2</v>
+      </c>
+      <c r="G604" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="H604" s="7" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="605" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A605" s="7" t="s">
+        <v>761</v>
+      </c>
+      <c r="B605" s="7">
+        <v>148</v>
+      </c>
+      <c r="C605" s="8">
+        <v>42894</v>
+      </c>
+      <c r="D605" s="7">
+        <v>4</v>
+      </c>
+      <c r="E605" s="7">
+        <v>5</v>
+      </c>
+      <c r="F605" s="7">
+        <v>1</v>
+      </c>
+      <c r="G605" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="H605" s="7" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="606" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A606" s="7" t="s">
+        <v>763</v>
+      </c>
+      <c r="B606" s="7">
+        <v>148</v>
+      </c>
+      <c r="C606" s="8">
+        <v>42894</v>
+      </c>
+      <c r="D606" s="7">
+        <v>4</v>
+      </c>
+      <c r="E606" s="7">
+        <v>6</v>
+      </c>
+      <c r="F606" s="7">
+        <v>1</v>
+      </c>
+      <c r="G606" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H606" s="6"/>
+    </row>
+    <row r="607" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A607" s="7" t="s">
+        <v>764</v>
+      </c>
+      <c r="B607" s="7">
+        <v>148</v>
+      </c>
+      <c r="C607" s="8">
+        <v>42894</v>
+      </c>
+      <c r="D607" s="7">
+        <v>4</v>
+      </c>
+      <c r="E607" s="7">
+        <v>7</v>
+      </c>
+      <c r="F607" s="7">
+        <v>1</v>
+      </c>
+      <c r="G607" s="7" t="s">
+        <v>765</v>
+      </c>
+      <c r="H607" s="6"/>
+    </row>
+    <row r="608" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A608" s="7" t="s">
+        <v>766</v>
+      </c>
+      <c r="B608" s="7">
+        <v>148</v>
+      </c>
+      <c r="C608" s="8">
+        <v>42894</v>
+      </c>
+      <c r="D608" s="7">
+        <v>4</v>
+      </c>
+      <c r="E608" s="7">
+        <v>8</v>
+      </c>
+      <c r="F608" s="7">
+        <v>1</v>
+      </c>
+      <c r="G608" s="7" t="s">
+        <v>767</v>
+      </c>
+      <c r="H608" s="6"/>
+    </row>
+    <row r="609" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A609" s="7" t="s">
+        <v>768</v>
+      </c>
+      <c r="B609" s="7">
+        <v>148</v>
+      </c>
+      <c r="C609" s="8">
+        <v>42897</v>
+      </c>
+      <c r="D609" s="7">
+        <v>4</v>
+      </c>
+      <c r="E609" s="7">
+        <v>1</v>
+      </c>
+      <c r="F609" s="7">
+        <v>1</v>
+      </c>
+      <c r="G609" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="610" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A610" s="7" t="s">
+        <v>769</v>
+      </c>
+      <c r="B610" s="7">
+        <v>148</v>
+      </c>
+      <c r="C610" s="8">
+        <v>42898</v>
+      </c>
+      <c r="D610" s="7">
+        <v>1</v>
+      </c>
+      <c r="E610" s="7">
+        <v>1</v>
+      </c>
+      <c r="F610" s="7">
+        <v>2</v>
+      </c>
+      <c r="G610" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="611" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A611" s="7" t="s">
+        <v>770</v>
+      </c>
+      <c r="B611" s="7">
+        <v>148</v>
+      </c>
+      <c r="C611" s="8">
+        <v>42898</v>
+      </c>
+      <c r="D611" s="7">
+        <v>1</v>
+      </c>
+      <c r="E611" s="7">
+        <v>2</v>
+      </c>
+      <c r="F611" s="7">
+        <v>1</v>
+      </c>
+      <c r="G611" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="612" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A612" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="B612" s="7">
+        <v>148</v>
+      </c>
+      <c r="C612" s="8">
+        <v>42898</v>
+      </c>
+      <c r="D612" s="7">
+        <v>1</v>
+      </c>
+      <c r="E612" s="7">
+        <v>3</v>
+      </c>
+      <c r="F612" s="7">
+        <v>1</v>
+      </c>
+      <c r="G612" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="613" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A613" s="7" t="s">
+        <v>772</v>
+      </c>
+      <c r="B613" s="7">
+        <v>148</v>
+      </c>
+      <c r="C613" s="8">
+        <v>42898</v>
+      </c>
+      <c r="D613" s="7">
+        <v>1</v>
+      </c>
+      <c r="E613" s="7">
+        <v>4</v>
+      </c>
+      <c r="F613" s="7">
+        <v>1</v>
+      </c>
+      <c r="G613" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="614" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A614" s="7" t="s">
+        <v>773</v>
+      </c>
+      <c r="B614" s="7">
+        <v>148</v>
+      </c>
+      <c r="C614" s="8">
+        <v>42898</v>
+      </c>
+      <c r="D614" s="7">
+        <v>1</v>
+      </c>
+      <c r="E614" s="7">
+        <v>5</v>
+      </c>
+      <c r="F614" s="7">
+        <v>1</v>
+      </c>
+      <c r="G614" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="615" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A615" s="7" t="s">
+        <v>774</v>
+      </c>
+      <c r="B615" s="7">
+        <v>148</v>
+      </c>
+      <c r="C615" s="8">
+        <v>42899</v>
+      </c>
+      <c r="D615" s="7">
+        <v>1</v>
+      </c>
+      <c r="E615" s="7">
+        <v>1</v>
+      </c>
+      <c r="F615" s="7">
+        <v>2</v>
+      </c>
+      <c r="G615" s="6"/>
+    </row>
+    <row r="616" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A616" s="7" t="s">
+        <v>775</v>
+      </c>
+      <c r="B616" s="7">
+        <v>148</v>
+      </c>
+      <c r="C616" s="8">
+        <v>42899</v>
+      </c>
+      <c r="D616" s="7">
+        <v>1</v>
+      </c>
+      <c r="E616" s="7">
+        <v>2</v>
+      </c>
+      <c r="F616" s="7">
+        <v>1</v>
+      </c>
+      <c r="G616" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="617" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A617" s="7" t="s">
+        <v>776</v>
+      </c>
+      <c r="B617" s="7">
+        <v>148</v>
+      </c>
+      <c r="C617" s="8">
+        <v>42899</v>
+      </c>
+      <c r="D617" s="7">
+        <v>1</v>
+      </c>
+      <c r="E617" s="7">
+        <v>3</v>
+      </c>
+      <c r="F617" s="7">
+        <v>1</v>
+      </c>
+      <c r="G617" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="618" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A618" s="7" t="s">
+        <v>777</v>
+      </c>
+      <c r="B618" s="7">
+        <v>148</v>
+      </c>
+      <c r="C618" s="8">
+        <v>42899</v>
+      </c>
+      <c r="D618" s="7">
+        <v>1</v>
+      </c>
+      <c r="E618" s="7">
+        <v>4</v>
+      </c>
+      <c r="F618" s="7">
+        <v>1</v>
+      </c>
+      <c r="G618" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="619" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A619" s="7" t="s">
+        <v>778</v>
+      </c>
+      <c r="B619" s="7">
+        <v>148</v>
+      </c>
+      <c r="C619" s="8">
+        <v>42899</v>
+      </c>
+      <c r="D619" s="7">
+        <v>1</v>
+      </c>
+      <c r="E619" s="7">
+        <v>5</v>
+      </c>
+      <c r="F619" s="7">
+        <v>1</v>
+      </c>
+      <c r="G619" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="620" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A620" s="7" t="s">
+        <v>779</v>
+      </c>
+      <c r="B620" s="7">
+        <v>148</v>
+      </c>
+      <c r="C620" s="8">
+        <v>42900</v>
+      </c>
+      <c r="D620" s="7">
+        <v>1</v>
+      </c>
+      <c r="E620" s="7">
+        <v>1</v>
+      </c>
+      <c r="F620" s="7">
+        <v>2</v>
+      </c>
+      <c r="G620" s="6"/>
+    </row>
+    <row r="621" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A621" s="7" t="s">
+        <v>780</v>
+      </c>
+      <c r="B621" s="7">
+        <v>148</v>
+      </c>
+      <c r="C621" s="8">
+        <v>42900</v>
+      </c>
+      <c r="D621" s="7">
+        <v>1</v>
+      </c>
+      <c r="E621" s="7">
+        <v>2</v>
+      </c>
+      <c r="F621" s="7">
+        <v>2</v>
+      </c>
+      <c r="G621" s="6"/>
+    </row>
+    <row r="622" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A622" s="7" t="s">
+        <v>781</v>
+      </c>
+      <c r="B622" s="7">
+        <v>148</v>
+      </c>
+      <c r="C622" s="8">
+        <v>42900</v>
+      </c>
+      <c r="D622" s="7">
+        <v>1</v>
+      </c>
+      <c r="E622" s="7">
+        <v>3</v>
+      </c>
+      <c r="F622" s="7">
+        <v>1</v>
+      </c>
+      <c r="G622" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="623" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A623" s="7" t="s">
+        <v>782</v>
+      </c>
+      <c r="B623" s="7">
+        <v>148</v>
+      </c>
+      <c r="C623" s="8">
+        <v>42900</v>
+      </c>
+      <c r="D623" s="7">
+        <v>4</v>
+      </c>
+      <c r="E623" s="7">
+        <v>1</v>
+      </c>
+      <c r="F623" s="7">
+        <v>2</v>
+      </c>
+      <c r="G623" s="6"/>
+    </row>
+    <row r="624" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A624" s="7" t="s">
+        <v>783</v>
+      </c>
+      <c r="B624" s="7">
+        <v>148</v>
+      </c>
+      <c r="C624" s="8">
+        <v>42900</v>
+      </c>
+      <c r="D624" s="7">
+        <v>4</v>
+      </c>
+      <c r="E624" s="7">
+        <v>2</v>
+      </c>
+      <c r="F624" s="7">
+        <v>1</v>
+      </c>
+      <c r="G624" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="625" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A625" s="7" t="s">
+        <v>784</v>
+      </c>
+      <c r="B625" s="7">
+        <v>148</v>
+      </c>
+      <c r="C625" s="8">
+        <v>42900</v>
+      </c>
+      <c r="D625" s="7">
+        <v>4</v>
+      </c>
+      <c r="E625" s="7">
+        <v>3</v>
+      </c>
+      <c r="F625" s="7">
+        <v>1</v>
+      </c>
+      <c r="G625" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H625" s="6"/>
+    </row>
+    <row r="626" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A626" s="7" t="s">
+        <v>785</v>
+      </c>
+      <c r="B626" s="7">
+        <v>148</v>
+      </c>
+      <c r="C626" s="8">
+        <v>42900</v>
+      </c>
+      <c r="D626" s="7">
+        <v>4</v>
+      </c>
+      <c r="E626" s="7">
+        <v>4</v>
+      </c>
+      <c r="F626" s="7">
+        <v>1</v>
+      </c>
+      <c r="G626" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H626" s="6"/>
+    </row>
+    <row r="627" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A627" s="7" t="s">
+        <v>786</v>
+      </c>
+      <c r="B627" s="7">
+        <v>148</v>
+      </c>
+      <c r="C627" s="8">
+        <v>42901</v>
+      </c>
+      <c r="D627" s="7">
+        <v>1</v>
+      </c>
+      <c r="E627" s="7">
+        <v>1</v>
+      </c>
+      <c r="F627" s="7">
+        <v>2</v>
+      </c>
+      <c r="G627" s="6"/>
+      <c r="H627" s="6"/>
+    </row>
+    <row r="628" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A628" s="7" t="s">
+        <v>787</v>
+      </c>
+      <c r="B628" s="7">
+        <v>148</v>
+      </c>
+      <c r="C628" s="8">
+        <v>42901</v>
+      </c>
+      <c r="D628" s="7">
+        <v>1</v>
+      </c>
+      <c r="E628" s="7">
+        <v>2</v>
+      </c>
+      <c r="F628" s="7">
+        <v>1</v>
+      </c>
+      <c r="G628" s="7" t="s">
+        <v>788</v>
+      </c>
+      <c r="H628" s="6"/>
+    </row>
+    <row r="629" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A629" s="7" t="s">
+        <v>789</v>
+      </c>
+      <c r="B629" s="7">
+        <v>148</v>
+      </c>
+      <c r="C629" s="8">
+        <v>42901</v>
+      </c>
+      <c r="D629" s="7">
+        <v>1</v>
+      </c>
+      <c r="E629" s="7">
+        <v>3</v>
+      </c>
+      <c r="F629" s="7">
+        <v>1</v>
+      </c>
+      <c r="G629" s="7" t="s">
+        <v>790</v>
+      </c>
+      <c r="H629" s="6"/>
+    </row>
+    <row r="630" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A630" s="7" t="s">
+        <v>791</v>
+      </c>
+      <c r="B630" s="7">
+        <v>148</v>
+      </c>
+      <c r="C630" s="8">
+        <v>42901</v>
+      </c>
+      <c r="D630" s="7">
+        <v>1</v>
+      </c>
+      <c r="E630" s="7">
+        <v>4</v>
+      </c>
+      <c r="F630" s="7">
+        <v>1</v>
+      </c>
+      <c r="G630" s="7" t="s">
+        <v>792</v>
+      </c>
+      <c r="H630" s="6"/>
+    </row>
+    <row r="631" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A631" s="7" t="s">
+        <v>793</v>
+      </c>
+      <c r="B631" s="7">
+        <v>148</v>
+      </c>
+      <c r="C631" s="8">
+        <v>42901</v>
+      </c>
+      <c r="D631" s="7">
+        <v>1</v>
+      </c>
+      <c r="E631" s="7">
+        <v>5</v>
+      </c>
+      <c r="F631" s="7">
+        <v>1</v>
+      </c>
+      <c r="G631" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="H631" s="6"/>
+    </row>
+    <row r="632" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A632" s="7" t="s">
+        <v>794</v>
+      </c>
+      <c r="B632" s="7">
+        <v>148</v>
+      </c>
+      <c r="C632" s="8">
+        <v>42901</v>
+      </c>
+      <c r="D632" s="7">
+        <v>4</v>
+      </c>
+      <c r="E632" s="7">
+        <v>1</v>
+      </c>
+      <c r="F632" s="7">
+        <v>2</v>
+      </c>
+      <c r="G632" s="6"/>
+      <c r="H632" s="6"/>
+    </row>
+    <row r="633" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A633" s="7" t="s">
+        <v>795</v>
+      </c>
+      <c r="B633" s="7">
+        <v>148</v>
+      </c>
+      <c r="C633" s="8">
+        <v>42904</v>
+      </c>
+      <c r="D633" s="7">
+        <v>1</v>
+      </c>
+      <c r="E633" s="7">
+        <v>1</v>
+      </c>
+      <c r="F633" s="7">
+        <v>2</v>
+      </c>
+      <c r="G633" s="6"/>
+      <c r="H633" s="6"/>
+    </row>
+    <row r="634" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A634" s="7" t="s">
+        <v>796</v>
+      </c>
+      <c r="B634" s="7">
+        <v>148</v>
+      </c>
+      <c r="C634" s="8">
+        <v>42904</v>
+      </c>
+      <c r="D634" s="7">
+        <v>1</v>
+      </c>
+      <c r="E634" s="7">
+        <v>2</v>
+      </c>
+      <c r="F634" s="7">
+        <v>1</v>
+      </c>
+      <c r="G634" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="H634" s="6"/>
+    </row>
+    <row r="635" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A635" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="B635" s="7">
+        <v>148</v>
+      </c>
+      <c r="C635" s="8">
+        <v>42904</v>
+      </c>
+      <c r="D635" s="7">
+        <v>1</v>
+      </c>
+      <c r="E635" s="7">
+        <v>3</v>
+      </c>
+      <c r="F635" s="7">
+        <v>1</v>
+      </c>
+      <c r="G635" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="H635" s="6"/>
+    </row>
+    <row r="636" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A636" s="7" t="s">
+        <v>798</v>
+      </c>
+      <c r="B636" s="7">
+        <v>148</v>
+      </c>
+      <c r="C636" s="8">
+        <v>42904</v>
+      </c>
+      <c r="D636" s="7">
+        <v>1</v>
+      </c>
+      <c r="E636" s="7">
+        <v>4</v>
+      </c>
+      <c r="F636" s="7">
+        <v>1</v>
+      </c>
+      <c r="G636" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="H636" s="6"/>
+    </row>
+    <row r="637" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A637" s="7" t="s">
+        <v>799</v>
+      </c>
+      <c r="B637" s="7">
+        <v>148</v>
+      </c>
+      <c r="C637" s="8">
+        <v>42904</v>
+      </c>
+      <c r="D637" s="7">
+        <v>4</v>
+      </c>
+      <c r="E637" s="7">
+        <v>1</v>
+      </c>
+      <c r="F637" s="7">
+        <v>2</v>
+      </c>
+      <c r="G637" s="6"/>
+      <c r="H637" s="7" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="638" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A638" s="7" t="s">
+        <v>801</v>
+      </c>
+      <c r="B638" s="7">
+        <v>148</v>
+      </c>
+      <c r="C638" s="8">
+        <v>42904</v>
+      </c>
+      <c r="D638" s="7">
+        <v>4</v>
+      </c>
+      <c r="E638" s="7">
+        <v>2</v>
+      </c>
+      <c r="F638" s="7">
+        <v>1</v>
+      </c>
+      <c r="G638" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H638" s="7" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="639" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A639" s="7" t="s">
+        <v>802</v>
+      </c>
+      <c r="B639" s="7">
+        <v>148</v>
+      </c>
+      <c r="C639" s="8">
+        <v>42905</v>
+      </c>
+      <c r="D639" s="7">
+        <v>1</v>
+      </c>
+      <c r="E639" s="7">
+        <v>1</v>
+      </c>
+      <c r="F639" s="7">
+        <v>2</v>
+      </c>
+      <c r="G639" s="6"/>
+      <c r="H639" s="6"/>
+    </row>
+    <row r="640" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A640" s="7" t="s">
+        <v>803</v>
+      </c>
+      <c r="B640" s="7">
+        <v>148</v>
+      </c>
+      <c r="C640" s="8">
+        <v>42905</v>
+      </c>
+      <c r="D640" s="7">
+        <v>1</v>
+      </c>
+      <c r="E640" s="7">
+        <v>2</v>
+      </c>
+      <c r="F640" s="7">
+        <v>1</v>
+      </c>
+      <c r="G640" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H640" s="6"/>
+    </row>
+    <row r="641" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A641" s="7" t="s">
+        <v>804</v>
+      </c>
+      <c r="B641" s="7">
+        <v>148</v>
+      </c>
+      <c r="C641" s="8">
+        <v>42905</v>
+      </c>
+      <c r="D641" s="7">
+        <v>1</v>
+      </c>
+      <c r="E641" s="7">
+        <v>3</v>
+      </c>
+      <c r="F641" s="7">
+        <v>1</v>
+      </c>
+      <c r="G641" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="642" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A642" s="7" t="s">
+        <v>805</v>
+      </c>
+      <c r="B642" s="7">
+        <v>148</v>
+      </c>
+      <c r="C642" s="8">
+        <v>42905</v>
+      </c>
+      <c r="D642" s="7">
+        <v>1</v>
+      </c>
+      <c r="E642" s="7">
+        <v>4</v>
+      </c>
+      <c r="F642" s="7">
+        <v>1</v>
+      </c>
+      <c r="G642" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="643" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A643" s="7" t="s">
+        <v>806</v>
+      </c>
+      <c r="B643" s="7">
+        <v>148</v>
+      </c>
+      <c r="C643" s="8">
+        <v>42905</v>
+      </c>
+      <c r="D643" s="7">
+        <v>4</v>
+      </c>
+      <c r="E643" s="7">
+        <v>1</v>
+      </c>
+      <c r="F643" s="7">
+        <v>2</v>
+      </c>
+      <c r="G643" s="6"/>
+    </row>
+    <row r="644" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A644" s="7" t="s">
+        <v>807</v>
+      </c>
+      <c r="B644" s="7">
+        <v>148</v>
+      </c>
+      <c r="C644" s="8">
+        <v>42905</v>
+      </c>
+      <c r="D644" s="7">
+        <v>4</v>
+      </c>
+      <c r="E644" s="7">
+        <v>2</v>
+      </c>
+      <c r="F644" s="7">
+        <v>2</v>
+      </c>
+      <c r="G644" s="6"/>
+    </row>
+    <row r="645" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A645" s="7" t="s">
+        <v>808</v>
+      </c>
+      <c r="B645" s="7">
+        <v>148</v>
+      </c>
+      <c r="C645" s="8">
+        <v>42905</v>
+      </c>
+      <c r="D645" s="7">
+        <v>4</v>
+      </c>
+      <c r="E645" s="7">
+        <v>3</v>
+      </c>
+      <c r="F645" s="7">
+        <v>1</v>
+      </c>
+      <c r="G645" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="646" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A646" s="7" t="s">
+        <v>809</v>
+      </c>
+      <c r="B646" s="7">
+        <v>148</v>
+      </c>
+      <c r="C646" s="8">
+        <v>42905</v>
+      </c>
+      <c r="D646" s="7">
+        <v>4</v>
+      </c>
+      <c r="E646" s="7">
+        <v>4</v>
+      </c>
+      <c r="F646" s="7">
+        <v>1</v>
+      </c>
+      <c r="G646" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="647" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A647" s="7" t="s">
+        <v>810</v>
+      </c>
+      <c r="B647" s="7">
+        <v>148</v>
+      </c>
+      <c r="C647" s="8">
+        <v>42906</v>
+      </c>
+      <c r="D647" s="7">
+        <v>1</v>
+      </c>
+      <c r="E647" s="7">
+        <v>1</v>
+      </c>
+      <c r="F647" s="7">
+        <v>2</v>
+      </c>
+      <c r="G647" s="6"/>
+    </row>
+    <row r="648" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A648" s="7" t="s">
+        <v>811</v>
+      </c>
+      <c r="B648" s="7">
+        <v>148</v>
+      </c>
+      <c r="C648" s="8">
+        <v>42906</v>
+      </c>
+      <c r="D648" s="7">
+        <v>1</v>
+      </c>
+      <c r="E648" s="7">
+        <v>2</v>
+      </c>
+      <c r="F648" s="7">
+        <v>1</v>
+      </c>
+      <c r="G648" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="649" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A649" s="7" t="s">
+        <v>812</v>
+      </c>
+      <c r="B649" s="7">
+        <v>148</v>
+      </c>
+      <c r="C649" s="8">
+        <v>42906</v>
+      </c>
+      <c r="D649" s="7">
+        <v>4</v>
+      </c>
+      <c r="E649" s="7">
+        <v>1</v>
+      </c>
+      <c r="F649" s="7">
+        <v>2</v>
+      </c>
+      <c r="G649" s="6"/>
+    </row>
+    <row r="650" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A650" s="7" t="s">
+        <v>813</v>
+      </c>
+      <c r="B650" s="7">
+        <v>148</v>
+      </c>
+      <c r="C650" s="8">
+        <v>42906</v>
+      </c>
+      <c r="D650" s="7">
+        <v>4</v>
+      </c>
+      <c r="E650" s="7">
+        <v>2</v>
+      </c>
+      <c r="F650" s="7">
+        <v>2</v>
+      </c>
+      <c r="G650" s="6"/>
+    </row>
+    <row r="651" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A651" s="7" t="s">
+        <v>814</v>
+      </c>
+      <c r="B651" s="7">
+        <v>148</v>
+      </c>
+      <c r="C651" s="8">
+        <v>42906</v>
+      </c>
+      <c r="D651" s="7">
+        <v>4</v>
+      </c>
+      <c r="E651" s="7">
+        <v>3</v>
+      </c>
+      <c r="F651" s="7">
+        <v>2</v>
+      </c>
+      <c r="G651" s="6"/>
+    </row>
+    <row r="652" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A652" s="7" t="s">
+        <v>815</v>
+      </c>
+      <c r="B652" s="7">
+        <v>148</v>
+      </c>
+      <c r="C652" s="8">
+        <v>42906</v>
+      </c>
+      <c r="D652" s="7">
+        <v>4</v>
+      </c>
+      <c r="E652" s="7">
+        <v>4</v>
+      </c>
+      <c r="F652" s="7">
+        <v>1</v>
+      </c>
+      <c r="G652" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="653" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A653" s="7" t="s">
+        <v>816</v>
+      </c>
+      <c r="B653" s="7">
+        <v>148</v>
+      </c>
+      <c r="C653" s="8">
+        <v>42906</v>
+      </c>
+      <c r="D653" s="7">
+        <v>4</v>
+      </c>
+      <c r="E653" s="7">
+        <v>5</v>
+      </c>
+      <c r="F653" s="7">
+        <v>1</v>
+      </c>
+      <c r="G653" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="654" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A654" s="7" t="s">
+        <v>817</v>
+      </c>
+      <c r="B654" s="7">
+        <v>148</v>
+      </c>
+      <c r="C654" s="8">
+        <v>42907</v>
+      </c>
+      <c r="D654" s="7">
+        <v>1</v>
+      </c>
+      <c r="E654" s="7">
+        <v>1</v>
+      </c>
+      <c r="F654" s="7">
+        <v>2</v>
+      </c>
+      <c r="G654" s="6"/>
+    </row>
+    <row r="655" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A655" s="7" t="s">
+        <v>818</v>
+      </c>
+      <c r="B655" s="7">
+        <v>148</v>
+      </c>
+      <c r="C655" s="8">
+        <v>42907</v>
+      </c>
+      <c r="D655" s="7">
+        <v>1</v>
+      </c>
+      <c r="E655" s="7">
+        <v>2</v>
+      </c>
+      <c r="F655" s="7">
+        <v>1</v>
+      </c>
+      <c r="G655" s="7" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="656" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A656" s="7" t="s">
+        <v>819</v>
+      </c>
+      <c r="B656" s="7">
+        <v>148</v>
+      </c>
+      <c r="C656" s="8">
+        <v>42907</v>
+      </c>
+      <c r="D656" s="7">
+        <v>1</v>
+      </c>
+      <c r="E656" s="7">
+        <v>3</v>
+      </c>
+      <c r="F656" s="7">
+        <v>1</v>
+      </c>
+      <c r="G656" s="7" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="657" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A657" s="7" t="s">
+        <v>821</v>
+      </c>
+      <c r="B657" s="7">
+        <v>148</v>
+      </c>
+      <c r="C657" s="8">
+        <v>42907</v>
+      </c>
+      <c r="D657" s="7">
+        <v>1</v>
+      </c>
+      <c r="E657" s="7">
+        <v>4</v>
+      </c>
+      <c r="F657" s="7">
+        <v>1</v>
+      </c>
+      <c r="G657" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H657" s="6"/>
+    </row>
+    <row r="658" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A658" s="7" t="s">
+        <v>822</v>
+      </c>
+      <c r="B658" s="7">
+        <v>148</v>
+      </c>
+      <c r="C658" s="8">
+        <v>42907</v>
+      </c>
+      <c r="D658" s="7">
+        <v>4</v>
+      </c>
+      <c r="E658" s="7">
+        <v>1</v>
+      </c>
+      <c r="F658" s="7">
+        <v>2</v>
+      </c>
+      <c r="G658" s="6"/>
+      <c r="H658" s="6"/>
+    </row>
+    <row r="659" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A659" s="7" t="s">
+        <v>823</v>
+      </c>
+      <c r="B659" s="7">
+        <v>148</v>
+      </c>
+      <c r="C659" s="8">
+        <v>42907</v>
+      </c>
+      <c r="D659" s="7">
+        <v>4</v>
+      </c>
+      <c r="E659" s="7">
+        <v>2</v>
+      </c>
+      <c r="F659" s="7">
+        <v>2</v>
+      </c>
+      <c r="G659" s="6"/>
+      <c r="H659" s="6"/>
+    </row>
+    <row r="660" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A660" s="7" t="s">
+        <v>824</v>
+      </c>
+      <c r="B660" s="7">
+        <v>148</v>
+      </c>
+      <c r="C660" s="8">
+        <v>42907</v>
+      </c>
+      <c r="D660" s="7">
+        <v>4</v>
+      </c>
+      <c r="E660" s="7">
+        <v>3</v>
+      </c>
+      <c r="F660" s="7">
+        <v>1</v>
+      </c>
+      <c r="G660" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H660" s="6"/>
+    </row>
+    <row r="661" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A661" s="7" t="s">
+        <v>825</v>
+      </c>
+      <c r="B661" s="7">
+        <v>148</v>
+      </c>
+      <c r="C661" s="8">
+        <v>42908</v>
+      </c>
+      <c r="D661" s="7">
+        <v>1</v>
+      </c>
+      <c r="E661" s="7">
+        <v>1</v>
+      </c>
+      <c r="F661" s="7">
+        <v>2</v>
+      </c>
+      <c r="G661" s="6"/>
+      <c r="H661" s="6"/>
+    </row>
+    <row r="662" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A662" s="7" t="s">
+        <v>826</v>
+      </c>
+      <c r="B662" s="7">
+        <v>148</v>
+      </c>
+      <c r="C662" s="8">
+        <v>42908</v>
+      </c>
+      <c r="D662" s="7">
+        <v>1</v>
+      </c>
+      <c r="E662" s="7">
+        <v>2</v>
+      </c>
+      <c r="F662" s="7">
+        <v>1</v>
+      </c>
+      <c r="G662" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H662" s="6"/>
+    </row>
+    <row r="663" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A663" s="7" t="s">
+        <v>827</v>
+      </c>
+      <c r="B663" s="7">
+        <v>148</v>
+      </c>
+      <c r="C663" s="8">
+        <v>42908</v>
+      </c>
+      <c r="D663" s="7">
+        <v>4</v>
+      </c>
+      <c r="E663" s="7">
+        <v>1</v>
+      </c>
+      <c r="F663" s="7">
+        <v>1</v>
+      </c>
+      <c r="G663" s="7" t="s">
+        <v>788</v>
+      </c>
+      <c r="H663" s="6"/>
+    </row>
+    <row r="664" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A664" s="7" t="s">
+        <v>828</v>
+      </c>
+      <c r="B664" s="7">
+        <v>148</v>
+      </c>
+      <c r="C664" s="8">
+        <v>42908</v>
+      </c>
+      <c r="D664" s="7">
+        <v>4</v>
+      </c>
+      <c r="E664" s="7">
+        <v>2</v>
+      </c>
+      <c r="F664" s="7">
+        <v>1</v>
+      </c>
+      <c r="G664" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H664" s="6"/>
+    </row>
+    <row r="665" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A665" s="7" t="s">
+        <v>829</v>
+      </c>
+      <c r="B665" s="7">
+        <v>148</v>
+      </c>
+      <c r="C665" s="8">
+        <v>42908</v>
+      </c>
+      <c r="D665" s="7">
+        <v>4</v>
+      </c>
+      <c r="E665" s="7">
+        <v>3</v>
+      </c>
+      <c r="F665" s="7">
+        <v>1</v>
+      </c>
+      <c r="G665" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H665" s="6"/>
+    </row>
+    <row r="666" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A666" s="7" t="s">
+        <v>830</v>
+      </c>
+      <c r="B666" s="7">
+        <v>148</v>
+      </c>
+      <c r="C666" s="8">
+        <v>42908</v>
+      </c>
+      <c r="D666" s="7">
+        <v>4</v>
+      </c>
+      <c r="E666" s="7">
+        <v>4</v>
+      </c>
+      <c r="F666" s="7">
+        <v>1</v>
+      </c>
+      <c r="G666" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H666" s="7" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="667" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A667" s="7" t="s">
+        <v>832</v>
+      </c>
+      <c r="B667" s="7">
+        <v>148</v>
+      </c>
+      <c r="C667" s="8">
+        <v>42908</v>
+      </c>
+      <c r="D667" s="7">
+        <v>4</v>
+      </c>
+      <c r="E667" s="7">
+        <v>5</v>
+      </c>
+      <c r="F667" s="7">
+        <v>1</v>
+      </c>
+      <c r="G667" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H667" s="7" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="668" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A668" s="7" t="s">
+        <v>833</v>
+      </c>
+      <c r="B668" s="7">
+        <v>148</v>
+      </c>
+      <c r="C668" s="8">
+        <v>42911</v>
+      </c>
+      <c r="D668" s="7">
+        <v>1</v>
+      </c>
+      <c r="E668" s="7">
+        <v>1</v>
+      </c>
+      <c r="F668" s="7">
+        <v>2</v>
+      </c>
+      <c r="G668" s="6"/>
+      <c r="H668" s="6"/>
+    </row>
+    <row r="669" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A669" s="7" t="s">
+        <v>834</v>
+      </c>
+      <c r="B669" s="7">
+        <v>148</v>
+      </c>
+      <c r="C669" s="8">
+        <v>42911</v>
+      </c>
+      <c r="D669" s="7">
+        <v>1</v>
+      </c>
+      <c r="E669" s="7">
+        <v>2</v>
+      </c>
+      <c r="F669" s="7">
+        <v>1</v>
+      </c>
+      <c r="G669" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="H669" s="6"/>
+    </row>
+    <row r="670" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A670" s="7" t="s">
+        <v>835</v>
+      </c>
+      <c r="B670" s="7">
+        <v>148</v>
+      </c>
+      <c r="C670" s="8">
+        <v>42911</v>
+      </c>
+      <c r="D670" s="7">
+        <v>4</v>
+      </c>
+      <c r="E670" s="7">
+        <v>1</v>
+      </c>
+      <c r="F670" s="7">
+        <v>2</v>
+      </c>
+      <c r="G670" s="6"/>
+      <c r="H670" s="6"/>
+    </row>
+    <row r="671" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A671" s="7" t="s">
+        <v>836</v>
+      </c>
+      <c r="B671" s="7">
+        <v>148</v>
+      </c>
+      <c r="C671" s="8">
+        <v>42911</v>
+      </c>
+      <c r="D671" s="7">
+        <v>4</v>
+      </c>
+      <c r="E671" s="7">
+        <v>2</v>
+      </c>
+      <c r="F671" s="7">
+        <v>2</v>
+      </c>
+      <c r="G671" s="6"/>
+      <c r="H671" s="6"/>
+    </row>
+    <row r="672" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A672" s="7" t="s">
+        <v>837</v>
+      </c>
+      <c r="B672" s="7">
+        <v>148</v>
+      </c>
+      <c r="C672" s="8">
+        <v>42911</v>
+      </c>
+      <c r="D672" s="7">
+        <v>4</v>
+      </c>
+      <c r="E672" s="7">
+        <v>3</v>
+      </c>
+      <c r="F672" s="7">
+        <v>2</v>
+      </c>
+      <c r="G672" s="6"/>
+      <c r="H672" s="6"/>
+    </row>
+    <row r="673" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A673" s="7" t="s">
+        <v>838</v>
+      </c>
+      <c r="B673" s="7">
+        <v>148</v>
+      </c>
+      <c r="C673" s="8">
+        <v>42911</v>
+      </c>
+      <c r="D673" s="7">
+        <v>4</v>
+      </c>
+      <c r="E673" s="7">
+        <v>4</v>
+      </c>
+      <c r="F673" s="7">
+        <v>2</v>
+      </c>
+      <c r="G673" s="7" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="674" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A674" s="7" t="s">
+        <v>840</v>
+      </c>
+      <c r="B674" s="7">
+        <v>148</v>
+      </c>
+      <c r="C674" s="8">
+        <v>42911</v>
+      </c>
+      <c r="D674" s="7">
+        <v>4</v>
+      </c>
+      <c r="E674" s="7">
+        <v>5</v>
+      </c>
+      <c r="F674" s="7">
+        <v>2</v>
+      </c>
+      <c r="G674" s="7" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="675" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A675" s="7" t="s">
+        <v>842</v>
+      </c>
+      <c r="B675" s="7">
+        <v>148</v>
+      </c>
+      <c r="C675" s="8">
+        <v>42911</v>
+      </c>
+      <c r="D675" s="7">
+        <v>4</v>
+      </c>
+      <c r="E675" s="7">
+        <v>6</v>
+      </c>
+      <c r="F675" s="7">
+        <v>2</v>
+      </c>
+      <c r="G675" s="6"/>
+    </row>
+    <row r="676" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A676" s="7" t="s">
+        <v>843</v>
+      </c>
+      <c r="B676" s="7">
+        <v>148</v>
+      </c>
+      <c r="C676" s="8">
+        <v>42911</v>
+      </c>
+      <c r="D676" s="7">
+        <v>4</v>
+      </c>
+      <c r="E676" s="7">
+        <v>7</v>
+      </c>
+      <c r="F676" s="7">
+        <v>2</v>
+      </c>
+      <c r="G676" s="6"/>
+    </row>
+    <row r="677" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A677" s="7" t="s">
+        <v>844</v>
+      </c>
+      <c r="B677" s="7">
+        <v>148</v>
+      </c>
+      <c r="C677" s="8">
+        <v>42911</v>
+      </c>
+      <c r="D677" s="7">
+        <v>4</v>
+      </c>
+      <c r="E677" s="7">
+        <v>8</v>
+      </c>
+      <c r="F677" s="7">
+        <v>1</v>
+      </c>
+      <c r="G677" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="678" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A678" s="7" t="s">
+        <v>845</v>
+      </c>
+      <c r="B678" s="7">
+        <v>148</v>
+      </c>
+      <c r="C678" s="8">
+        <v>42911</v>
+      </c>
+      <c r="D678" s="7">
+        <v>4</v>
+      </c>
+      <c r="E678" s="7">
+        <v>9</v>
+      </c>
+      <c r="F678" s="7">
+        <v>2</v>
+      </c>
+      <c r="G678" s="6"/>
+    </row>
+    <row r="679" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A679" s="7" t="s">
+        <v>846</v>
+      </c>
+      <c r="B679" s="7">
+        <v>148</v>
+      </c>
+      <c r="C679" s="8">
+        <v>42911</v>
+      </c>
+      <c r="D679" s="7">
+        <v>4</v>
+      </c>
+      <c r="E679" s="7">
+        <v>10</v>
+      </c>
+      <c r="F679" s="7">
+        <v>1</v>
+      </c>
+      <c r="G679" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="680" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A680" s="7" t="s">
+        <v>847</v>
+      </c>
+      <c r="B680" s="7">
+        <v>148</v>
+      </c>
+      <c r="C680" s="8">
+        <v>42911</v>
+      </c>
+      <c r="D680" s="7">
+        <v>4</v>
+      </c>
+      <c r="E680" s="7">
+        <v>11</v>
+      </c>
+      <c r="F680" s="7">
+        <v>1</v>
+      </c>
+      <c r="G680" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="681" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A681" s="7" t="s">
+        <v>848</v>
+      </c>
+      <c r="B681" s="7">
+        <v>148</v>
+      </c>
+      <c r="C681" s="8">
+        <v>42911</v>
+      </c>
+      <c r="D681" s="7">
+        <v>4</v>
+      </c>
+      <c r="E681" s="7">
+        <v>12</v>
+      </c>
+      <c r="F681" s="7">
+        <v>1</v>
+      </c>
+      <c r="G681" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="682" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A682" s="7" t="s">
+        <v>849</v>
+      </c>
+      <c r="B682" s="7">
+        <v>148</v>
+      </c>
+      <c r="C682" s="8">
+        <v>42912</v>
+      </c>
+      <c r="D682" s="7">
+        <v>1</v>
+      </c>
+      <c r="E682" s="7">
+        <v>1</v>
+      </c>
+      <c r="F682" s="7">
+        <v>2</v>
+      </c>
+      <c r="G682" s="6"/>
+    </row>
+    <row r="683" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A683" s="7" t="s">
+        <v>850</v>
+      </c>
+      <c r="B683" s="7">
+        <v>148</v>
+      </c>
+      <c r="C683" s="8">
+        <v>42912</v>
+      </c>
+      <c r="D683" s="7">
+        <v>1</v>
+      </c>
+      <c r="E683" s="7">
+        <v>2</v>
+      </c>
+      <c r="F683" s="7">
+        <v>2</v>
+      </c>
+      <c r="G683" s="6"/>
+    </row>
+    <row r="684" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A684" s="7" t="s">
+        <v>851</v>
+      </c>
+      <c r="B684" s="7">
+        <v>148</v>
+      </c>
+      <c r="C684" s="8">
+        <v>42912</v>
+      </c>
+      <c r="D684" s="7">
+        <v>1</v>
+      </c>
+      <c r="E684" s="7">
+        <v>3</v>
+      </c>
+      <c r="F684" s="7">
+        <v>1</v>
+      </c>
+      <c r="G684" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="685" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A685" s="7" t="s">
+        <v>852</v>
+      </c>
+      <c r="B685" s="7">
+        <v>148</v>
+      </c>
+      <c r="C685" s="8">
+        <v>42912</v>
+      </c>
+      <c r="D685" s="7">
+        <v>1</v>
+      </c>
+      <c r="E685" s="7">
+        <v>4</v>
+      </c>
+      <c r="F685" s="7">
+        <v>1</v>
+      </c>
+      <c r="G685" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="686" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A686" s="7" t="s">
+        <v>853</v>
+      </c>
+      <c r="B686" s="7">
+        <v>148</v>
+      </c>
+      <c r="C686" s="8">
+        <v>42912</v>
+      </c>
+      <c r="D686" s="7">
+        <v>4</v>
+      </c>
+      <c r="E686" s="7">
+        <v>1</v>
+      </c>
+      <c r="F686" s="7">
+        <v>2</v>
+      </c>
+      <c r="G686" s="6"/>
+    </row>
+    <row r="687" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A687" s="7" t="s">
+        <v>854</v>
+      </c>
+      <c r="B687" s="7">
+        <v>148</v>
+      </c>
+      <c r="C687" s="8">
+        <v>42912</v>
+      </c>
+      <c r="D687" s="7">
+        <v>4</v>
+      </c>
+      <c r="E687" s="7">
+        <v>2</v>
+      </c>
+      <c r="F687" s="7">
+        <v>1</v>
+      </c>
+      <c r="G687" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="688" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A688" s="7" t="s">
+        <v>855</v>
+      </c>
+      <c r="B688" s="7">
+        <v>148</v>
+      </c>
+      <c r="C688" s="8">
+        <v>42913</v>
+      </c>
+      <c r="D688" s="7">
+        <v>1</v>
+      </c>
+      <c r="E688" s="7">
+        <v>1</v>
+      </c>
+      <c r="F688" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="G688" s="7" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="689" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A689" s="7" t="s">
+        <v>857</v>
+      </c>
+      <c r="B689" s="7">
+        <v>148</v>
+      </c>
+      <c r="C689" s="8">
+        <v>42913</v>
+      </c>
+      <c r="D689" s="7">
+        <v>1</v>
+      </c>
+      <c r="E689" s="7">
+        <v>2</v>
+      </c>
+      <c r="F689" s="7">
+        <v>1</v>
+      </c>
+      <c r="G689" s="7" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="690" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A690" s="7" t="s">
+        <v>858</v>
+      </c>
+      <c r="B690" s="7">
+        <v>148</v>
+      </c>
+      <c r="C690" s="8">
+        <v>42913</v>
+      </c>
+      <c r="D690" s="7">
+        <v>1</v>
+      </c>
+      <c r="E690" s="7">
+        <v>3</v>
+      </c>
+      <c r="F690" s="7">
+        <v>1</v>
+      </c>
+      <c r="G690" s="7" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="691" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A691" s="7" t="s">
+        <v>859</v>
+      </c>
+      <c r="B691" s="7">
+        <v>148</v>
+      </c>
+      <c r="C691" s="8">
+        <v>42913</v>
+      </c>
+      <c r="D691" s="7">
+        <v>1</v>
+      </c>
+      <c r="E691" s="7">
+        <v>4</v>
+      </c>
+      <c r="F691" s="7">
+        <v>1</v>
+      </c>
+      <c r="G691" s="7" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="692" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A692" s="7" t="s">
+        <v>861</v>
+      </c>
+      <c r="B692" s="7">
+        <v>148</v>
+      </c>
+      <c r="C692" s="8">
+        <v>42913</v>
+      </c>
+      <c r="D692" s="7">
+        <v>1</v>
+      </c>
+      <c r="E692" s="7">
+        <v>5</v>
+      </c>
+      <c r="F692" s="7">
+        <v>1</v>
+      </c>
+      <c r="G692" s="7" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="693" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A693" s="7" t="s">
+        <v>862</v>
+      </c>
+      <c r="B693" s="7">
+        <v>148</v>
+      </c>
+      <c r="C693" s="8">
+        <v>42913</v>
+      </c>
+      <c r="D693" s="7">
+        <v>1</v>
+      </c>
+      <c r="E693" s="7">
+        <v>6</v>
+      </c>
+      <c r="F693" s="7">
+        <v>1</v>
+      </c>
+      <c r="G693" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="694" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A694" s="7" t="s">
+        <v>863</v>
+      </c>
+      <c r="B694" s="7">
+        <v>148</v>
+      </c>
+      <c r="C694" s="8">
+        <v>42913</v>
+      </c>
+      <c r="D694" s="7">
+        <v>4</v>
+      </c>
+      <c r="E694" s="7">
+        <v>1</v>
+      </c>
+      <c r="F694" s="7">
+        <v>2</v>
+      </c>
+      <c r="G694" s="6"/>
+    </row>
+    <row r="695" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A695" s="7" t="s">
+        <v>864</v>
+      </c>
+      <c r="B695" s="7">
+        <v>148</v>
+      </c>
+      <c r="C695" s="8">
+        <v>42913</v>
+      </c>
+      <c r="D695" s="7">
+        <v>4</v>
+      </c>
+      <c r="E695" s="7">
+        <v>2</v>
+      </c>
+      <c r="F695" s="7">
+        <v>2</v>
+      </c>
+      <c r="G695" s="6"/>
+    </row>
+    <row r="696" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A696" s="7" t="s">
+        <v>865</v>
+      </c>
+      <c r="B696" s="7">
+        <v>148</v>
+      </c>
+      <c r="C696" s="8">
+        <v>42913</v>
+      </c>
+      <c r="D696" s="7">
+        <v>4</v>
+      </c>
+      <c r="E696" s="7">
+        <v>3</v>
+      </c>
+      <c r="F696" s="7">
+        <v>2</v>
+      </c>
+      <c r="G696" s="6"/>
+    </row>
+    <row r="697" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A697" s="7" t="s">
+        <v>866</v>
+      </c>
+      <c r="B697" s="7">
+        <v>148</v>
+      </c>
+      <c r="C697" s="8">
+        <v>42913</v>
+      </c>
+      <c r="D697" s="7">
+        <v>4</v>
+      </c>
+      <c r="E697" s="7">
+        <v>4</v>
+      </c>
+      <c r="F697" s="7">
+        <v>1</v>
+      </c>
+      <c r="G697" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="698" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A698" s="7" t="s">
+        <v>867</v>
+      </c>
+      <c r="B698" s="7">
+        <v>148</v>
+      </c>
+      <c r="C698" s="8">
+        <v>42913</v>
+      </c>
+      <c r="D698" s="7">
+        <v>4</v>
+      </c>
+      <c r="E698" s="7">
+        <v>5</v>
+      </c>
+      <c r="F698" s="7">
+        <v>1</v>
+      </c>
+      <c r="G698" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="699" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A699" s="7" t="s">
+        <v>868</v>
+      </c>
+      <c r="B699" s="7">
+        <v>148</v>
+      </c>
+      <c r="C699" s="8">
+        <v>42913</v>
+      </c>
+      <c r="D699" s="7">
+        <v>4</v>
+      </c>
+      <c r="E699" s="7">
+        <v>6</v>
+      </c>
+      <c r="F699" s="7">
+        <v>1</v>
+      </c>
+      <c r="G699" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="700" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A700" s="7" t="s">
+        <v>869</v>
+      </c>
+      <c r="B700" s="7">
+        <v>148</v>
+      </c>
+      <c r="C700" s="8">
+        <v>42913</v>
+      </c>
+      <c r="D700" s="7">
+        <v>4</v>
+      </c>
+      <c r="E700" s="7">
+        <v>7</v>
+      </c>
+      <c r="F700" s="7">
+        <v>1</v>
+      </c>
+      <c r="G700" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="701" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A701" s="7" t="s">
+        <v>870</v>
+      </c>
+      <c r="B701" s="7">
+        <v>148</v>
+      </c>
+      <c r="C701" s="8">
+        <v>42914</v>
+      </c>
+      <c r="D701" s="7">
+        <v>1</v>
+      </c>
+      <c r="E701" s="7">
+        <v>1</v>
+      </c>
+      <c r="F701" s="7">
+        <v>2</v>
+      </c>
+      <c r="G701" s="6"/>
+    </row>
+    <row r="702" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A702" s="7" t="s">
+        <v>871</v>
+      </c>
+      <c r="B702" s="7">
+        <v>148</v>
+      </c>
+      <c r="C702" s="8">
+        <v>42914</v>
+      </c>
+      <c r="D702" s="7">
+        <v>1</v>
+      </c>
+      <c r="E702" s="7">
+        <v>2</v>
+      </c>
+      <c r="F702" s="7">
+        <v>2</v>
+      </c>
+      <c r="G702" s="6"/>
+    </row>
+    <row r="703" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A703" s="7" t="s">
+        <v>872</v>
+      </c>
+      <c r="B703" s="7">
+        <v>148</v>
+      </c>
+      <c r="C703" s="8">
+        <v>42914</v>
+      </c>
+      <c r="D703" s="7">
+        <v>1</v>
+      </c>
+      <c r="E703" s="7">
+        <v>3</v>
+      </c>
+      <c r="F703" s="7">
+        <v>2</v>
+      </c>
+      <c r="G703" s="6"/>
+    </row>
+    <row r="704" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A704" s="7" t="s">
+        <v>873</v>
+      </c>
+      <c r="B704" s="7">
+        <v>148</v>
+      </c>
+      <c r="C704" s="8">
+        <v>42914</v>
+      </c>
+      <c r="D704" s="7">
+        <v>1</v>
+      </c>
+      <c r="E704" s="7">
+        <v>4</v>
+      </c>
+      <c r="F704" s="7">
+        <v>2</v>
+      </c>
+      <c r="G704" s="6"/>
+    </row>
+    <row r="705" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A705" s="7" t="s">
+        <v>874</v>
+      </c>
+      <c r="B705" s="7">
+        <v>148</v>
+      </c>
+      <c r="C705" s="8">
+        <v>42914</v>
+      </c>
+      <c r="D705" s="7">
+        <v>1</v>
+      </c>
+      <c r="E705" s="7">
+        <v>5</v>
+      </c>
+      <c r="F705" s="7">
+        <v>1</v>
+      </c>
+      <c r="G705" s="7" t="s">
+        <v>788</v>
+      </c>
+      <c r="H705" s="6"/>
+    </row>
+    <row r="706" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A706" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="B706" s="7">
+        <v>148</v>
+      </c>
+      <c r="C706" s="8">
+        <v>42914</v>
+      </c>
+      <c r="D706" s="7">
+        <v>1</v>
+      </c>
+      <c r="E706" s="7">
+        <v>6</v>
+      </c>
+      <c r="F706" s="7">
+        <v>1</v>
+      </c>
+      <c r="G706" s="7" t="s">
+        <v>788</v>
+      </c>
+      <c r="H706" s="6"/>
+    </row>
+    <row r="707" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A707" s="7" t="s">
+        <v>876</v>
+      </c>
+      <c r="B707" s="7">
+        <v>148</v>
+      </c>
+      <c r="C707" s="8">
+        <v>42914</v>
+      </c>
+      <c r="D707" s="7">
+        <v>1</v>
+      </c>
+      <c r="E707" s="7">
+        <v>7</v>
+      </c>
+      <c r="F707" s="7">
+        <v>1</v>
+      </c>
+      <c r="G707" s="7" t="s">
+        <v>788</v>
+      </c>
+      <c r="H707" s="6"/>
+    </row>
+    <row r="708" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A708" s="7" t="s">
+        <v>877</v>
+      </c>
+      <c r="B708" s="7">
+        <v>148</v>
+      </c>
+      <c r="C708" s="8">
+        <v>42914</v>
+      </c>
+      <c r="D708" s="7">
+        <v>1</v>
+      </c>
+      <c r="E708" s="7">
+        <v>8</v>
+      </c>
+      <c r="F708" s="7">
+        <v>1</v>
+      </c>
+      <c r="G708" s="7" t="s">
+        <v>788</v>
+      </c>
+      <c r="H708" s="6"/>
+    </row>
+    <row r="709" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A709" s="7" t="s">
+        <v>878</v>
+      </c>
+      <c r="B709" s="7">
+        <v>148</v>
+      </c>
+      <c r="C709" s="8">
+        <v>42914</v>
+      </c>
+      <c r="D709" s="7">
+        <v>1</v>
+      </c>
+      <c r="E709" s="7">
+        <v>9</v>
+      </c>
+      <c r="F709" s="7">
+        <v>1</v>
+      </c>
+      <c r="G709" s="7" t="s">
+        <v>788</v>
+      </c>
+      <c r="H709" s="6"/>
+    </row>
+    <row r="710" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A710" s="7" t="s">
+        <v>879</v>
+      </c>
+      <c r="B710" s="7">
+        <v>148</v>
+      </c>
+      <c r="C710" s="8">
+        <v>42914</v>
+      </c>
+      <c r="D710" s="7">
+        <v>1</v>
+      </c>
+      <c r="E710" s="7">
+        <v>10</v>
+      </c>
+      <c r="F710" s="7">
+        <v>1</v>
+      </c>
+      <c r="G710" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H710" s="6"/>
+    </row>
+    <row r="711" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A711" s="7" t="s">
+        <v>880</v>
+      </c>
+      <c r="B711" s="7">
+        <v>148</v>
+      </c>
+      <c r="C711" s="8">
+        <v>42914</v>
+      </c>
+      <c r="D711" s="7">
+        <v>1</v>
+      </c>
+      <c r="E711" s="7">
+        <v>11</v>
+      </c>
+      <c r="F711" s="7">
+        <v>1</v>
+      </c>
+      <c r="G711" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H711" s="6"/>
+    </row>
+    <row r="712" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A712" s="7" t="s">
+        <v>881</v>
+      </c>
+      <c r="B712" s="7">
+        <v>148</v>
+      </c>
+      <c r="C712" s="8">
+        <v>42914</v>
+      </c>
+      <c r="D712" s="7">
+        <v>4</v>
+      </c>
+      <c r="E712" s="7">
+        <v>1</v>
+      </c>
+      <c r="F712" s="7">
+        <v>2</v>
+      </c>
+      <c r="G712" s="6"/>
+      <c r="H712" s="6"/>
+    </row>
+    <row r="713" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A713" s="7" t="s">
+        <v>882</v>
+      </c>
+      <c r="B713" s="7">
+        <v>148</v>
+      </c>
+      <c r="C713" s="8">
+        <v>42914</v>
+      </c>
+      <c r="D713" s="7">
+        <v>4</v>
+      </c>
+      <c r="E713" s="7">
+        <v>2</v>
+      </c>
+      <c r="F713" s="7">
+        <v>1</v>
+      </c>
+      <c r="G713" s="7" t="s">
+        <v>788</v>
+      </c>
+      <c r="H713" s="6"/>
+    </row>
+    <row r="714" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A714" s="7" t="s">
+        <v>883</v>
+      </c>
+      <c r="B714" s="7">
+        <v>148</v>
+      </c>
+      <c r="C714" s="8">
+        <v>42914</v>
+      </c>
+      <c r="D714" s="7">
+        <v>4</v>
+      </c>
+      <c r="E714" s="7">
+        <v>3</v>
+      </c>
+      <c r="F714" s="7">
+        <v>2</v>
+      </c>
+      <c r="G714" s="6"/>
+      <c r="H714" s="7" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="715" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A715" s="7" t="s">
+        <v>885</v>
+      </c>
+      <c r="B715" s="7">
+        <v>148</v>
+      </c>
+      <c r="C715" s="8">
+        <v>42914</v>
+      </c>
+      <c r="D715" s="7">
+        <v>4</v>
+      </c>
+      <c r="E715" s="7">
+        <v>4</v>
+      </c>
+      <c r="F715" s="7">
+        <v>2</v>
+      </c>
+      <c r="G715" s="6"/>
+      <c r="H715" s="6"/>
+    </row>
+    <row r="716" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A716" s="7" t="s">
+        <v>886</v>
+      </c>
+      <c r="B716" s="7">
+        <v>148</v>
+      </c>
+      <c r="C716" s="8">
+        <v>42914</v>
+      </c>
+      <c r="D716" s="7">
+        <v>4</v>
+      </c>
+      <c r="E716" s="7">
+        <v>5</v>
+      </c>
+      <c r="F716" s="7">
+        <v>1</v>
+      </c>
+      <c r="G716" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H716" s="6"/>
+    </row>
+    <row r="717" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A717" s="7" t="s">
+        <v>887</v>
+      </c>
+      <c r="B717" s="7">
+        <v>148</v>
+      </c>
+      <c r="C717" s="8">
+        <v>42919</v>
+      </c>
+      <c r="D717" s="7">
+        <v>1</v>
+      </c>
+      <c r="E717" s="7">
+        <v>1</v>
+      </c>
+      <c r="F717" s="7">
+        <v>1</v>
+      </c>
+      <c r="G717" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H717" s="6"/>
+    </row>
+    <row r="718" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A718" s="7" t="s">
+        <v>888</v>
+      </c>
+      <c r="B718" s="7">
+        <v>148</v>
+      </c>
+      <c r="C718" s="8">
+        <v>42919</v>
+      </c>
+      <c r="D718" s="7">
+        <v>1</v>
+      </c>
+      <c r="E718" s="7">
+        <v>2</v>
+      </c>
+      <c r="F718" s="7">
+        <v>1</v>
+      </c>
+      <c r="G718" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H718" s="6"/>
+    </row>
+    <row r="719" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A719" s="7" t="s">
+        <v>889</v>
+      </c>
+      <c r="B719" s="7">
+        <v>148</v>
+      </c>
+      <c r="C719" s="8">
+        <v>42919</v>
+      </c>
+      <c r="D719" s="7">
+        <v>1</v>
+      </c>
+      <c r="E719" s="7">
+        <v>3</v>
+      </c>
+      <c r="F719" s="7">
+        <v>1</v>
+      </c>
+      <c r="G719" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H719" s="6"/>
+    </row>
+    <row r="720" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A720" s="7" t="s">
+        <v>890</v>
+      </c>
+      <c r="B720" s="7">
+        <v>148</v>
+      </c>
+      <c r="C720" s="8">
+        <v>42919</v>
+      </c>
+      <c r="D720" s="7">
+        <v>1</v>
+      </c>
+      <c r="E720" s="7">
+        <v>4</v>
+      </c>
+      <c r="F720" s="7">
+        <v>1</v>
+      </c>
+      <c r="G720" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H720" s="6"/>
+    </row>
+    <row r="721" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A721" s="7" t="s">
+        <v>891</v>
+      </c>
+      <c r="B721" s="7">
+        <v>148</v>
+      </c>
+      <c r="C721" s="8">
+        <v>42919</v>
+      </c>
+      <c r="D721" s="7">
+        <v>4</v>
+      </c>
+      <c r="E721" s="7">
+        <v>1</v>
+      </c>
+      <c r="F721" s="7">
+        <v>2</v>
+      </c>
+      <c r="G721" s="6"/>
+    </row>
+    <row r="722" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A722" s="7" t="s">
+        <v>892</v>
+      </c>
+      <c r="B722" s="7">
+        <v>148</v>
+      </c>
+      <c r="C722" s="8">
+        <v>42919</v>
+      </c>
+      <c r="D722" s="7">
+        <v>4</v>
+      </c>
+      <c r="E722" s="7">
+        <v>2</v>
+      </c>
+      <c r="F722" s="7">
+        <v>1</v>
+      </c>
+      <c r="G722" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="723" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A723" s="7" t="s">
+        <v>893</v>
+      </c>
+      <c r="B723" s="7">
+        <v>148</v>
+      </c>
+      <c r="C723" s="8">
+        <v>42919</v>
+      </c>
+      <c r="D723" s="7">
+        <v>4</v>
+      </c>
+      <c r="E723" s="7">
+        <v>3</v>
+      </c>
+      <c r="F723" s="7">
+        <v>1</v>
+      </c>
+      <c r="G723" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="724" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A724" s="7" t="s">
+        <v>894</v>
+      </c>
+      <c r="B724" s="7">
+        <v>148</v>
+      </c>
+      <c r="C724" s="8">
+        <v>42919</v>
+      </c>
+      <c r="D724" s="7">
+        <v>4</v>
+      </c>
+      <c r="E724" s="7">
+        <v>4</v>
+      </c>
+      <c r="F724" s="7">
+        <v>1</v>
+      </c>
+      <c r="G724" s="7" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correct typo in cells summary
</commit_message>
<xml_diff>
--- a/inclusion_lists/cells_summary.xlsx
+++ b/inclusion_lists/cells_summary.xlsx
@@ -3063,8 +3063,8 @@
   <dimension ref="A1:S724"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A684" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G691" sqref="G691"/>
+      <pane ySplit="1" topLeftCell="A552" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G573" sqref="G573"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -16043,7 +16043,7 @@
         <v>720</v>
       </c>
       <c r="B576" s="7">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C576" s="8">
         <v>42892</v>
@@ -16067,7 +16067,7 @@
         <v>721</v>
       </c>
       <c r="B577" s="7">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C577" s="8">
         <v>42892</v>
@@ -16091,7 +16091,7 @@
         <v>722</v>
       </c>
       <c r="B578" s="7">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C578" s="8">
         <v>42892</v>
@@ -16115,7 +16115,7 @@
         <v>723</v>
       </c>
       <c r="B579" s="7">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C579" s="8">
         <v>42892</v>

</xml_diff>

<commit_message>
ignore fields in low speed area near balls
</commit_message>
<xml_diff>
--- a/inclusion_lists/cells_summary.xlsx
+++ b/inclusion_lists/cells_summary.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="914">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="918">
   <si>
     <t>bat</t>
   </si>
@@ -2771,6 +2771,18 @@
   </si>
   <si>
     <t>cell_num</t>
+  </si>
+  <si>
+    <t>TODO: take only the second half (unstable!)</t>
+  </si>
+  <si>
+    <t>same as unit 2</t>
+  </si>
+  <si>
+    <t>same as unit 1</t>
+  </si>
+  <si>
+    <t>same unit as unit 4???</t>
   </si>
 </sst>
 </file>
@@ -3120,8 +3132,8 @@
   <dimension ref="A1:T733"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H155" sqref="H155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4257,6 +4269,9 @@
       <c r="G42" s="1">
         <v>2</v>
       </c>
+      <c r="H42" s="3" t="s">
+        <v>914</v>
+      </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
@@ -8624,6 +8639,9 @@
       <c r="G211" s="1">
         <v>2</v>
       </c>
+      <c r="H211" s="3" t="s">
+        <v>917</v>
+      </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
@@ -14723,6 +14741,9 @@
       <c r="G447" s="1">
         <v>2</v>
       </c>
+      <c r="H447" s="3" t="s">
+        <v>915</v>
+      </c>
     </row>
     <row r="448" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A448" s="1" t="s">
@@ -14745,6 +14766,9 @@
       </c>
       <c r="G448" s="1">
         <v>2</v>
+      </c>
+      <c r="H448" s="3" t="s">
+        <v>916</v>
       </c>
     </row>
     <row r="449" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add initial version of the paper figures
</commit_message>
<xml_diff>
--- a/inclusion_lists/cells_summary.xlsx
+++ b/inclusion_lists/cells_summary.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="918">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="919">
   <si>
     <t>bat</t>
   </si>
@@ -2783,6 +2783,9 @@
   </si>
   <si>
     <t>same unit as unit 4???</t>
+  </si>
+  <si>
+    <t>too close to the noise; maybe can be isolated from the noise (should add spikes!!)</t>
   </si>
 </sst>
 </file>
@@ -3132,8 +3135,8 @@
   <dimension ref="A1:T733"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H155" sqref="H155"/>
+      <pane ySplit="1" topLeftCell="A613" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H639" sqref="H639"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -19651,8 +19654,8 @@
       <c r="G640" s="7">
         <v>1</v>
       </c>
-      <c r="H640" s="7" t="s">
-        <v>115</v>
+      <c r="H640" s="3" t="s">
+        <v>918</v>
       </c>
       <c r="I640" s="6"/>
     </row>

</xml_diff>